<commit_message>
New main script, fixed bio allocate
</commit_message>
<xml_diff>
--- a/notebooks/GenVeg/GenVeg_Example_Simulation.xlsx
+++ b/notebooks/GenVeg/GenVeg_Example_Simulation.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\RDEL1CMC\Desktop\LandLab\landlab\notebooks\GenVeg\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Python\landlab\notebooks\GenVeg\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{0217537A-F97A-4F2A-83B3-E02482F17CC5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F40A609-DD56-4571-8111-BBCD973BFBFB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{4FA2BB3E-4334-4C54-90D8-DFF869504B66}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{4FA2BB3E-4334-4C54-90D8-DFF869504B66}"/>
   </bookViews>
   <sheets>
     <sheet name="Corn" sheetId="1" r:id="rId1"/>
@@ -125,9 +125,6 @@
   </si>
   <si>
     <t>Respiration coefficients</t>
-  </si>
-  <si>
-    <t>respiration_coeffecient</t>
   </si>
   <si>
     <t>Roots</t>
@@ -529,6 +526,9 @@
   </si>
   <si>
     <t>per file:///C:/Users/RDEL1CMC/Downloads/Charisma-a_simulation_model_of_the_dynamics_of_submerged_plants.PDF.pdf</t>
+  </si>
+  <si>
+    <t>respiration_coefficient</t>
   </si>
 </sst>
 </file>
@@ -1064,20 +1064,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{59430052-850A-4E52-8B29-0C7825B169C3}">
   <dimension ref="A1:G201"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="E20" sqref="E20"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="37.44140625" style="23" customWidth="1"/>
-    <col min="2" max="2" width="20.33203125" style="15" customWidth="1"/>
-    <col min="3" max="3" width="15.44140625" style="24" customWidth="1"/>
-    <col min="4" max="4" width="20.33203125" customWidth="1"/>
-    <col min="5" max="5" width="64.109375" customWidth="1"/>
+    <col min="1" max="1" width="37.42578125" style="23" customWidth="1"/>
+    <col min="2" max="2" width="20.28515625" style="15" customWidth="1"/>
+    <col min="3" max="3" width="15.42578125" style="24" customWidth="1"/>
+    <col min="4" max="4" width="20.28515625" customWidth="1"/>
+    <col min="5" max="5" width="64.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="20.399999999999999" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:6" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1097,7 +1097,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="18.600000000000001" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:6" ht="18.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="5" t="s">
         <v>5</v>
       </c>
@@ -1109,7 +1109,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="15" thickTop="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A3" s="9" t="s">
         <v>6</v>
       </c>
@@ -1118,13 +1118,13 @@
       </c>
       <c r="C3" s="11"/>
       <c r="D3" s="12" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="F3">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="9" t="s">
         <v>8</v>
       </c>
@@ -1139,7 +1139,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="9" t="s">
         <v>11</v>
       </c>
@@ -1154,7 +1154,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="9" t="s">
         <v>14</v>
       </c>
@@ -1169,7 +1169,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="9" t="s">
         <v>17</v>
       </c>
@@ -1178,13 +1178,13 @@
       </c>
       <c r="C7" s="11"/>
       <c r="D7" s="12" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="F7">
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="9" t="s">
         <v>19</v>
       </c>
@@ -1193,13 +1193,13 @@
       </c>
       <c r="C8" s="11"/>
       <c r="D8" s="12" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="F8">
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="18" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:6" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A9" s="5" t="s">
         <v>22</v>
       </c>
@@ -1211,7 +1211,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="15" thickTop="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:6" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A10" s="9" t="s">
         <v>23</v>
       </c>
@@ -1226,7 +1226,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="9" t="s">
         <v>25</v>
       </c>
@@ -1241,7 +1241,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="9" t="s">
         <v>27</v>
       </c>
@@ -1256,15 +1256,15 @@
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="25" t="s">
         <v>29</v>
       </c>
       <c r="B13" s="10" t="s">
+        <v>110</v>
+      </c>
+      <c r="C13" s="11" t="s">
         <v>30</v>
-      </c>
-      <c r="C13" s="11" t="s">
-        <v>31</v>
       </c>
       <c r="D13" s="15">
         <v>1.4999999999999999E-2</v>
@@ -1273,13 +1273,13 @@
         <v>12</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="25"/>
       <c r="B14" s="10" t="s">
-        <v>30</v>
+        <v>110</v>
       </c>
       <c r="C14" s="11" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D14" s="15">
         <v>1.4999999999999999E-2</v>
@@ -1288,13 +1288,13 @@
         <v>13</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="25"/>
       <c r="B15" s="10" t="s">
-        <v>30</v>
+        <v>110</v>
       </c>
       <c r="C15" s="11" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D15" s="15">
         <v>0.03</v>
@@ -1303,15 +1303,15 @@
         <v>14</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="25" t="s">
+        <v>33</v>
+      </c>
+      <c r="B16" s="10" t="s">
         <v>34</v>
       </c>
-      <c r="B16" s="10" t="s">
-        <v>35</v>
-      </c>
       <c r="C16" s="11" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D16" s="15">
         <v>1.444</v>
@@ -1320,13 +1320,13 @@
         <v>15</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="25"/>
       <c r="B17" s="10" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C17" s="11" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D17" s="15">
         <v>1.5129999999999999</v>
@@ -1335,13 +1335,13 @@
         <v>16</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" s="25"/>
       <c r="B18" s="10" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C18" s="11" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D18" s="15">
         <v>1.4630000000000001</v>
@@ -1350,12 +1350,12 @@
         <v>17</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="B19" s="10" t="s">
         <v>36</v>
-      </c>
-      <c r="B19" s="10" t="s">
-        <v>37</v>
       </c>
       <c r="C19" s="11"/>
       <c r="D19" s="15">
@@ -1365,30 +1365,30 @@
         <v>18</v>
       </c>
     </row>
-    <row r="20" spans="1:7" ht="30.6" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:7" ht="32.25" x14ac:dyDescent="0.25">
       <c r="A20" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="B20" s="10" t="s">
         <v>38</v>
-      </c>
-      <c r="B20" s="10" t="s">
-        <v>39</v>
       </c>
       <c r="C20" s="11"/>
       <c r="D20" s="15">
         <v>100</v>
       </c>
       <c r="E20" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="F20">
         <v>19</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="B21" s="10" t="s">
         <v>40</v>
-      </c>
-      <c r="B21" s="10" t="s">
-        <v>41</v>
       </c>
       <c r="C21" s="11"/>
       <c r="D21" s="15">
@@ -1398,101 +1398,101 @@
         <v>20</v>
       </c>
     </row>
-    <row r="22" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A22" s="26" t="s">
+        <v>41</v>
+      </c>
+      <c r="B22" s="10" t="s">
         <v>42</v>
       </c>
-      <c r="B22" s="10" t="s">
+      <c r="C22" s="11" t="s">
         <v>43</v>
-      </c>
-      <c r="C22" s="11" t="s">
-        <v>44</v>
       </c>
       <c r="D22" s="15"/>
       <c r="E22" s="16" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="F22">
         <v>21</v>
       </c>
       <c r="G22" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" s="26"/>
       <c r="B23" s="10" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C23" s="11" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D23" s="15"/>
       <c r="F23">
         <v>22</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" s="26"/>
       <c r="B24" s="10" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C24" s="11" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D24" s="15"/>
       <c r="F24">
         <v>23</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" s="26"/>
       <c r="B25" s="10" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C25" s="11" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D25" s="15"/>
       <c r="F25">
         <v>24</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" s="26"/>
       <c r="B26" s="10" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C26" s="11" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D26" s="15"/>
       <c r="F26">
         <v>25</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" s="26"/>
       <c r="B27" s="10" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C27" s="11" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D27" s="15"/>
       <c r="F27">
         <v>26</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" s="27" t="s">
+        <v>49</v>
+      </c>
+      <c r="B28" s="17" t="s">
         <v>50</v>
       </c>
-      <c r="B28" s="17" t="s">
-        <v>51</v>
-      </c>
       <c r="C28" s="18" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D28" s="15">
         <v>0.01</v>
@@ -1501,13 +1501,13 @@
         <v>27</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" s="27"/>
       <c r="B29" s="17" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C29" s="18" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D29" s="15">
         <v>0.1</v>
@@ -1516,13 +1516,13 @@
         <v>28</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" s="27"/>
       <c r="B30" s="17" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C30" s="18" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D30" s="15">
         <v>0.5</v>
@@ -1531,9 +1531,9 @@
         <v>29</v>
       </c>
     </row>
-    <row r="31" spans="1:7" ht="18" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="31" spans="1:7" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A31" s="5" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B31" s="6"/>
       <c r="C31" s="7"/>
@@ -1543,12 +1543,12 @@
         <v>30</v>
       </c>
     </row>
-    <row r="32" spans="1:7" ht="16.8" thickTop="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:7" ht="18" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A32" s="19" t="s">
+        <v>52</v>
+      </c>
+      <c r="B32" s="17" t="s">
         <v>53</v>
-      </c>
-      <c r="B32" s="17" t="s">
-        <v>54</v>
       </c>
       <c r="C32" s="18"/>
       <c r="D32" s="15">
@@ -1558,12 +1558,12 @@
         <v>31</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" s="19" t="s">
+        <v>54</v>
+      </c>
+      <c r="B33" s="17" t="s">
         <v>55</v>
-      </c>
-      <c r="B33" s="17" t="s">
-        <v>56</v>
       </c>
       <c r="C33" s="18"/>
       <c r="D33" s="15">
@@ -1573,12 +1573,12 @@
         <v>32</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34" s="19" t="s">
+        <v>56</v>
+      </c>
+      <c r="B34" s="17" t="s">
         <v>57</v>
-      </c>
-      <c r="B34" s="17" t="s">
-        <v>58</v>
       </c>
       <c r="C34" s="18"/>
       <c r="D34" s="15">
@@ -1588,12 +1588,12 @@
         <v>33</v>
       </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35" s="19" t="s">
+        <v>58</v>
+      </c>
+      <c r="B35" s="17" t="s">
         <v>59</v>
-      </c>
-      <c r="B35" s="17" t="s">
-        <v>60</v>
       </c>
       <c r="C35" s="18"/>
       <c r="D35" s="15">
@@ -1603,12 +1603,12 @@
         <v>34</v>
       </c>
     </row>
-    <row r="36" spans="1:6" ht="16.2" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:6" ht="17.25" x14ac:dyDescent="0.25">
       <c r="A36" s="19" t="s">
+        <v>60</v>
+      </c>
+      <c r="B36" s="17" t="s">
         <v>61</v>
-      </c>
-      <c r="B36" s="17" t="s">
-        <v>62</v>
       </c>
       <c r="C36" s="18"/>
       <c r="D36" s="15">
@@ -1618,9 +1618,9 @@
         <v>35</v>
       </c>
     </row>
-    <row r="37" spans="1:6" ht="18" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="37" spans="1:6" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A37" s="5" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B37" s="6"/>
       <c r="C37" s="7"/>
@@ -1630,12 +1630,12 @@
         <v>36</v>
       </c>
     </row>
-    <row r="38" spans="1:6" ht="29.4" thickTop="1" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:6" ht="30.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A38" s="19" t="s">
+        <v>63</v>
+      </c>
+      <c r="B38" s="17" t="s">
         <v>64</v>
-      </c>
-      <c r="B38" s="17" t="s">
-        <v>65</v>
       </c>
       <c r="C38" s="18"/>
       <c r="D38" s="15">
@@ -1645,12 +1645,12 @@
         <v>37</v>
       </c>
     </row>
-    <row r="39" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A39" s="19" t="s">
+        <v>65</v>
+      </c>
+      <c r="B39" s="17" t="s">
         <v>66</v>
-      </c>
-      <c r="B39" s="17" t="s">
-        <v>67</v>
       </c>
       <c r="C39" s="18"/>
       <c r="D39" s="15">
@@ -1660,12 +1660,12 @@
         <v>38</v>
       </c>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A40" s="19" t="s">
+        <v>67</v>
+      </c>
+      <c r="B40" s="17" t="s">
         <v>68</v>
-      </c>
-      <c r="B40" s="17" t="s">
-        <v>69</v>
       </c>
       <c r="C40" s="18"/>
       <c r="D40" s="15">
@@ -1675,9 +1675,9 @@
         <v>39</v>
       </c>
     </row>
-    <row r="41" spans="1:6" ht="18" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="41" spans="1:6" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A41" s="5" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B41" s="6"/>
       <c r="C41" s="7"/>
@@ -1687,12 +1687,12 @@
         <v>40</v>
       </c>
     </row>
-    <row r="42" spans="1:6" ht="15" thickTop="1" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:6" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A42" s="19" t="s">
+        <v>70</v>
+      </c>
+      <c r="B42" s="17" t="s">
         <v>71</v>
-      </c>
-      <c r="B42" s="17" t="s">
-        <v>72</v>
       </c>
       <c r="C42" s="18"/>
       <c r="D42" s="15">
@@ -1702,12 +1702,12 @@
         <v>41</v>
       </c>
     </row>
-    <row r="43" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A43" s="19" t="s">
+        <v>72</v>
+      </c>
+      <c r="B43" s="17" t="s">
         <v>73</v>
-      </c>
-      <c r="B43" s="17" t="s">
-        <v>74</v>
       </c>
       <c r="C43" s="18"/>
       <c r="D43" s="15">
@@ -1717,9 +1717,9 @@
         <v>42</v>
       </c>
     </row>
-    <row r="44" spans="1:6" ht="18" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="44" spans="1:6" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A44" s="5" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B44" s="6"/>
       <c r="C44" s="7"/>
@@ -1729,30 +1729,30 @@
         <v>43</v>
       </c>
     </row>
-    <row r="45" spans="1:6" ht="29.4" thickTop="1" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:6" ht="30.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A45" s="19" t="s">
+        <v>75</v>
+      </c>
+      <c r="B45" s="17" t="s">
         <v>76</v>
-      </c>
-      <c r="B45" s="17" t="s">
-        <v>77</v>
       </c>
       <c r="C45" s="18"/>
       <c r="D45" s="15">
         <v>0.25</v>
       </c>
       <c r="E45" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="F45">
         <v>44</v>
       </c>
     </row>
-    <row r="46" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A46" s="19" t="s">
+        <v>78</v>
+      </c>
+      <c r="B46" s="17" t="s">
         <v>79</v>
-      </c>
-      <c r="B46" s="17" t="s">
-        <v>80</v>
       </c>
       <c r="C46" s="18"/>
       <c r="D46" s="15">
@@ -1762,44 +1762,44 @@
         <v>45</v>
       </c>
     </row>
-    <row r="47" spans="1:6" ht="18" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="47" spans="1:6" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A47" s="5" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B47" s="6"/>
       <c r="C47" s="7"/>
       <c r="D47" s="6"/>
       <c r="E47" s="8" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="F47">
         <v>46</v>
       </c>
     </row>
-    <row r="48" spans="1:6" ht="15" thickTop="1" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:6" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A48" s="19" t="s">
+        <v>82</v>
+      </c>
+      <c r="B48" s="17" t="s">
         <v>83</v>
-      </c>
-      <c r="B48" s="17" t="s">
-        <v>84</v>
       </c>
       <c r="C48" s="18"/>
       <c r="D48" s="12" t="s">
+        <v>84</v>
+      </c>
+      <c r="E48" t="s">
         <v>85</v>
-      </c>
-      <c r="E48" t="s">
-        <v>86</v>
       </c>
       <c r="F48">
         <v>47</v>
       </c>
     </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A49" s="19" t="s">
+        <v>86</v>
+      </c>
+      <c r="B49" s="17" t="s">
         <v>87</v>
-      </c>
-      <c r="B49" s="17" t="s">
-        <v>88</v>
       </c>
       <c r="C49" s="18"/>
       <c r="D49" s="15">
@@ -1809,12 +1809,12 @@
         <v>48</v>
       </c>
     </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A50" s="19" t="s">
+        <v>88</v>
+      </c>
+      <c r="B50" s="17" t="s">
         <v>89</v>
-      </c>
-      <c r="B50" s="17" t="s">
-        <v>90</v>
       </c>
       <c r="C50" s="18">
         <v>1</v>
@@ -1826,10 +1826,10 @@
         <v>49</v>
       </c>
     </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A51" s="19"/>
       <c r="B51" s="17" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C51" s="18">
         <v>2</v>
@@ -1841,10 +1841,10 @@
         <v>50</v>
       </c>
     </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A52" s="19"/>
       <c r="B52" s="17" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C52" s="18">
         <v>3</v>
@@ -1856,10 +1856,10 @@
         <v>51</v>
       </c>
     </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A53" s="19"/>
       <c r="B53" s="17" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C53" s="18">
         <v>4</v>
@@ -1869,10 +1869,10 @@
         <v>52</v>
       </c>
     </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A54" s="19"/>
       <c r="B54" s="17" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C54" s="18">
         <v>5</v>
@@ -1882,12 +1882,12 @@
         <v>53</v>
       </c>
     </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A55" s="19" t="s">
+        <v>90</v>
+      </c>
+      <c r="B55" s="17" t="s">
         <v>91</v>
-      </c>
-      <c r="B55" s="17" t="s">
-        <v>92</v>
       </c>
       <c r="C55" s="18">
         <v>1</v>
@@ -1899,10 +1899,10 @@
         <v>54</v>
       </c>
     </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A56" s="19"/>
       <c r="B56" s="17" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C56" s="18">
         <v>2</v>
@@ -1914,10 +1914,10 @@
         <v>55</v>
       </c>
     </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A57" s="19"/>
       <c r="B57" s="17" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C57" s="18">
         <v>3</v>
@@ -1929,10 +1929,10 @@
         <v>56</v>
       </c>
     </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A58" s="19"/>
       <c r="B58" s="17" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C58" s="18">
         <v>4</v>
@@ -1942,10 +1942,10 @@
         <v>57</v>
       </c>
     </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A59" s="19"/>
       <c r="B59" s="17" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C59" s="18">
         <v>5</v>
@@ -1955,12 +1955,12 @@
         <v>58</v>
       </c>
     </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A60" s="19" t="s">
+        <v>92</v>
+      </c>
+      <c r="B60" s="17" t="s">
         <v>93</v>
-      </c>
-      <c r="B60" s="17" t="s">
-        <v>94</v>
       </c>
       <c r="C60" s="18">
         <v>1</v>
@@ -1972,10 +1972,10 @@
         <v>59</v>
       </c>
     </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A61" s="19"/>
       <c r="B61" s="17" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C61" s="18">
         <v>2</v>
@@ -1987,10 +1987,10 @@
         <v>60</v>
       </c>
     </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A62" s="19"/>
       <c r="B62" s="17" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C62" s="18">
         <v>3</v>
@@ -2002,10 +2002,10 @@
         <v>61</v>
       </c>
     </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A63" s="19"/>
       <c r="B63" s="17" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C63" s="18">
         <v>4</v>
@@ -2015,10 +2015,10 @@
         <v>62</v>
       </c>
     </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A64" s="19"/>
       <c r="B64" s="17" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C64" s="18">
         <v>5</v>
@@ -2028,27 +2028,27 @@
         <v>63</v>
       </c>
     </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A65" s="19" t="s">
+        <v>94</v>
+      </c>
+      <c r="B65" s="17" t="s">
         <v>95</v>
-      </c>
-      <c r="B65" s="17" t="s">
-        <v>96</v>
       </c>
       <c r="C65" s="18"/>
       <c r="D65" s="12" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="F65">
         <v>64</v>
       </c>
     </row>
-    <row r="66" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A66" s="19" t="s">
+        <v>97</v>
+      </c>
+      <c r="B66" s="17" t="s">
         <v>98</v>
-      </c>
-      <c r="B66" s="17" t="s">
-        <v>99</v>
       </c>
       <c r="C66" s="18"/>
       <c r="D66" s="15">
@@ -2058,12 +2058,12 @@
         <v>65</v>
       </c>
     </row>
-    <row r="67" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A67" s="19" t="s">
+        <v>99</v>
+      </c>
+      <c r="B67" s="17" t="s">
         <v>100</v>
-      </c>
-      <c r="B67" s="17" t="s">
-        <v>101</v>
       </c>
       <c r="C67" s="18">
         <v>1</v>
@@ -2075,10 +2075,10 @@
         <v>66</v>
       </c>
     </row>
-    <row r="68" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A68" s="19"/>
       <c r="B68" s="17" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C68" s="18">
         <v>2</v>
@@ -2090,10 +2090,10 @@
         <v>67</v>
       </c>
     </row>
-    <row r="69" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A69" s="19"/>
       <c r="B69" s="17" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C69" s="18">
         <v>3</v>
@@ -2105,10 +2105,10 @@
         <v>68</v>
       </c>
     </row>
-    <row r="70" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A70" s="19"/>
       <c r="B70" s="17" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C70" s="18">
         <v>4</v>
@@ -2120,10 +2120,10 @@
         <v>69</v>
       </c>
     </row>
-    <row r="71" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A71" s="19"/>
       <c r="B71" s="17" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C71" s="18">
         <v>5</v>
@@ -2135,12 +2135,12 @@
         <v>70</v>
       </c>
     </row>
-    <row r="72" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A72" s="19" t="s">
+        <v>101</v>
+      </c>
+      <c r="B72" s="17" t="s">
         <v>102</v>
-      </c>
-      <c r="B72" s="17" t="s">
-        <v>103</v>
       </c>
       <c r="C72" s="18">
         <v>1</v>
@@ -2152,10 +2152,10 @@
         <v>71</v>
       </c>
     </row>
-    <row r="73" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A73" s="19"/>
       <c r="B73" s="17" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C73" s="18">
         <v>2</v>
@@ -2167,10 +2167,10 @@
         <v>72</v>
       </c>
     </row>
-    <row r="74" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A74" s="19"/>
       <c r="B74" s="17" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C74" s="18">
         <v>3</v>
@@ -2182,10 +2182,10 @@
         <v>73</v>
       </c>
     </row>
-    <row r="75" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A75" s="19"/>
       <c r="B75" s="17" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C75" s="18">
         <v>4</v>
@@ -2197,10 +2197,10 @@
         <v>74</v>
       </c>
     </row>
-    <row r="76" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A76" s="19"/>
       <c r="B76" s="17" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C76" s="18">
         <v>5</v>
@@ -2212,12 +2212,12 @@
         <v>75</v>
       </c>
     </row>
-    <row r="77" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A77" s="19" t="s">
+        <v>103</v>
+      </c>
+      <c r="B77" s="17" t="s">
         <v>104</v>
-      </c>
-      <c r="B77" s="17" t="s">
-        <v>105</v>
       </c>
       <c r="C77" s="18">
         <v>1</v>
@@ -2229,10 +2229,10 @@
         <v>76</v>
       </c>
     </row>
-    <row r="78" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A78" s="19"/>
       <c r="B78" s="17" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C78" s="18">
         <v>2</v>
@@ -2244,10 +2244,10 @@
         <v>77</v>
       </c>
     </row>
-    <row r="79" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A79" s="19"/>
       <c r="B79" s="17" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C79" s="18">
         <v>3</v>
@@ -2259,10 +2259,10 @@
         <v>78</v>
       </c>
     </row>
-    <row r="80" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A80" s="19"/>
       <c r="B80" s="17" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C80" s="18">
         <v>4</v>
@@ -2274,10 +2274,10 @@
         <v>79</v>
       </c>
     </row>
-    <row r="81" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A81" s="19"/>
       <c r="B81" s="17" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C81" s="18">
         <v>5</v>
@@ -2289,602 +2289,602 @@
         <v>80</v>
       </c>
     </row>
-    <row r="82" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A82" s="20"/>
       <c r="B82" s="21"/>
       <c r="C82" s="22"/>
     </row>
-    <row r="83" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A83" s="20"/>
       <c r="B83" s="21"/>
       <c r="C83" s="22"/>
     </row>
-    <row r="84" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A84" s="20"/>
       <c r="B84" s="21"/>
       <c r="C84" s="22"/>
     </row>
-    <row r="85" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A85" s="20"/>
       <c r="B85" s="21"/>
       <c r="C85" s="22"/>
     </row>
-    <row r="86" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A86" s="20"/>
       <c r="B86" s="21"/>
       <c r="C86" s="22"/>
     </row>
-    <row r="87" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A87" s="20"/>
       <c r="B87" s="21"/>
       <c r="C87" s="22"/>
     </row>
-    <row r="88" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A88" s="20"/>
       <c r="B88" s="21"/>
       <c r="C88" s="22"/>
     </row>
-    <row r="89" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A89" s="20"/>
       <c r="B89" s="21"/>
       <c r="C89" s="22"/>
     </row>
-    <row r="90" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A90" s="20"/>
       <c r="B90" s="21"/>
       <c r="C90" s="22"/>
     </row>
-    <row r="91" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A91" s="20"/>
       <c r="B91" s="21"/>
       <c r="C91" s="22"/>
     </row>
-    <row r="92" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A92" s="20"/>
       <c r="B92" s="21"/>
       <c r="C92" s="22"/>
     </row>
-    <row r="93" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A93" s="20"/>
       <c r="B93" s="21"/>
       <c r="C93" s="22"/>
     </row>
-    <row r="94" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A94" s="20"/>
       <c r="B94" s="21"/>
       <c r="C94" s="22"/>
     </row>
-    <row r="95" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A95" s="20"/>
       <c r="B95" s="21"/>
       <c r="C95" s="22"/>
     </row>
-    <row r="96" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A96" s="20"/>
       <c r="B96" s="21"/>
       <c r="C96" s="22"/>
     </row>
-    <row r="97" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A97" s="20"/>
       <c r="B97" s="21"/>
       <c r="C97" s="22"/>
     </row>
-    <row r="98" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A98" s="20"/>
       <c r="B98" s="21"/>
       <c r="C98" s="22"/>
     </row>
-    <row r="99" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A99" s="20"/>
       <c r="B99" s="21"/>
       <c r="C99" s="22"/>
     </row>
-    <row r="100" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A100" s="20"/>
       <c r="B100" s="21"/>
       <c r="C100" s="22"/>
     </row>
-    <row r="101" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A101" s="20"/>
       <c r="B101" s="21"/>
       <c r="C101" s="22"/>
     </row>
-    <row r="102" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A102" s="20"/>
       <c r="B102" s="21"/>
       <c r="C102" s="22"/>
     </row>
-    <row r="103" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A103" s="20"/>
       <c r="B103" s="21"/>
       <c r="C103" s="22"/>
     </row>
-    <row r="104" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A104" s="20"/>
       <c r="B104" s="21"/>
       <c r="C104" s="22"/>
     </row>
-    <row r="105" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A105" s="20"/>
       <c r="B105" s="21"/>
       <c r="C105" s="22"/>
     </row>
-    <row r="106" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A106" s="20"/>
       <c r="B106" s="21"/>
       <c r="C106" s="22"/>
     </row>
-    <row r="107" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A107" s="20"/>
       <c r="B107" s="21"/>
       <c r="C107" s="22"/>
     </row>
-    <row r="108" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A108" s="20"/>
       <c r="B108" s="21"/>
       <c r="C108" s="22"/>
     </row>
-    <row r="109" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A109" s="20"/>
       <c r="B109" s="21"/>
       <c r="C109" s="22"/>
     </row>
-    <row r="110" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A110" s="20"/>
       <c r="B110" s="21"/>
       <c r="C110" s="22"/>
     </row>
-    <row r="111" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A111" s="20"/>
       <c r="B111" s="21"/>
       <c r="C111" s="22"/>
     </row>
-    <row r="112" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A112" s="20"/>
       <c r="B112" s="21"/>
       <c r="C112" s="22"/>
     </row>
-    <row r="113" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A113" s="20"/>
       <c r="B113" s="21"/>
       <c r="C113" s="22"/>
     </row>
-    <row r="114" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A114" s="20"/>
       <c r="B114" s="21"/>
       <c r="C114" s="22"/>
     </row>
-    <row r="115" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A115" s="20"/>
       <c r="B115" s="21"/>
       <c r="C115" s="22"/>
     </row>
-    <row r="116" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A116" s="20"/>
       <c r="B116" s="21"/>
       <c r="C116" s="22"/>
     </row>
-    <row r="117" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A117" s="20"/>
       <c r="B117" s="21"/>
       <c r="C117" s="22"/>
     </row>
-    <row r="118" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A118" s="20"/>
       <c r="B118" s="21"/>
       <c r="C118" s="22"/>
     </row>
-    <row r="119" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A119" s="20"/>
       <c r="B119" s="21"/>
       <c r="C119" s="22"/>
     </row>
-    <row r="120" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A120" s="20"/>
       <c r="B120" s="21"/>
       <c r="C120" s="22"/>
     </row>
-    <row r="121" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A121" s="20"/>
       <c r="B121" s="21"/>
       <c r="C121" s="22"/>
     </row>
-    <row r="122" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A122" s="20"/>
       <c r="B122" s="21"/>
       <c r="C122" s="22"/>
     </row>
-    <row r="123" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A123" s="20"/>
       <c r="B123" s="21"/>
       <c r="C123" s="22"/>
     </row>
-    <row r="124" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A124" s="20"/>
       <c r="B124" s="21"/>
       <c r="C124" s="22"/>
     </row>
-    <row r="125" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A125" s="20"/>
       <c r="B125" s="21"/>
       <c r="C125" s="22"/>
     </row>
-    <row r="126" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="126" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A126" s="20"/>
       <c r="B126" s="21"/>
       <c r="C126" s="22"/>
     </row>
-    <row r="127" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="127" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A127" s="20"/>
       <c r="B127" s="21"/>
       <c r="C127" s="22"/>
     </row>
-    <row r="128" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="128" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A128" s="20"/>
       <c r="B128" s="21"/>
       <c r="C128" s="22"/>
     </row>
-    <row r="129" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="129" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A129" s="20"/>
       <c r="B129" s="21"/>
       <c r="C129" s="22"/>
     </row>
-    <row r="130" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="130" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A130" s="20"/>
       <c r="B130" s="21"/>
       <c r="C130" s="22"/>
     </row>
-    <row r="131" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="131" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A131" s="20"/>
       <c r="B131" s="21"/>
       <c r="C131" s="22"/>
     </row>
-    <row r="132" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="132" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A132" s="20"/>
       <c r="B132" s="21"/>
       <c r="C132" s="22"/>
     </row>
-    <row r="133" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="133" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A133" s="20"/>
       <c r="B133" s="21"/>
       <c r="C133" s="22"/>
     </row>
-    <row r="134" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="134" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A134" s="20"/>
       <c r="B134" s="21"/>
       <c r="C134" s="22"/>
     </row>
-    <row r="135" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="135" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A135" s="20"/>
       <c r="B135" s="21"/>
       <c r="C135" s="22"/>
     </row>
-    <row r="136" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="136" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A136" s="20"/>
       <c r="B136" s="21"/>
       <c r="C136" s="22"/>
     </row>
-    <row r="137" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="137" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A137" s="20"/>
       <c r="B137" s="21"/>
       <c r="C137" s="22"/>
     </row>
-    <row r="138" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="138" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A138" s="20"/>
       <c r="B138" s="21"/>
       <c r="C138" s="22"/>
     </row>
-    <row r="139" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="139" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A139" s="20"/>
       <c r="B139" s="21"/>
       <c r="C139" s="22"/>
     </row>
-    <row r="140" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="140" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A140" s="20"/>
       <c r="B140" s="21"/>
       <c r="C140" s="22"/>
     </row>
-    <row r="141" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="141" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A141" s="20"/>
       <c r="B141" s="21"/>
       <c r="C141" s="22"/>
     </row>
-    <row r="142" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="142" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A142" s="20"/>
       <c r="B142" s="21"/>
       <c r="C142" s="22"/>
     </row>
-    <row r="143" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="143" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A143" s="20"/>
       <c r="B143" s="21"/>
       <c r="C143" s="22"/>
     </row>
-    <row r="144" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="144" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A144" s="20"/>
       <c r="B144" s="21"/>
       <c r="C144" s="22"/>
     </row>
-    <row r="145" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="145" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A145" s="20"/>
       <c r="B145" s="21"/>
       <c r="C145" s="22"/>
     </row>
-    <row r="146" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="146" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A146" s="20"/>
       <c r="B146" s="21"/>
       <c r="C146" s="22"/>
     </row>
-    <row r="147" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="147" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A147" s="20"/>
       <c r="B147" s="21"/>
       <c r="C147" s="22"/>
     </row>
-    <row r="148" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="148" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A148" s="20"/>
       <c r="B148" s="21"/>
       <c r="C148" s="22"/>
     </row>
-    <row r="149" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="149" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A149" s="20"/>
       <c r="B149" s="21"/>
       <c r="C149" s="22"/>
     </row>
-    <row r="150" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="150" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A150" s="20"/>
       <c r="B150" s="21"/>
       <c r="C150" s="22"/>
     </row>
-    <row r="151" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="151" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A151" s="20"/>
       <c r="B151" s="21"/>
       <c r="C151" s="22"/>
     </row>
-    <row r="152" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="152" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A152" s="20"/>
       <c r="B152" s="21"/>
       <c r="C152" s="22"/>
     </row>
-    <row r="153" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="153" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A153" s="20"/>
       <c r="B153" s="21"/>
       <c r="C153" s="22"/>
     </row>
-    <row r="154" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="154" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A154" s="20"/>
       <c r="B154" s="21"/>
       <c r="C154" s="22"/>
     </row>
-    <row r="155" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="155" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A155" s="20"/>
       <c r="B155" s="21"/>
       <c r="C155" s="22"/>
     </row>
-    <row r="156" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="156" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A156" s="20"/>
       <c r="B156" s="21"/>
       <c r="C156" s="22"/>
     </row>
-    <row r="157" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="157" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A157" s="20"/>
       <c r="B157" s="21"/>
       <c r="C157" s="22"/>
     </row>
-    <row r="158" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="158" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A158" s="20"/>
       <c r="B158" s="21"/>
       <c r="C158" s="22"/>
     </row>
-    <row r="159" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="159" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A159" s="20"/>
       <c r="B159" s="21"/>
       <c r="C159" s="22"/>
     </row>
-    <row r="160" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="160" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A160" s="20"/>
       <c r="B160" s="21"/>
       <c r="C160" s="22"/>
     </row>
-    <row r="161" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="161" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A161" s="20"/>
       <c r="B161" s="21"/>
       <c r="C161" s="22"/>
     </row>
-    <row r="162" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="162" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A162" s="20"/>
       <c r="B162" s="21"/>
       <c r="C162" s="22"/>
     </row>
-    <row r="163" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="163" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A163" s="20"/>
       <c r="B163" s="21"/>
       <c r="C163" s="22"/>
     </row>
-    <row r="164" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="164" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A164" s="20"/>
       <c r="B164" s="21"/>
       <c r="C164" s="22"/>
     </row>
-    <row r="165" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="165" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A165" s="20"/>
       <c r="B165" s="21"/>
       <c r="C165" s="22"/>
     </row>
-    <row r="166" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="166" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A166" s="20"/>
       <c r="B166" s="21"/>
       <c r="C166" s="22"/>
     </row>
-    <row r="167" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="167" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A167" s="20"/>
       <c r="B167" s="21"/>
       <c r="C167" s="22"/>
     </row>
-    <row r="168" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="168" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A168" s="20"/>
       <c r="B168" s="21"/>
       <c r="C168" s="22"/>
     </row>
-    <row r="169" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="169" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A169" s="20"/>
       <c r="B169" s="21"/>
       <c r="C169" s="22"/>
     </row>
-    <row r="170" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="170" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A170" s="20"/>
       <c r="B170" s="21"/>
       <c r="C170" s="22"/>
     </row>
-    <row r="171" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="171" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A171" s="20"/>
       <c r="B171" s="21"/>
       <c r="C171" s="22"/>
     </row>
-    <row r="172" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="172" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A172" s="20"/>
       <c r="B172" s="21"/>
       <c r="C172" s="22"/>
     </row>
-    <row r="173" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="173" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A173" s="20"/>
       <c r="B173" s="21"/>
       <c r="C173" s="22"/>
     </row>
-    <row r="174" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="174" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A174" s="20"/>
       <c r="B174" s="21"/>
       <c r="C174" s="22"/>
     </row>
-    <row r="175" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="175" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A175" s="20"/>
       <c r="B175" s="21"/>
       <c r="C175" s="22"/>
     </row>
-    <row r="176" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="176" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A176" s="20"/>
       <c r="B176" s="21"/>
       <c r="C176" s="22"/>
     </row>
-    <row r="177" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="177" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A177" s="20"/>
       <c r="B177" s="21"/>
       <c r="C177" s="22"/>
     </row>
-    <row r="178" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="178" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A178" s="20"/>
       <c r="B178" s="21"/>
       <c r="C178" s="22"/>
     </row>
-    <row r="179" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="179" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A179" s="20"/>
       <c r="B179" s="21"/>
       <c r="C179" s="22"/>
     </row>
-    <row r="180" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="180" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A180" s="20"/>
       <c r="B180" s="21"/>
       <c r="C180" s="22"/>
     </row>
-    <row r="181" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="181" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A181" s="20"/>
       <c r="B181" s="21"/>
       <c r="C181" s="22"/>
     </row>
-    <row r="182" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="182" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A182" s="20"/>
       <c r="B182" s="21"/>
       <c r="C182" s="22"/>
     </row>
-    <row r="183" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="183" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A183" s="20"/>
       <c r="B183" s="21"/>
       <c r="C183" s="22"/>
     </row>
-    <row r="184" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="184" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A184" s="20"/>
       <c r="B184" s="21"/>
       <c r="C184" s="22"/>
     </row>
-    <row r="185" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="185" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A185" s="20"/>
       <c r="B185" s="21"/>
       <c r="C185" s="22"/>
     </row>
-    <row r="186" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="186" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A186" s="20"/>
       <c r="B186" s="21"/>
       <c r="C186" s="22"/>
     </row>
-    <row r="187" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="187" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A187" s="20"/>
       <c r="B187" s="21"/>
       <c r="C187" s="22"/>
     </row>
-    <row r="188" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="188" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A188" s="20"/>
       <c r="B188" s="21"/>
       <c r="C188" s="22"/>
     </row>
-    <row r="189" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="189" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A189" s="20"/>
       <c r="B189" s="21"/>
       <c r="C189" s="22"/>
     </row>
-    <row r="190" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="190" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A190" s="20"/>
       <c r="B190" s="21"/>
       <c r="C190" s="22"/>
     </row>
-    <row r="191" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="191" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A191" s="20"/>
       <c r="B191" s="21"/>
       <c r="C191" s="22"/>
     </row>
-    <row r="192" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="192" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A192" s="20"/>
       <c r="B192" s="21"/>
       <c r="C192" s="22"/>
     </row>
-    <row r="193" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="193" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A193" s="20"/>
       <c r="B193" s="21"/>
       <c r="C193" s="22"/>
     </row>
-    <row r="194" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="194" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A194" s="20"/>
       <c r="B194" s="21"/>
       <c r="C194" s="22"/>
     </row>
-    <row r="195" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="195" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A195" s="20"/>
       <c r="B195" s="21"/>
       <c r="C195" s="22"/>
     </row>
-    <row r="196" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="196" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A196" s="20"/>
       <c r="B196" s="21"/>
       <c r="C196" s="22"/>
     </row>
-    <row r="197" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="197" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A197" s="20"/>
       <c r="B197" s="21"/>
       <c r="C197" s="22"/>
     </row>
-    <row r="198" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="198" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A198" s="20"/>
       <c r="B198" s="21"/>
       <c r="C198" s="22"/>
     </row>
-    <row r="199" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="199" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A199" s="20"/>
       <c r="B199" s="21"/>
       <c r="C199" s="22"/>
     </row>
-    <row r="200" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="200" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A200" s="20"/>
       <c r="B200" s="21"/>
       <c r="C200" s="22"/>
     </row>
-    <row r="201" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="201" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A201" s="20"/>
       <c r="B201" s="21"/>
       <c r="C201" s="22"/>
@@ -2935,20 +2935,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7A5B2ED1-E60A-481E-A183-520033C5AF7F}">
   <dimension ref="A1:G201"/>
   <sheetViews>
-    <sheetView topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="A22" sqref="A22:A27"/>
+    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="37.44140625" style="23" customWidth="1"/>
-    <col min="2" max="2" width="20.33203125" style="15" customWidth="1"/>
-    <col min="3" max="3" width="15.44140625" style="24" customWidth="1"/>
-    <col min="4" max="4" width="20.33203125" customWidth="1"/>
-    <col min="5" max="5" width="64.109375" customWidth="1"/>
+    <col min="1" max="1" width="37.42578125" style="23" customWidth="1"/>
+    <col min="2" max="2" width="20.28515625" style="15" customWidth="1"/>
+    <col min="3" max="3" width="15.42578125" style="24" customWidth="1"/>
+    <col min="4" max="4" width="20.28515625" customWidth="1"/>
+    <col min="5" max="5" width="64.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="20.399999999999999" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:6" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2968,7 +2968,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="18.600000000000001" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:6" ht="18.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="5" t="s">
         <v>5</v>
       </c>
@@ -2980,7 +2980,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="15" thickTop="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A3" s="9" t="s">
         <v>6</v>
       </c>
@@ -2989,13 +2989,13 @@
       </c>
       <c r="C3" s="11"/>
       <c r="D3" s="12" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="F3">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="9" t="s">
         <v>8</v>
       </c>
@@ -3010,7 +3010,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="9" t="s">
         <v>11</v>
       </c>
@@ -3025,7 +3025,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="9" t="s">
         <v>14</v>
       </c>
@@ -3040,7 +3040,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="9" t="s">
         <v>17</v>
       </c>
@@ -3049,13 +3049,13 @@
       </c>
       <c r="C7" s="11"/>
       <c r="D7" s="12" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="F7">
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="9" t="s">
         <v>19</v>
       </c>
@@ -3070,7 +3070,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="18" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:6" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A9" s="5" t="s">
         <v>22</v>
       </c>
@@ -3082,7 +3082,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="15" thickTop="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:6" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A10" s="9" t="s">
         <v>23</v>
       </c>
@@ -3097,7 +3097,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="9" t="s">
         <v>25</v>
       </c>
@@ -3112,7 +3112,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="9" t="s">
         <v>27</v>
       </c>
@@ -3127,15 +3127,15 @@
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="25" t="s">
         <v>29</v>
       </c>
       <c r="B13" s="10" t="s">
+        <v>110</v>
+      </c>
+      <c r="C13" s="11" t="s">
         <v>30</v>
-      </c>
-      <c r="C13" s="11" t="s">
-        <v>31</v>
       </c>
       <c r="D13" s="15">
         <v>1.4999999999999999E-2</v>
@@ -3144,13 +3144,13 @@
         <v>12</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="25"/>
       <c r="B14" s="10" t="s">
-        <v>30</v>
+        <v>110</v>
       </c>
       <c r="C14" s="11" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D14" s="15">
         <v>1.4999999999999999E-2</v>
@@ -3159,13 +3159,13 @@
         <v>13</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="25"/>
       <c r="B15" s="10" t="s">
-        <v>30</v>
+        <v>110</v>
       </c>
       <c r="C15" s="11" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D15" s="15">
         <v>0.03</v>
@@ -3174,15 +3174,15 @@
         <v>14</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="25" t="s">
+        <v>33</v>
+      </c>
+      <c r="B16" s="10" t="s">
         <v>34</v>
       </c>
-      <c r="B16" s="10" t="s">
-        <v>35</v>
-      </c>
       <c r="C16" s="11" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D16" s="15">
         <v>1.444</v>
@@ -3191,13 +3191,13 @@
         <v>15</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="25"/>
       <c r="B17" s="10" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C17" s="11" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D17" s="15">
         <v>1.5129999999999999</v>
@@ -3206,13 +3206,13 @@
         <v>16</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" s="25"/>
       <c r="B18" s="10" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C18" s="11" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D18" s="15">
         <v>1.4630000000000001</v>
@@ -3221,12 +3221,12 @@
         <v>17</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="B19" s="10" t="s">
         <v>36</v>
-      </c>
-      <c r="B19" s="10" t="s">
-        <v>37</v>
       </c>
       <c r="C19" s="11"/>
       <c r="D19" s="15">
@@ -3236,30 +3236,30 @@
         <v>18</v>
       </c>
     </row>
-    <row r="20" spans="1:7" ht="30.6" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:7" ht="32.25" x14ac:dyDescent="0.25">
       <c r="A20" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="B20" s="10" t="s">
         <v>38</v>
-      </c>
-      <c r="B20" s="10" t="s">
-        <v>39</v>
       </c>
       <c r="C20" s="11"/>
       <c r="D20" s="15">
         <v>100</v>
       </c>
       <c r="E20" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="F20">
         <v>19</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="B21" s="10" t="s">
         <v>40</v>
-      </c>
-      <c r="B21" s="10" t="s">
-        <v>41</v>
       </c>
       <c r="C21" s="11"/>
       <c r="D21" s="15">
@@ -3269,101 +3269,101 @@
         <v>20</v>
       </c>
     </row>
-    <row r="22" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A22" s="26" t="s">
+        <v>41</v>
+      </c>
+      <c r="B22" s="10" t="s">
         <v>42</v>
       </c>
-      <c r="B22" s="10" t="s">
+      <c r="C22" s="11" t="s">
         <v>43</v>
-      </c>
-      <c r="C22" s="11" t="s">
-        <v>44</v>
       </c>
       <c r="D22" s="15"/>
       <c r="E22" s="16" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="F22">
         <v>21</v>
       </c>
       <c r="G22" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" s="26"/>
       <c r="B23" s="10" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C23" s="11" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D23" s="15"/>
       <c r="F23">
         <v>22</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" s="26"/>
       <c r="B24" s="10" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C24" s="11" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D24" s="15"/>
       <c r="F24">
         <v>23</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" s="26"/>
       <c r="B25" s="10" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C25" s="11" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D25" s="15"/>
       <c r="F25">
         <v>24</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" s="26"/>
       <c r="B26" s="10" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C26" s="11" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D26" s="15"/>
       <c r="F26">
         <v>25</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" s="26"/>
       <c r="B27" s="10" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C27" s="11" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D27" s="15"/>
       <c r="F27">
         <v>26</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" s="27" t="s">
+        <v>49</v>
+      </c>
+      <c r="B28" s="17" t="s">
         <v>50</v>
       </c>
-      <c r="B28" s="17" t="s">
-        <v>51</v>
-      </c>
       <c r="C28" s="18" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D28" s="15">
         <v>0.01</v>
@@ -3372,13 +3372,13 @@
         <v>27</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" s="27"/>
       <c r="B29" s="17" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C29" s="18" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D29" s="15">
         <v>0.1</v>
@@ -3387,13 +3387,13 @@
         <v>28</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" s="27"/>
       <c r="B30" s="17" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C30" s="18" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D30" s="15">
         <v>0.5</v>
@@ -3402,9 +3402,9 @@
         <v>29</v>
       </c>
     </row>
-    <row r="31" spans="1:7" ht="18" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="31" spans="1:7" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A31" s="5" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B31" s="6"/>
       <c r="C31" s="7"/>
@@ -3414,12 +3414,12 @@
         <v>30</v>
       </c>
     </row>
-    <row r="32" spans="1:7" ht="16.8" thickTop="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:7" ht="18" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A32" s="19" t="s">
+        <v>52</v>
+      </c>
+      <c r="B32" s="17" t="s">
         <v>53</v>
-      </c>
-      <c r="B32" s="17" t="s">
-        <v>54</v>
       </c>
       <c r="C32" s="18"/>
       <c r="D32" s="15">
@@ -3429,12 +3429,12 @@
         <v>31</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" s="19" t="s">
+        <v>54</v>
+      </c>
+      <c r="B33" s="17" t="s">
         <v>55</v>
-      </c>
-      <c r="B33" s="17" t="s">
-        <v>56</v>
       </c>
       <c r="C33" s="18"/>
       <c r="D33" s="15">
@@ -3444,12 +3444,12 @@
         <v>32</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34" s="19" t="s">
+        <v>56</v>
+      </c>
+      <c r="B34" s="17" t="s">
         <v>57</v>
-      </c>
-      <c r="B34" s="17" t="s">
-        <v>58</v>
       </c>
       <c r="C34" s="18"/>
       <c r="D34" s="15">
@@ -3459,12 +3459,12 @@
         <v>33</v>
       </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35" s="19" t="s">
+        <v>58</v>
+      </c>
+      <c r="B35" s="17" t="s">
         <v>59</v>
-      </c>
-      <c r="B35" s="17" t="s">
-        <v>60</v>
       </c>
       <c r="C35" s="18"/>
       <c r="D35" s="15">
@@ -3474,12 +3474,12 @@
         <v>34</v>
       </c>
     </row>
-    <row r="36" spans="1:6" ht="16.2" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:6" ht="17.25" x14ac:dyDescent="0.25">
       <c r="A36" s="19" t="s">
+        <v>60</v>
+      </c>
+      <c r="B36" s="17" t="s">
         <v>61</v>
-      </c>
-      <c r="B36" s="17" t="s">
-        <v>62</v>
       </c>
       <c r="C36" s="18"/>
       <c r="D36" s="15">
@@ -3489,9 +3489,9 @@
         <v>35</v>
       </c>
     </row>
-    <row r="37" spans="1:6" ht="18" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="37" spans="1:6" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A37" s="5" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B37" s="6"/>
       <c r="C37" s="7"/>
@@ -3501,12 +3501,12 @@
         <v>36</v>
       </c>
     </row>
-    <row r="38" spans="1:6" ht="29.4" thickTop="1" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:6" ht="30.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A38" s="19" t="s">
+        <v>63</v>
+      </c>
+      <c r="B38" s="17" t="s">
         <v>64</v>
-      </c>
-      <c r="B38" s="17" t="s">
-        <v>65</v>
       </c>
       <c r="C38" s="18"/>
       <c r="D38" s="15">
@@ -3516,12 +3516,12 @@
         <v>37</v>
       </c>
     </row>
-    <row r="39" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A39" s="19" t="s">
+        <v>65</v>
+      </c>
+      <c r="B39" s="17" t="s">
         <v>66</v>
-      </c>
-      <c r="B39" s="17" t="s">
-        <v>67</v>
       </c>
       <c r="C39" s="18"/>
       <c r="D39" s="15">
@@ -3531,12 +3531,12 @@
         <v>38</v>
       </c>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A40" s="19" t="s">
+        <v>67</v>
+      </c>
+      <c r="B40" s="17" t="s">
         <v>68</v>
-      </c>
-      <c r="B40" s="17" t="s">
-        <v>69</v>
       </c>
       <c r="C40" s="18"/>
       <c r="D40" s="15">
@@ -3546,9 +3546,9 @@
         <v>39</v>
       </c>
     </row>
-    <row r="41" spans="1:6" ht="18" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="41" spans="1:6" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A41" s="5" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B41" s="6"/>
       <c r="C41" s="7"/>
@@ -3558,12 +3558,12 @@
         <v>40</v>
       </c>
     </row>
-    <row r="42" spans="1:6" ht="15" thickTop="1" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:6" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A42" s="19" t="s">
+        <v>70</v>
+      </c>
+      <c r="B42" s="17" t="s">
         <v>71</v>
-      </c>
-      <c r="B42" s="17" t="s">
-        <v>72</v>
       </c>
       <c r="C42" s="18"/>
       <c r="D42" s="15">
@@ -3573,12 +3573,12 @@
         <v>41</v>
       </c>
     </row>
-    <row r="43" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A43" s="19" t="s">
+        <v>72</v>
+      </c>
+      <c r="B43" s="17" t="s">
         <v>73</v>
-      </c>
-      <c r="B43" s="17" t="s">
-        <v>74</v>
       </c>
       <c r="C43" s="18"/>
       <c r="D43" s="15">
@@ -3588,9 +3588,9 @@
         <v>42</v>
       </c>
     </row>
-    <row r="44" spans="1:6" ht="18" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="44" spans="1:6" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A44" s="5" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B44" s="6"/>
       <c r="C44" s="7"/>
@@ -3600,30 +3600,30 @@
         <v>43</v>
       </c>
     </row>
-    <row r="45" spans="1:6" ht="29.4" thickTop="1" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:6" ht="30.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A45" s="19" t="s">
+        <v>75</v>
+      </c>
+      <c r="B45" s="17" t="s">
         <v>76</v>
-      </c>
-      <c r="B45" s="17" t="s">
-        <v>77</v>
       </c>
       <c r="C45" s="18"/>
       <c r="D45" s="15">
         <v>0.25</v>
       </c>
       <c r="E45" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="F45">
         <v>44</v>
       </c>
     </row>
-    <row r="46" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A46" s="19" t="s">
+        <v>78</v>
+      </c>
+      <c r="B46" s="17" t="s">
         <v>79</v>
-      </c>
-      <c r="B46" s="17" t="s">
-        <v>80</v>
       </c>
       <c r="C46" s="18"/>
       <c r="D46" s="15">
@@ -3633,44 +3633,44 @@
         <v>45</v>
       </c>
     </row>
-    <row r="47" spans="1:6" ht="18" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="47" spans="1:6" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A47" s="5" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B47" s="6"/>
       <c r="C47" s="7"/>
       <c r="D47" s="6"/>
       <c r="E47" s="8" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="F47">
         <v>46</v>
       </c>
     </row>
-    <row r="48" spans="1:6" ht="15" thickTop="1" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:6" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A48" s="19" t="s">
+        <v>82</v>
+      </c>
+      <c r="B48" s="17" t="s">
         <v>83</v>
-      </c>
-      <c r="B48" s="17" t="s">
-        <v>84</v>
       </c>
       <c r="C48" s="18"/>
       <c r="D48" s="12" t="s">
+        <v>84</v>
+      </c>
+      <c r="E48" t="s">
         <v>85</v>
-      </c>
-      <c r="E48" t="s">
-        <v>86</v>
       </c>
       <c r="F48">
         <v>47</v>
       </c>
     </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A49" s="19" t="s">
+        <v>86</v>
+      </c>
+      <c r="B49" s="17" t="s">
         <v>87</v>
-      </c>
-      <c r="B49" s="17" t="s">
-        <v>88</v>
       </c>
       <c r="C49" s="18"/>
       <c r="D49" s="15">
@@ -3680,12 +3680,12 @@
         <v>48</v>
       </c>
     </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A50" s="19" t="s">
+        <v>88</v>
+      </c>
+      <c r="B50" s="17" t="s">
         <v>89</v>
-      </c>
-      <c r="B50" s="17" t="s">
-        <v>90</v>
       </c>
       <c r="C50" s="18">
         <v>1</v>
@@ -3697,10 +3697,10 @@
         <v>49</v>
       </c>
     </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A51" s="19"/>
       <c r="B51" s="17" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C51" s="18">
         <v>2</v>
@@ -3712,10 +3712,10 @@
         <v>50</v>
       </c>
     </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A52" s="19"/>
       <c r="B52" s="17" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C52" s="18">
         <v>3</v>
@@ -3727,10 +3727,10 @@
         <v>51</v>
       </c>
     </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A53" s="19"/>
       <c r="B53" s="17" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C53" s="18">
         <v>4</v>
@@ -3740,10 +3740,10 @@
         <v>52</v>
       </c>
     </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A54" s="19"/>
       <c r="B54" s="17" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C54" s="18">
         <v>5</v>
@@ -3753,12 +3753,12 @@
         <v>53</v>
       </c>
     </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A55" s="19" t="s">
+        <v>90</v>
+      </c>
+      <c r="B55" s="17" t="s">
         <v>91</v>
-      </c>
-      <c r="B55" s="17" t="s">
-        <v>92</v>
       </c>
       <c r="C55" s="18">
         <v>1</v>
@@ -3770,10 +3770,10 @@
         <v>54</v>
       </c>
     </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A56" s="19"/>
       <c r="B56" s="17" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C56" s="18">
         <v>2</v>
@@ -3785,10 +3785,10 @@
         <v>55</v>
       </c>
     </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A57" s="19"/>
       <c r="B57" s="17" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C57" s="18">
         <v>3</v>
@@ -3800,10 +3800,10 @@
         <v>56</v>
       </c>
     </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A58" s="19"/>
       <c r="B58" s="17" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C58" s="18">
         <v>4</v>
@@ -3813,10 +3813,10 @@
         <v>57</v>
       </c>
     </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A59" s="19"/>
       <c r="B59" s="17" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C59" s="18">
         <v>5</v>
@@ -3826,12 +3826,12 @@
         <v>58</v>
       </c>
     </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A60" s="19" t="s">
+        <v>92</v>
+      </c>
+      <c r="B60" s="17" t="s">
         <v>93</v>
-      </c>
-      <c r="B60" s="17" t="s">
-        <v>94</v>
       </c>
       <c r="C60" s="18">
         <v>1</v>
@@ -3843,10 +3843,10 @@
         <v>59</v>
       </c>
     </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A61" s="19"/>
       <c r="B61" s="17" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C61" s="18">
         <v>2</v>
@@ -3858,10 +3858,10 @@
         <v>60</v>
       </c>
     </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A62" s="19"/>
       <c r="B62" s="17" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C62" s="18">
         <v>3</v>
@@ -3873,10 +3873,10 @@
         <v>61</v>
       </c>
     </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A63" s="19"/>
       <c r="B63" s="17" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C63" s="18">
         <v>4</v>
@@ -3886,10 +3886,10 @@
         <v>62</v>
       </c>
     </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A64" s="19"/>
       <c r="B64" s="17" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C64" s="18">
         <v>5</v>
@@ -3899,27 +3899,27 @@
         <v>63</v>
       </c>
     </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A65" s="19" t="s">
+        <v>94</v>
+      </c>
+      <c r="B65" s="17" t="s">
         <v>95</v>
-      </c>
-      <c r="B65" s="17" t="s">
-        <v>96</v>
       </c>
       <c r="C65" s="18"/>
       <c r="D65" s="12" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="F65">
         <v>64</v>
       </c>
     </row>
-    <row r="66" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A66" s="19" t="s">
+        <v>97</v>
+      </c>
+      <c r="B66" s="17" t="s">
         <v>98</v>
-      </c>
-      <c r="B66" s="17" t="s">
-        <v>99</v>
       </c>
       <c r="C66" s="18"/>
       <c r="D66" s="15">
@@ -3929,12 +3929,12 @@
         <v>65</v>
       </c>
     </row>
-    <row r="67" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A67" s="19" t="s">
+        <v>99</v>
+      </c>
+      <c r="B67" s="17" t="s">
         <v>100</v>
-      </c>
-      <c r="B67" s="17" t="s">
-        <v>101</v>
       </c>
       <c r="C67" s="18">
         <v>1</v>
@@ -3946,10 +3946,10 @@
         <v>66</v>
       </c>
     </row>
-    <row r="68" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A68" s="19"/>
       <c r="B68" s="17" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C68" s="18">
         <v>2</v>
@@ -3961,10 +3961,10 @@
         <v>67</v>
       </c>
     </row>
-    <row r="69" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A69" s="19"/>
       <c r="B69" s="17" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C69" s="18">
         <v>3</v>
@@ -3976,10 +3976,10 @@
         <v>68</v>
       </c>
     </row>
-    <row r="70" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A70" s="19"/>
       <c r="B70" s="17" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C70" s="18">
         <v>4</v>
@@ -3991,10 +3991,10 @@
         <v>69</v>
       </c>
     </row>
-    <row r="71" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A71" s="19"/>
       <c r="B71" s="17" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C71" s="18">
         <v>5</v>
@@ -4006,12 +4006,12 @@
         <v>70</v>
       </c>
     </row>
-    <row r="72" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A72" s="19" t="s">
+        <v>101</v>
+      </c>
+      <c r="B72" s="17" t="s">
         <v>102</v>
-      </c>
-      <c r="B72" s="17" t="s">
-        <v>103</v>
       </c>
       <c r="C72" s="18">
         <v>1</v>
@@ -4023,10 +4023,10 @@
         <v>71</v>
       </c>
     </row>
-    <row r="73" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A73" s="19"/>
       <c r="B73" s="17" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C73" s="18">
         <v>2</v>
@@ -4038,10 +4038,10 @@
         <v>72</v>
       </c>
     </row>
-    <row r="74" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A74" s="19"/>
       <c r="B74" s="17" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C74" s="18">
         <v>3</v>
@@ -4053,10 +4053,10 @@
         <v>73</v>
       </c>
     </row>
-    <row r="75" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A75" s="19"/>
       <c r="B75" s="17" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C75" s="18">
         <v>4</v>
@@ -4068,10 +4068,10 @@
         <v>74</v>
       </c>
     </row>
-    <row r="76" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A76" s="19"/>
       <c r="B76" s="17" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C76" s="18">
         <v>5</v>
@@ -4083,12 +4083,12 @@
         <v>75</v>
       </c>
     </row>
-    <row r="77" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A77" s="19" t="s">
+        <v>103</v>
+      </c>
+      <c r="B77" s="17" t="s">
         <v>104</v>
-      </c>
-      <c r="B77" s="17" t="s">
-        <v>105</v>
       </c>
       <c r="C77" s="18">
         <v>1</v>
@@ -4100,10 +4100,10 @@
         <v>76</v>
       </c>
     </row>
-    <row r="78" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A78" s="19"/>
       <c r="B78" s="17" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C78" s="18">
         <v>2</v>
@@ -4115,10 +4115,10 @@
         <v>77</v>
       </c>
     </row>
-    <row r="79" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A79" s="19"/>
       <c r="B79" s="17" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C79" s="18">
         <v>3</v>
@@ -4130,10 +4130,10 @@
         <v>78</v>
       </c>
     </row>
-    <row r="80" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A80" s="19"/>
       <c r="B80" s="17" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C80" s="18">
         <v>4</v>
@@ -4145,10 +4145,10 @@
         <v>79</v>
       </c>
     </row>
-    <row r="81" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A81" s="19"/>
       <c r="B81" s="17" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C81" s="18">
         <v>5</v>
@@ -4160,602 +4160,602 @@
         <v>80</v>
       </c>
     </row>
-    <row r="82" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A82" s="20"/>
       <c r="B82" s="21"/>
       <c r="C82" s="22"/>
     </row>
-    <row r="83" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A83" s="20"/>
       <c r="B83" s="21"/>
       <c r="C83" s="22"/>
     </row>
-    <row r="84" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A84" s="20"/>
       <c r="B84" s="21"/>
       <c r="C84" s="22"/>
     </row>
-    <row r="85" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A85" s="20"/>
       <c r="B85" s="21"/>
       <c r="C85" s="22"/>
     </row>
-    <row r="86" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A86" s="20"/>
       <c r="B86" s="21"/>
       <c r="C86" s="22"/>
     </row>
-    <row r="87" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A87" s="20"/>
       <c r="B87" s="21"/>
       <c r="C87" s="22"/>
     </row>
-    <row r="88" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A88" s="20"/>
       <c r="B88" s="21"/>
       <c r="C88" s="22"/>
     </row>
-    <row r="89" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A89" s="20"/>
       <c r="B89" s="21"/>
       <c r="C89" s="22"/>
     </row>
-    <row r="90" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A90" s="20"/>
       <c r="B90" s="21"/>
       <c r="C90" s="22"/>
     </row>
-    <row r="91" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A91" s="20"/>
       <c r="B91" s="21"/>
       <c r="C91" s="22"/>
     </row>
-    <row r="92" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A92" s="20"/>
       <c r="B92" s="21"/>
       <c r="C92" s="22"/>
     </row>
-    <row r="93" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A93" s="20"/>
       <c r="B93" s="21"/>
       <c r="C93" s="22"/>
     </row>
-    <row r="94" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A94" s="20"/>
       <c r="B94" s="21"/>
       <c r="C94" s="22"/>
     </row>
-    <row r="95" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A95" s="20"/>
       <c r="B95" s="21"/>
       <c r="C95" s="22"/>
     </row>
-    <row r="96" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A96" s="20"/>
       <c r="B96" s="21"/>
       <c r="C96" s="22"/>
     </row>
-    <row r="97" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A97" s="20"/>
       <c r="B97" s="21"/>
       <c r="C97" s="22"/>
     </row>
-    <row r="98" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A98" s="20"/>
       <c r="B98" s="21"/>
       <c r="C98" s="22"/>
     </row>
-    <row r="99" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A99" s="20"/>
       <c r="B99" s="21"/>
       <c r="C99" s="22"/>
     </row>
-    <row r="100" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A100" s="20"/>
       <c r="B100" s="21"/>
       <c r="C100" s="22"/>
     </row>
-    <row r="101" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A101" s="20"/>
       <c r="B101" s="21"/>
       <c r="C101" s="22"/>
     </row>
-    <row r="102" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A102" s="20"/>
       <c r="B102" s="21"/>
       <c r="C102" s="22"/>
     </row>
-    <row r="103" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A103" s="20"/>
       <c r="B103" s="21"/>
       <c r="C103" s="22"/>
     </row>
-    <row r="104" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A104" s="20"/>
       <c r="B104" s="21"/>
       <c r="C104" s="22"/>
     </row>
-    <row r="105" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A105" s="20"/>
       <c r="B105" s="21"/>
       <c r="C105" s="22"/>
     </row>
-    <row r="106" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A106" s="20"/>
       <c r="B106" s="21"/>
       <c r="C106" s="22"/>
     </row>
-    <row r="107" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A107" s="20"/>
       <c r="B107" s="21"/>
       <c r="C107" s="22"/>
     </row>
-    <row r="108" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A108" s="20"/>
       <c r="B108" s="21"/>
       <c r="C108" s="22"/>
     </row>
-    <row r="109" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A109" s="20"/>
       <c r="B109" s="21"/>
       <c r="C109" s="22"/>
     </row>
-    <row r="110" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A110" s="20"/>
       <c r="B110" s="21"/>
       <c r="C110" s="22"/>
     </row>
-    <row r="111" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A111" s="20"/>
       <c r="B111" s="21"/>
       <c r="C111" s="22"/>
     </row>
-    <row r="112" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A112" s="20"/>
       <c r="B112" s="21"/>
       <c r="C112" s="22"/>
     </row>
-    <row r="113" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A113" s="20"/>
       <c r="B113" s="21"/>
       <c r="C113" s="22"/>
     </row>
-    <row r="114" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A114" s="20"/>
       <c r="B114" s="21"/>
       <c r="C114" s="22"/>
     </row>
-    <row r="115" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A115" s="20"/>
       <c r="B115" s="21"/>
       <c r="C115" s="22"/>
     </row>
-    <row r="116" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A116" s="20"/>
       <c r="B116" s="21"/>
       <c r="C116" s="22"/>
     </row>
-    <row r="117" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A117" s="20"/>
       <c r="B117" s="21"/>
       <c r="C117" s="22"/>
     </row>
-    <row r="118" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A118" s="20"/>
       <c r="B118" s="21"/>
       <c r="C118" s="22"/>
     </row>
-    <row r="119" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A119" s="20"/>
       <c r="B119" s="21"/>
       <c r="C119" s="22"/>
     </row>
-    <row r="120" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A120" s="20"/>
       <c r="B120" s="21"/>
       <c r="C120" s="22"/>
     </row>
-    <row r="121" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A121" s="20"/>
       <c r="B121" s="21"/>
       <c r="C121" s="22"/>
     </row>
-    <row r="122" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A122" s="20"/>
       <c r="B122" s="21"/>
       <c r="C122" s="22"/>
     </row>
-    <row r="123" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A123" s="20"/>
       <c r="B123" s="21"/>
       <c r="C123" s="22"/>
     </row>
-    <row r="124" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A124" s="20"/>
       <c r="B124" s="21"/>
       <c r="C124" s="22"/>
     </row>
-    <row r="125" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A125" s="20"/>
       <c r="B125" s="21"/>
       <c r="C125" s="22"/>
     </row>
-    <row r="126" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="126" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A126" s="20"/>
       <c r="B126" s="21"/>
       <c r="C126" s="22"/>
     </row>
-    <row r="127" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="127" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A127" s="20"/>
       <c r="B127" s="21"/>
       <c r="C127" s="22"/>
     </row>
-    <row r="128" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="128" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A128" s="20"/>
       <c r="B128" s="21"/>
       <c r="C128" s="22"/>
     </row>
-    <row r="129" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="129" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A129" s="20"/>
       <c r="B129" s="21"/>
       <c r="C129" s="22"/>
     </row>
-    <row r="130" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="130" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A130" s="20"/>
       <c r="B130" s="21"/>
       <c r="C130" s="22"/>
     </row>
-    <row r="131" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="131" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A131" s="20"/>
       <c r="B131" s="21"/>
       <c r="C131" s="22"/>
     </row>
-    <row r="132" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="132" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A132" s="20"/>
       <c r="B132" s="21"/>
       <c r="C132" s="22"/>
     </row>
-    <row r="133" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="133" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A133" s="20"/>
       <c r="B133" s="21"/>
       <c r="C133" s="22"/>
     </row>
-    <row r="134" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="134" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A134" s="20"/>
       <c r="B134" s="21"/>
       <c r="C134" s="22"/>
     </row>
-    <row r="135" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="135" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A135" s="20"/>
       <c r="B135" s="21"/>
       <c r="C135" s="22"/>
     </row>
-    <row r="136" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="136" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A136" s="20"/>
       <c r="B136" s="21"/>
       <c r="C136" s="22"/>
     </row>
-    <row r="137" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="137" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A137" s="20"/>
       <c r="B137" s="21"/>
       <c r="C137" s="22"/>
     </row>
-    <row r="138" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="138" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A138" s="20"/>
       <c r="B138" s="21"/>
       <c r="C138" s="22"/>
     </row>
-    <row r="139" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="139" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A139" s="20"/>
       <c r="B139" s="21"/>
       <c r="C139" s="22"/>
     </row>
-    <row r="140" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="140" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A140" s="20"/>
       <c r="B140" s="21"/>
       <c r="C140" s="22"/>
     </row>
-    <row r="141" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="141" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A141" s="20"/>
       <c r="B141" s="21"/>
       <c r="C141" s="22"/>
     </row>
-    <row r="142" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="142" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A142" s="20"/>
       <c r="B142" s="21"/>
       <c r="C142" s="22"/>
     </row>
-    <row r="143" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="143" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A143" s="20"/>
       <c r="B143" s="21"/>
       <c r="C143" s="22"/>
     </row>
-    <row r="144" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="144" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A144" s="20"/>
       <c r="B144" s="21"/>
       <c r="C144" s="22"/>
     </row>
-    <row r="145" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="145" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A145" s="20"/>
       <c r="B145" s="21"/>
       <c r="C145" s="22"/>
     </row>
-    <row r="146" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="146" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A146" s="20"/>
       <c r="B146" s="21"/>
       <c r="C146" s="22"/>
     </row>
-    <row r="147" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="147" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A147" s="20"/>
       <c r="B147" s="21"/>
       <c r="C147" s="22"/>
     </row>
-    <row r="148" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="148" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A148" s="20"/>
       <c r="B148" s="21"/>
       <c r="C148" s="22"/>
     </row>
-    <row r="149" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="149" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A149" s="20"/>
       <c r="B149" s="21"/>
       <c r="C149" s="22"/>
     </row>
-    <row r="150" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="150" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A150" s="20"/>
       <c r="B150" s="21"/>
       <c r="C150" s="22"/>
     </row>
-    <row r="151" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="151" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A151" s="20"/>
       <c r="B151" s="21"/>
       <c r="C151" s="22"/>
     </row>
-    <row r="152" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="152" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A152" s="20"/>
       <c r="B152" s="21"/>
       <c r="C152" s="22"/>
     </row>
-    <row r="153" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="153" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A153" s="20"/>
       <c r="B153" s="21"/>
       <c r="C153" s="22"/>
     </row>
-    <row r="154" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="154" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A154" s="20"/>
       <c r="B154" s="21"/>
       <c r="C154" s="22"/>
     </row>
-    <row r="155" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="155" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A155" s="20"/>
       <c r="B155" s="21"/>
       <c r="C155" s="22"/>
     </row>
-    <row r="156" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="156" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A156" s="20"/>
       <c r="B156" s="21"/>
       <c r="C156" s="22"/>
     </row>
-    <row r="157" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="157" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A157" s="20"/>
       <c r="B157" s="21"/>
       <c r="C157" s="22"/>
     </row>
-    <row r="158" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="158" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A158" s="20"/>
       <c r="B158" s="21"/>
       <c r="C158" s="22"/>
     </row>
-    <row r="159" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="159" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A159" s="20"/>
       <c r="B159" s="21"/>
       <c r="C159" s="22"/>
     </row>
-    <row r="160" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="160" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A160" s="20"/>
       <c r="B160" s="21"/>
       <c r="C160" s="22"/>
     </row>
-    <row r="161" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="161" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A161" s="20"/>
       <c r="B161" s="21"/>
       <c r="C161" s="22"/>
     </row>
-    <row r="162" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="162" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A162" s="20"/>
       <c r="B162" s="21"/>
       <c r="C162" s="22"/>
     </row>
-    <row r="163" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="163" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A163" s="20"/>
       <c r="B163" s="21"/>
       <c r="C163" s="22"/>
     </row>
-    <row r="164" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="164" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A164" s="20"/>
       <c r="B164" s="21"/>
       <c r="C164" s="22"/>
     </row>
-    <row r="165" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="165" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A165" s="20"/>
       <c r="B165" s="21"/>
       <c r="C165" s="22"/>
     </row>
-    <row r="166" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="166" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A166" s="20"/>
       <c r="B166" s="21"/>
       <c r="C166" s="22"/>
     </row>
-    <row r="167" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="167" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A167" s="20"/>
       <c r="B167" s="21"/>
       <c r="C167" s="22"/>
     </row>
-    <row r="168" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="168" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A168" s="20"/>
       <c r="B168" s="21"/>
       <c r="C168" s="22"/>
     </row>
-    <row r="169" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="169" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A169" s="20"/>
       <c r="B169" s="21"/>
       <c r="C169" s="22"/>
     </row>
-    <row r="170" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="170" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A170" s="20"/>
       <c r="B170" s="21"/>
       <c r="C170" s="22"/>
     </row>
-    <row r="171" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="171" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A171" s="20"/>
       <c r="B171" s="21"/>
       <c r="C171" s="22"/>
     </row>
-    <row r="172" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="172" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A172" s="20"/>
       <c r="B172" s="21"/>
       <c r="C172" s="22"/>
     </row>
-    <row r="173" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="173" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A173" s="20"/>
       <c r="B173" s="21"/>
       <c r="C173" s="22"/>
     </row>
-    <row r="174" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="174" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A174" s="20"/>
       <c r="B174" s="21"/>
       <c r="C174" s="22"/>
     </row>
-    <row r="175" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="175" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A175" s="20"/>
       <c r="B175" s="21"/>
       <c r="C175" s="22"/>
     </row>
-    <row r="176" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="176" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A176" s="20"/>
       <c r="B176" s="21"/>
       <c r="C176" s="22"/>
     </row>
-    <row r="177" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="177" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A177" s="20"/>
       <c r="B177" s="21"/>
       <c r="C177" s="22"/>
     </row>
-    <row r="178" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="178" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A178" s="20"/>
       <c r="B178" s="21"/>
       <c r="C178" s="22"/>
     </row>
-    <row r="179" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="179" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A179" s="20"/>
       <c r="B179" s="21"/>
       <c r="C179" s="22"/>
     </row>
-    <row r="180" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="180" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A180" s="20"/>
       <c r="B180" s="21"/>
       <c r="C180" s="22"/>
     </row>
-    <row r="181" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="181" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A181" s="20"/>
       <c r="B181" s="21"/>
       <c r="C181" s="22"/>
     </row>
-    <row r="182" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="182" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A182" s="20"/>
       <c r="B182" s="21"/>
       <c r="C182" s="22"/>
     </row>
-    <row r="183" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="183" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A183" s="20"/>
       <c r="B183" s="21"/>
       <c r="C183" s="22"/>
     </row>
-    <row r="184" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="184" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A184" s="20"/>
       <c r="B184" s="21"/>
       <c r="C184" s="22"/>
     </row>
-    <row r="185" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="185" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A185" s="20"/>
       <c r="B185" s="21"/>
       <c r="C185" s="22"/>
     </row>
-    <row r="186" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="186" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A186" s="20"/>
       <c r="B186" s="21"/>
       <c r="C186" s="22"/>
     </row>
-    <row r="187" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="187" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A187" s="20"/>
       <c r="B187" s="21"/>
       <c r="C187" s="22"/>
     </row>
-    <row r="188" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="188" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A188" s="20"/>
       <c r="B188" s="21"/>
       <c r="C188" s="22"/>
     </row>
-    <row r="189" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="189" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A189" s="20"/>
       <c r="B189" s="21"/>
       <c r="C189" s="22"/>
     </row>
-    <row r="190" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="190" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A190" s="20"/>
       <c r="B190" s="21"/>
       <c r="C190" s="22"/>
     </row>
-    <row r="191" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="191" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A191" s="20"/>
       <c r="B191" s="21"/>
       <c r="C191" s="22"/>
     </row>
-    <row r="192" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="192" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A192" s="20"/>
       <c r="B192" s="21"/>
       <c r="C192" s="22"/>
     </row>
-    <row r="193" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="193" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A193" s="20"/>
       <c r="B193" s="21"/>
       <c r="C193" s="22"/>
     </row>
-    <row r="194" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="194" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A194" s="20"/>
       <c r="B194" s="21"/>
       <c r="C194" s="22"/>
     </row>
-    <row r="195" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="195" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A195" s="20"/>
       <c r="B195" s="21"/>
       <c r="C195" s="22"/>
     </row>
-    <row r="196" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="196" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A196" s="20"/>
       <c r="B196" s="21"/>
       <c r="C196" s="22"/>
     </row>
-    <row r="197" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="197" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A197" s="20"/>
       <c r="B197" s="21"/>
       <c r="C197" s="22"/>
     </row>
-    <row r="198" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="198" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A198" s="20"/>
       <c r="B198" s="21"/>
       <c r="C198" s="22"/>
     </row>
-    <row r="199" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="199" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A199" s="20"/>
       <c r="B199" s="21"/>
       <c r="C199" s="22"/>
     </row>
-    <row r="200" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="200" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A200" s="20"/>
       <c r="B200" s="21"/>
       <c r="C200" s="22"/>
     </row>
-    <row r="201" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="201" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A201" s="20"/>
       <c r="B201" s="21"/>
       <c r="C201" s="22"/>

</xml_diff>

<commit_message>
Restructured code to species composition
</commit_message>
<xml_diff>
--- a/notebooks/GenVeg/GenVeg_Example_Simulation.xlsx
+++ b/notebooks/GenVeg/GenVeg_Example_Simulation.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Python\landlab\notebooks\GenVeg\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1DFEACA2-D51B-4883-8359-4E8017C2EB1C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36748BE5-7A68-4415-B0BC-E113603454ED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{4FA2BB3E-4334-4C54-90D8-DFF869504B66}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="304" uniqueCount="111">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="322" uniqueCount="120">
   <si>
     <t>Parameter</t>
   </si>
@@ -91,16 +91,10 @@
     <t>Duration</t>
   </si>
   <si>
-    <t>annual_perennial</t>
-  </si>
-  <si>
     <t>Photosynthesis type</t>
   </si>
   <si>
     <t>ptype</t>
-  </si>
-  <si>
-    <t>C3</t>
   </si>
   <si>
     <t>Photosythesis variables</t>
@@ -522,13 +516,46 @@
     <t>C4</t>
   </si>
   <si>
-    <t>wheat</t>
-  </si>
-  <si>
     <t>per file:///C:/Users/RDEL1CMC/Downloads/Charisma-a_simulation_model_of_the_dynamics_of_submerged_plants.PDF.pdf</t>
   </si>
   <si>
     <t>respiration_coefficient</t>
+  </si>
+  <si>
+    <t>Leaf retention</t>
+  </si>
+  <si>
+    <t>Growth form</t>
+  </si>
+  <si>
+    <t>Shape and orientation</t>
+  </si>
+  <si>
+    <t>shape</t>
+  </si>
+  <si>
+    <t>deciduous</t>
+  </si>
+  <si>
+    <t>single_stem</t>
+  </si>
+  <si>
+    <t>erect</t>
+  </si>
+  <si>
+    <t>bunch</t>
+  </si>
+  <si>
+    <t>duration</t>
+  </si>
+  <si>
+    <t>growth_habit</t>
+  </si>
+  <si>
+    <t>leaf_retention</t>
+  </si>
+  <si>
+    <t>Wheat</t>
   </si>
 </sst>
 </file>
@@ -1062,10 +1089,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{59430052-850A-4E52-8B29-0C7825B169C3}">
-  <dimension ref="A1:G201"/>
+  <dimension ref="A1:G204"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+      <selection activeCell="D24" sqref="D24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1093,9 +1120,6 @@
       <c r="E1" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="F1">
-        <v>0</v>
-      </c>
     </row>
     <row r="2" spans="1:6" ht="18.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="5" t="s">
@@ -1106,7 +1130,7 @@
       <c r="D2" s="8"/>
       <c r="E2" s="8"/>
       <c r="F2">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
@@ -1118,10 +1142,10 @@
       </c>
       <c r="C3" s="11"/>
       <c r="D3" s="12" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="F3">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
@@ -1129,14 +1153,14 @@
         <v>8</v>
       </c>
       <c r="B4" s="10" t="s">
-        <v>9</v>
+        <v>117</v>
       </c>
       <c r="C4" s="11"/>
       <c r="D4" s="12" t="s">
         <v>10</v>
       </c>
       <c r="F4">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
@@ -1151,7 +1175,7 @@
         <v>13</v>
       </c>
       <c r="F5">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
@@ -1166,7 +1190,7 @@
         <v>16</v>
       </c>
       <c r="F6">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
@@ -1174,1135 +1198,1165 @@
         <v>17</v>
       </c>
       <c r="B7" s="10" t="s">
-        <v>18</v>
+        <v>116</v>
       </c>
       <c r="C7" s="11"/>
       <c r="D7" s="12" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="F7">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="9" t="s">
-        <v>19</v>
+        <v>108</v>
       </c>
       <c r="B8" s="10" t="s">
-        <v>20</v>
+        <v>118</v>
       </c>
       <c r="C8" s="11"/>
       <c r="D8" s="12" t="s">
-        <v>107</v>
+        <v>112</v>
       </c>
       <c r="F8">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" s="9" t="s">
+        <v>109</v>
+      </c>
+      <c r="B9" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="C9" s="11"/>
+      <c r="D9" s="12" t="s">
+        <v>113</v>
+      </c>
+      <c r="F9">
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="18" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="B9" s="6"/>
-      <c r="C9" s="7"/>
-      <c r="D9" s="14"/>
-      <c r="E9" s="8"/>
-      <c r="F9">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" s="9" t="s">
+        <v>110</v>
+      </c>
+      <c r="B10" s="10" t="s">
+        <v>111</v>
+      </c>
+      <c r="C10" s="11"/>
+      <c r="D10" s="12" t="s">
+        <v>114</v>
+      </c>
+      <c r="F10">
         <v>8</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="B10" s="10" t="s">
-        <v>24</v>
-      </c>
-      <c r="C10" s="11"/>
-      <c r="D10" s="15">
-        <v>121</v>
-      </c>
-      <c r="F10">
-        <v>9</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="B11" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="C11" s="11"/>
+      <c r="D11" s="12" t="s">
+        <v>105</v>
+      </c>
+      <c r="F11">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" ht="18" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A12" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="B12" s="6"/>
+      <c r="C12" s="7"/>
+      <c r="D12" s="14"/>
+      <c r="E12" s="8"/>
+      <c r="F12">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="B13" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="C13" s="11"/>
+      <c r="D13" s="15">
+        <v>121</v>
+      </c>
+      <c r="F13">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="B14" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="C14" s="11"/>
+      <c r="D14" s="15">
+        <v>243</v>
+      </c>
+      <c r="F14">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="B11" s="10" t="s">
+      <c r="B15" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="C11" s="11"/>
-      <c r="D11" s="15">
-        <v>243</v>
-      </c>
-      <c r="F11">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12" s="9" t="s">
-        <v>27</v>
-      </c>
-      <c r="B12" s="10" t="s">
-        <v>28</v>
-      </c>
-      <c r="C12" s="11"/>
-      <c r="D12" s="15">
+      <c r="C15" s="11"/>
+      <c r="D15" s="15">
         <v>228</v>
       </c>
-      <c r="F12">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A13" s="25" t="s">
-        <v>29</v>
-      </c>
-      <c r="B13" s="10" t="s">
-        <v>110</v>
-      </c>
-      <c r="C13" s="11" t="s">
-        <v>30</v>
-      </c>
-      <c r="D13" s="15">
-        <v>1.4999999999999999E-2</v>
-      </c>
-      <c r="F13">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A14" s="25"/>
-      <c r="B14" s="10" t="s">
-        <v>110</v>
-      </c>
-      <c r="C14" s="11" t="s">
-        <v>31</v>
-      </c>
-      <c r="D14" s="15">
-        <v>1.4999999999999999E-2</v>
-      </c>
-      <c r="F14">
+      <c r="F15">
         <v>13</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A15" s="25"/>
-      <c r="B15" s="10" t="s">
-        <v>110</v>
-      </c>
-      <c r="C15" s="11" t="s">
-        <v>32</v>
-      </c>
-      <c r="D15" s="15">
-        <v>0.03</v>
-      </c>
-      <c r="F15">
-        <v>14</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="25" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="B16" s="10" t="s">
-        <v>34</v>
+        <v>107</v>
       </c>
       <c r="C16" s="11" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="D16" s="15">
-        <v>1.444</v>
+        <v>1.4999999999999999E-2</v>
       </c>
       <c r="F16">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="25"/>
       <c r="B17" s="10" t="s">
-        <v>34</v>
+        <v>107</v>
       </c>
       <c r="C17" s="11" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="D17" s="15">
-        <v>1.5129999999999999</v>
+        <v>1.4999999999999999E-2</v>
       </c>
       <c r="F17">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" s="25"/>
       <c r="B18" s="10" t="s">
+        <v>107</v>
+      </c>
+      <c r="C18" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="D18" s="15">
+        <v>0.03</v>
+      </c>
+      <c r="F18">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A19" s="25" t="s">
+        <v>31</v>
+      </c>
+      <c r="B19" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="C19" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="D19" s="15">
+        <v>1.444</v>
+      </c>
+      <c r="F19">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A20" s="25"/>
+      <c r="B20" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="C20" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="D20" s="15">
+        <v>1.5129999999999999</v>
+      </c>
+      <c r="F20">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A21" s="25"/>
+      <c r="B21" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="C21" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="D21" s="15">
+        <v>1.4630000000000001</v>
+      </c>
+      <c r="F21">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A22" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="B22" s="10" t="s">
         <v>34</v>
       </c>
-      <c r="C18" s="11" t="s">
-        <v>32</v>
-      </c>
-      <c r="D18" s="15">
-        <v>1.4630000000000001</v>
-      </c>
-      <c r="F18">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A19" s="9" t="s">
+      <c r="C22" s="11"/>
+      <c r="D22" s="15">
+        <v>0.51</v>
+      </c>
+      <c r="F22">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" ht="32.25" x14ac:dyDescent="0.25">
+      <c r="A23" s="9" t="s">
         <v>35</v>
       </c>
-      <c r="B19" s="10" t="s">
+      <c r="B23" s="10" t="s">
         <v>36</v>
       </c>
-      <c r="C19" s="11"/>
-      <c r="D19" s="15">
-        <v>0.51</v>
-      </c>
-      <c r="F19">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" ht="32.25" x14ac:dyDescent="0.25">
-      <c r="A20" s="9" t="s">
+      <c r="C23" s="11"/>
+      <c r="D23" s="15">
+        <v>100</v>
+      </c>
+      <c r="E23" t="s">
+        <v>106</v>
+      </c>
+      <c r="F23">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A24" s="9" t="s">
         <v>37</v>
       </c>
-      <c r="B20" s="10" t="s">
+      <c r="B24" s="10" t="s">
         <v>38</v>
       </c>
-      <c r="C20" s="11"/>
-      <c r="D20" s="15">
-        <v>100</v>
-      </c>
-      <c r="E20" t="s">
-        <v>109</v>
-      </c>
-      <c r="F20">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A21" s="9" t="s">
+      <c r="C24" s="11"/>
+      <c r="D24" s="15">
+        <v>3.7199999999999997E-2</v>
+      </c>
+      <c r="F24">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A25" s="26" t="s">
         <v>39</v>
       </c>
-      <c r="B21" s="10" t="s">
+      <c r="B25" s="10" t="s">
         <v>40</v>
       </c>
-      <c r="C21" s="11"/>
-      <c r="D21" s="15">
-        <v>3.7199999999999997E-2</v>
-      </c>
-      <c r="F21">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A22" s="26" t="s">
+      <c r="C25" s="11" t="s">
         <v>41</v>
       </c>
-      <c r="B22" s="10" t="s">
+      <c r="D25" s="15"/>
+      <c r="E25" s="16" t="s">
         <v>42</v>
       </c>
-      <c r="C22" s="11" t="s">
+      <c r="F25">
+        <v>23</v>
+      </c>
+      <c r="G25" t="s">
         <v>43</v>
-      </c>
-      <c r="D22" s="15"/>
-      <c r="E22" s="16" t="s">
-        <v>44</v>
-      </c>
-      <c r="F22">
-        <v>21</v>
-      </c>
-      <c r="G22" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A23" s="26"/>
-      <c r="B23" s="10" t="s">
-        <v>42</v>
-      </c>
-      <c r="C23" s="11" t="s">
-        <v>46</v>
-      </c>
-      <c r="D23" s="15"/>
-      <c r="F23">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A24" s="26"/>
-      <c r="B24" s="10" t="s">
-        <v>42</v>
-      </c>
-      <c r="C24" s="11" t="s">
-        <v>47</v>
-      </c>
-      <c r="D24" s="15"/>
-      <c r="F24">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A25" s="26"/>
-      <c r="B25" s="10" t="s">
-        <v>48</v>
-      </c>
-      <c r="C25" s="11" t="s">
-        <v>43</v>
-      </c>
-      <c r="D25" s="15"/>
-      <c r="F25">
-        <v>24</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" s="26"/>
       <c r="B26" s="10" t="s">
-        <v>48</v>
+        <v>40</v>
       </c>
       <c r="C26" s="11" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="D26" s="15"/>
       <c r="F26">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" s="26"/>
       <c r="B27" s="10" t="s">
-        <v>48</v>
+        <v>40</v>
       </c>
       <c r="C27" s="11" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="D27" s="15"/>
       <c r="F27">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A28" s="26"/>
+      <c r="B28" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="C28" s="11" t="s">
+        <v>41</v>
+      </c>
+      <c r="D28" s="15"/>
+      <c r="F28">
         <v>26</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A28" s="27" t="s">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A29" s="26"/>
+      <c r="B29" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="C29" s="11" t="s">
+        <v>44</v>
+      </c>
+      <c r="D29" s="15"/>
+      <c r="F29">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A30" s="26"/>
+      <c r="B30" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="C30" s="11" t="s">
+        <v>45</v>
+      </c>
+      <c r="D30" s="15"/>
+      <c r="F30">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A31" s="27" t="s">
+        <v>47</v>
+      </c>
+      <c r="B31" s="17" t="s">
+        <v>48</v>
+      </c>
+      <c r="C31" s="18" t="s">
+        <v>28</v>
+      </c>
+      <c r="D31" s="15">
+        <v>0.01</v>
+      </c>
+      <c r="F31">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A32" s="27"/>
+      <c r="B32" s="17" t="s">
+        <v>48</v>
+      </c>
+      <c r="C32" s="18" t="s">
+        <v>29</v>
+      </c>
+      <c r="D32" s="15">
+        <v>0.1</v>
+      </c>
+      <c r="F32">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A33" s="27"/>
+      <c r="B33" s="17" t="s">
+        <v>48</v>
+      </c>
+      <c r="C33" s="18" t="s">
+        <v>30</v>
+      </c>
+      <c r="D33" s="15">
+        <v>0.5</v>
+      </c>
+      <c r="F33">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" ht="18" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A34" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="B28" s="17" t="s">
+      <c r="B34" s="6"/>
+      <c r="C34" s="7"/>
+      <c r="D34" s="6"/>
+      <c r="E34" s="8"/>
+      <c r="F34">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" ht="18" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A35" s="19" t="s">
         <v>50</v>
       </c>
-      <c r="C28" s="18" t="s">
-        <v>30</v>
-      </c>
-      <c r="D28" s="15">
-        <v>0.01</v>
-      </c>
-      <c r="F28">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A29" s="27"/>
-      <c r="B29" s="17" t="s">
-        <v>50</v>
-      </c>
-      <c r="C29" s="18" t="s">
-        <v>31</v>
-      </c>
-      <c r="D29" s="15">
-        <v>0.1</v>
-      </c>
-      <c r="F29">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A30" s="27"/>
-      <c r="B30" s="17" t="s">
-        <v>50</v>
-      </c>
-      <c r="C30" s="18" t="s">
-        <v>32</v>
-      </c>
-      <c r="D30" s="15">
-        <v>0.5</v>
-      </c>
-      <c r="F30">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="31" spans="1:7" ht="18" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A31" s="5" t="s">
+      <c r="B35" s="17" t="s">
         <v>51</v>
-      </c>
-      <c r="B31" s="6"/>
-      <c r="C31" s="7"/>
-      <c r="D31" s="6"/>
-      <c r="E31" s="8"/>
-      <c r="F31">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="32" spans="1:7" ht="18" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="19" t="s">
-        <v>52</v>
-      </c>
-      <c r="B32" s="17" t="s">
-        <v>53</v>
-      </c>
-      <c r="C32" s="18"/>
-      <c r="D32" s="15">
-        <v>34</v>
-      </c>
-      <c r="F32">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A33" s="19" t="s">
-        <v>54</v>
-      </c>
-      <c r="B33" s="17" t="s">
-        <v>55</v>
-      </c>
-      <c r="C33" s="18"/>
-      <c r="D33" s="15">
-        <v>3</v>
-      </c>
-      <c r="F33">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A34" s="19" t="s">
-        <v>56</v>
-      </c>
-      <c r="B34" s="17" t="s">
-        <v>57</v>
-      </c>
-      <c r="C34" s="18"/>
-      <c r="D34" s="15">
-        <v>1</v>
-      </c>
-      <c r="F34">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A35" s="19" t="s">
-        <v>58</v>
-      </c>
-      <c r="B35" s="17" t="s">
-        <v>59</v>
       </c>
       <c r="C35" s="18"/>
       <c r="D35" s="15">
-        <v>1.45</v>
+        <v>34</v>
       </c>
       <c r="F35">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="36" spans="1:6" ht="17.25" x14ac:dyDescent="0.25">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36" s="19" t="s">
-        <v>60</v>
+        <v>52</v>
       </c>
       <c r="B36" s="17" t="s">
-        <v>61</v>
+        <v>53</v>
       </c>
       <c r="C36" s="18"/>
       <c r="D36" s="15">
-        <v>0.23100000000000001</v>
+        <v>3</v>
       </c>
       <c r="F36">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A37" s="19" t="s">
+        <v>54</v>
+      </c>
+      <c r="B37" s="17" t="s">
+        <v>55</v>
+      </c>
+      <c r="C37" s="18"/>
+      <c r="D37" s="15">
+        <v>1</v>
+      </c>
+      <c r="F37">
         <v>35</v>
       </c>
     </row>
-    <row r="37" spans="1:6" ht="18" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A37" s="5" t="s">
-        <v>62</v>
-      </c>
-      <c r="B37" s="6"/>
-      <c r="C37" s="7"/>
-      <c r="D37" s="6"/>
-      <c r="E37" s="8"/>
-      <c r="F37">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="38" spans="1:6" ht="30.75" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38" s="19" t="s">
-        <v>63</v>
+        <v>56</v>
       </c>
       <c r="B38" s="17" t="s">
-        <v>64</v>
+        <v>57</v>
       </c>
       <c r="C38" s="18"/>
       <c r="D38" s="15">
-        <v>4</v>
+        <v>1.45</v>
       </c>
       <c r="F38">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="39" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" ht="17.25" x14ac:dyDescent="0.25">
       <c r="A39" s="19" t="s">
-        <v>65</v>
+        <v>58</v>
       </c>
       <c r="B39" s="17" t="s">
-        <v>66</v>
+        <v>59</v>
       </c>
       <c r="C39" s="18"/>
       <c r="D39" s="15">
-        <v>0.5</v>
+        <v>0.23100000000000001</v>
       </c>
       <c r="F39">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" ht="18" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A40" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="B40" s="6"/>
+      <c r="C40" s="7"/>
+      <c r="D40" s="6"/>
+      <c r="E40" s="8"/>
+      <c r="F40">
         <v>38</v>
       </c>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A40" s="19" t="s">
-        <v>67</v>
-      </c>
-      <c r="B40" s="17" t="s">
-        <v>68</v>
-      </c>
-      <c r="C40" s="18"/>
-      <c r="D40" s="15">
-        <v>0</v>
-      </c>
-      <c r="F40">
+    <row r="41" spans="1:6" ht="30.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A41" s="19" t="s">
+        <v>61</v>
+      </c>
+      <c r="B41" s="17" t="s">
+        <v>62</v>
+      </c>
+      <c r="C41" s="18"/>
+      <c r="D41" s="15">
+        <v>4</v>
+      </c>
+      <c r="F41">
         <v>39</v>
       </c>
     </row>
-    <row r="41" spans="1:6" ht="18" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A41" s="5" t="s">
-        <v>69</v>
-      </c>
-      <c r="B41" s="6"/>
-      <c r="C41" s="7"/>
-      <c r="D41" s="6"/>
-      <c r="E41" s="8"/>
-      <c r="F41">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="42" spans="1:6" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A42" s="19" t="s">
-        <v>70</v>
+        <v>63</v>
       </c>
       <c r="B42" s="17" t="s">
-        <v>71</v>
+        <v>64</v>
       </c>
       <c r="C42" s="18"/>
       <c r="D42" s="15">
-        <v>0.01</v>
+        <v>0.5</v>
       </c>
       <c r="F42">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="43" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A43" s="19" t="s">
-        <v>72</v>
+        <v>65</v>
       </c>
       <c r="B43" s="17" t="s">
-        <v>73</v>
+        <v>66</v>
       </c>
       <c r="C43" s="18"/>
       <c r="D43" s="15">
-        <v>365</v>
+        <v>0</v>
       </c>
       <c r="F43">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="44" spans="1:6" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A44" s="5" t="s">
-        <v>74</v>
+        <v>67</v>
       </c>
       <c r="B44" s="6"/>
       <c r="C44" s="7"/>
       <c r="D44" s="6"/>
       <c r="E44" s="8"/>
       <c r="F44">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="45" spans="1:6" ht="30.75" thickTop="1" x14ac:dyDescent="0.25">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A45" s="19" t="s">
-        <v>75</v>
+        <v>68</v>
       </c>
       <c r="B45" s="17" t="s">
-        <v>76</v>
+        <v>69</v>
       </c>
       <c r="C45" s="18"/>
       <c r="D45" s="15">
-        <v>0.25</v>
-      </c>
-      <c r="E45" t="s">
-        <v>77</v>
+        <v>0.01</v>
       </c>
       <c r="F45">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="46" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A46" s="19" t="s">
-        <v>78</v>
+        <v>70</v>
       </c>
       <c r="B46" s="17" t="s">
-        <v>79</v>
+        <v>71</v>
       </c>
       <c r="C46" s="18"/>
       <c r="D46" s="15">
-        <v>0.25</v>
+        <v>365</v>
       </c>
       <c r="F46">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="47" spans="1:6" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A47" s="5" t="s">
-        <v>80</v>
+        <v>72</v>
       </c>
       <c r="B47" s="6"/>
       <c r="C47" s="7"/>
       <c r="D47" s="6"/>
-      <c r="E47" s="8" t="s">
-        <v>81</v>
-      </c>
+      <c r="E47" s="8"/>
       <c r="F47">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" ht="30.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A48" s="19" t="s">
+        <v>73</v>
+      </c>
+      <c r="B48" s="17" t="s">
+        <v>74</v>
+      </c>
+      <c r="C48" s="18"/>
+      <c r="D48" s="15">
+        <v>0.25</v>
+      </c>
+      <c r="E48" t="s">
+        <v>75</v>
+      </c>
+      <c r="F48">
         <v>46</v>
       </c>
     </row>
-    <row r="48" spans="1:6" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="19" t="s">
-        <v>82</v>
-      </c>
-      <c r="B48" s="17" t="s">
-        <v>83</v>
-      </c>
-      <c r="C48" s="18"/>
-      <c r="D48" s="12" t="s">
-        <v>84</v>
-      </c>
-      <c r="E48" t="s">
-        <v>85</v>
-      </c>
-      <c r="F48">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A49" s="19" t="s">
-        <v>86</v>
+        <v>76</v>
       </c>
       <c r="B49" s="17" t="s">
-        <v>87</v>
+        <v>77</v>
       </c>
       <c r="C49" s="18"/>
       <c r="D49" s="15">
+        <v>0.25</v>
+      </c>
+      <c r="F49">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" ht="18" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A50" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="B50" s="6"/>
+      <c r="C50" s="7"/>
+      <c r="D50" s="6"/>
+      <c r="E50" s="8" t="s">
+        <v>79</v>
+      </c>
+      <c r="F50">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A51" s="19" t="s">
+        <v>80</v>
+      </c>
+      <c r="B51" s="17" t="s">
+        <v>81</v>
+      </c>
+      <c r="C51" s="18"/>
+      <c r="D51" s="12" t="s">
+        <v>82</v>
+      </c>
+      <c r="E51" t="s">
+        <v>83</v>
+      </c>
+      <c r="F51">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A52" s="19" t="s">
+        <v>84</v>
+      </c>
+      <c r="B52" s="17" t="s">
+        <v>85</v>
+      </c>
+      <c r="C52" s="18"/>
+      <c r="D52" s="15">
         <v>207</v>
       </c>
-      <c r="F49">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A50" s="19" t="s">
-        <v>88</v>
-      </c>
-      <c r="B50" s="17" t="s">
-        <v>89</v>
-      </c>
-      <c r="C50" s="18">
+      <c r="F52">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A53" s="19" t="s">
+        <v>86</v>
+      </c>
+      <c r="B53" s="17" t="s">
+        <v>87</v>
+      </c>
+      <c r="C53" s="18">
         <v>1</v>
       </c>
-      <c r="D50" s="15">
+      <c r="D53" s="15">
         <v>30</v>
       </c>
-      <c r="F50">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A51" s="19"/>
-      <c r="B51" s="17" t="s">
-        <v>89</v>
-      </c>
-      <c r="C51" s="18">
-        <v>2</v>
-      </c>
-      <c r="D51" s="15">
-        <v>40</v>
-      </c>
-      <c r="F51">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A52" s="19"/>
-      <c r="B52" s="17" t="s">
-        <v>89</v>
-      </c>
-      <c r="C52" s="18">
-        <v>3</v>
-      </c>
-      <c r="D52" s="15">
-        <v>50</v>
-      </c>
-      <c r="F52">
+      <c r="F53">
         <v>51</v>
-      </c>
-    </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A53" s="19"/>
-      <c r="B53" s="17" t="s">
-        <v>89</v>
-      </c>
-      <c r="C53" s="18">
-        <v>4</v>
-      </c>
-      <c r="D53" s="15"/>
-      <c r="F53">
-        <v>52</v>
       </c>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A54" s="19"/>
       <c r="B54" s="17" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="C54" s="18">
-        <v>5</v>
-      </c>
-      <c r="D54" s="15"/>
+        <v>2</v>
+      </c>
+      <c r="D54" s="15">
+        <v>40</v>
+      </c>
       <c r="F54">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A55" s="19"/>
+      <c r="B55" s="17" t="s">
+        <v>87</v>
+      </c>
+      <c r="C55" s="18">
+        <v>3</v>
+      </c>
+      <c r="D55" s="15">
+        <v>50</v>
+      </c>
+      <c r="F55">
         <v>53</v>
-      </c>
-    </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A55" s="19" t="s">
-        <v>90</v>
-      </c>
-      <c r="B55" s="17" t="s">
-        <v>91</v>
-      </c>
-      <c r="C55" s="18">
-        <v>1</v>
-      </c>
-      <c r="D55" s="15">
-        <v>0.01</v>
-      </c>
-      <c r="F55">
-        <v>54</v>
       </c>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A56" s="19"/>
       <c r="B56" s="17" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="C56" s="18">
-        <v>2</v>
-      </c>
-      <c r="D56" s="15">
-        <v>0.25</v>
-      </c>
+        <v>4</v>
+      </c>
+      <c r="D56" s="15"/>
       <c r="F56">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A57" s="19"/>
       <c r="B57" s="17" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="C57" s="18">
-        <v>3</v>
-      </c>
-      <c r="D57" s="15">
-        <v>0.67</v>
-      </c>
+        <v>5</v>
+      </c>
+      <c r="D57" s="15"/>
       <c r="F57">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A58" s="19" t="s">
+        <v>88</v>
+      </c>
+      <c r="B58" s="17" t="s">
+        <v>89</v>
+      </c>
+      <c r="C58" s="18">
+        <v>1</v>
+      </c>
+      <c r="D58" s="15">
+        <v>0.01</v>
+      </c>
+      <c r="F58">
         <v>56</v>
-      </c>
-    </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A58" s="19"/>
-      <c r="B58" s="17" t="s">
-        <v>91</v>
-      </c>
-      <c r="C58" s="18">
-        <v>4</v>
-      </c>
-      <c r="D58" s="15"/>
-      <c r="F58">
-        <v>57</v>
       </c>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A59" s="19"/>
       <c r="B59" s="17" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="C59" s="18">
-        <v>5</v>
-      </c>
-      <c r="D59" s="15"/>
+        <v>2</v>
+      </c>
+      <c r="D59" s="15">
+        <v>0.25</v>
+      </c>
       <c r="F59">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A60" s="19"/>
+      <c r="B60" s="17" t="s">
+        <v>89</v>
+      </c>
+      <c r="C60" s="18">
+        <v>3</v>
+      </c>
+      <c r="D60" s="15">
+        <v>0.67</v>
+      </c>
+      <c r="F60">
         <v>58</v>
-      </c>
-    </row>
-    <row r="60" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A60" s="19" t="s">
-        <v>92</v>
-      </c>
-      <c r="B60" s="17" t="s">
-        <v>93</v>
-      </c>
-      <c r="C60" s="18">
-        <v>1</v>
-      </c>
-      <c r="D60" s="15">
-        <v>1</v>
-      </c>
-      <c r="F60">
-        <v>59</v>
       </c>
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A61" s="19"/>
       <c r="B61" s="17" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="C61" s="18">
-        <v>2</v>
-      </c>
-      <c r="D61" s="15">
-        <v>1</v>
-      </c>
+        <v>4</v>
+      </c>
+      <c r="D61" s="15"/>
       <c r="F61">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A62" s="19"/>
       <c r="B62" s="17" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="C62" s="18">
-        <v>3</v>
-      </c>
-      <c r="D62" s="15">
+        <v>5</v>
+      </c>
+      <c r="D62" s="15"/>
+      <c r="F62">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A63" s="19" t="s">
+        <v>90</v>
+      </c>
+      <c r="B63" s="17" t="s">
+        <v>91</v>
+      </c>
+      <c r="C63" s="18">
         <v>1</v>
       </c>
-      <c r="F62">
+      <c r="D63" s="15">
+        <v>1</v>
+      </c>
+      <c r="F63">
         <v>61</v>
-      </c>
-    </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A63" s="19"/>
-      <c r="B63" s="17" t="s">
-        <v>93</v>
-      </c>
-      <c r="C63" s="18">
-        <v>4</v>
-      </c>
-      <c r="D63" s="15"/>
-      <c r="F63">
-        <v>62</v>
       </c>
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A64" s="19"/>
       <c r="B64" s="17" t="s">
+        <v>91</v>
+      </c>
+      <c r="C64" s="18">
+        <v>2</v>
+      </c>
+      <c r="D64" s="15">
+        <v>1</v>
+      </c>
+      <c r="F64">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A65" s="19"/>
+      <c r="B65" s="17" t="s">
+        <v>91</v>
+      </c>
+      <c r="C65" s="18">
+        <v>3</v>
+      </c>
+      <c r="D65" s="15">
+        <v>1</v>
+      </c>
+      <c r="F65">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="66" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A66" s="19"/>
+      <c r="B66" s="17" t="s">
+        <v>91</v>
+      </c>
+      <c r="C66" s="18">
+        <v>4</v>
+      </c>
+      <c r="D66" s="15"/>
+      <c r="F66">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="67" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A67" s="19"/>
+      <c r="B67" s="17" t="s">
+        <v>91</v>
+      </c>
+      <c r="C67" s="18">
+        <v>5</v>
+      </c>
+      <c r="D67" s="15"/>
+      <c r="F67">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="68" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A68" s="19" t="s">
+        <v>92</v>
+      </c>
+      <c r="B68" s="17" t="s">
         <v>93</v>
       </c>
-      <c r="C64" s="18">
-        <v>5</v>
-      </c>
-      <c r="D64" s="15"/>
-      <c r="F64">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A65" s="19" t="s">
+      <c r="C68" s="18"/>
+      <c r="D68" s="12" t="s">
         <v>94</v>
       </c>
-      <c r="B65" s="17" t="s">
+      <c r="F68">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="69" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A69" s="19" t="s">
         <v>95</v>
       </c>
-      <c r="C65" s="18"/>
-      <c r="D65" s="12" t="s">
+      <c r="B69" s="17" t="s">
         <v>96</v>
       </c>
-      <c r="F65">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="66" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A66" s="19" t="s">
+      <c r="C69" s="18"/>
+      <c r="D69" s="15">
+        <v>365</v>
+      </c>
+      <c r="F69">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="70" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A70" s="19" t="s">
         <v>97</v>
       </c>
-      <c r="B66" s="17" t="s">
+      <c r="B70" s="17" t="s">
         <v>98</v>
       </c>
-      <c r="C66" s="18"/>
-      <c r="D66" s="15">
-        <v>365</v>
-      </c>
-      <c r="F66">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="67" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A67" s="19" t="s">
-        <v>99</v>
-      </c>
-      <c r="B67" s="17" t="s">
-        <v>100</v>
-      </c>
-      <c r="C67" s="18">
+      <c r="C70" s="18">
         <v>1</v>
       </c>
-      <c r="D67" s="15">
+      <c r="D70" s="15">
         <v>0</v>
       </c>
-      <c r="F67">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="68" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A68" s="19"/>
-      <c r="B68" s="17" t="s">
-        <v>100</v>
-      </c>
-      <c r="C68" s="18">
-        <v>2</v>
-      </c>
-      <c r="D68" s="15">
-        <v>0.2</v>
-      </c>
-      <c r="F68">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="69" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A69" s="19"/>
-      <c r="B69" s="17" t="s">
-        <v>100</v>
-      </c>
-      <c r="C69" s="18">
-        <v>3</v>
-      </c>
-      <c r="D69" s="15">
-        <v>0.5</v>
-      </c>
-      <c r="F69">
+      <c r="F70">
         <v>68</v>
-      </c>
-    </row>
-    <row r="70" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A70" s="19"/>
-      <c r="B70" s="17" t="s">
-        <v>100</v>
-      </c>
-      <c r="C70" s="18">
-        <v>4</v>
-      </c>
-      <c r="D70" s="15">
-        <v>0.68</v>
-      </c>
-      <c r="F70">
-        <v>69</v>
       </c>
     </row>
     <row r="71" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A71" s="19"/>
       <c r="B71" s="17" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="C71" s="18">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="D71" s="15">
-        <v>1.1200000000000001</v>
+        <v>0.2</v>
       </c>
       <c r="F71">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="72" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A72" s="19"/>
+      <c r="B72" s="17" t="s">
+        <v>98</v>
+      </c>
+      <c r="C72" s="18">
+        <v>3</v>
+      </c>
+      <c r="D72" s="15">
+        <v>0.5</v>
+      </c>
+      <c r="F72">
         <v>70</v>
-      </c>
-    </row>
-    <row r="72" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A72" s="19" t="s">
-        <v>101</v>
-      </c>
-      <c r="B72" s="17" t="s">
-        <v>102</v>
-      </c>
-      <c r="C72" s="18">
-        <v>1</v>
-      </c>
-      <c r="D72" s="15">
-        <v>0</v>
-      </c>
-      <c r="F72">
-        <v>71</v>
       </c>
     </row>
     <row r="73" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A73" s="19"/>
       <c r="B73" s="17" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="C73" s="18">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="D73" s="15">
-        <v>0</v>
+        <v>0.68</v>
       </c>
       <c r="F73">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="74" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A74" s="19"/>
       <c r="B74" s="17" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="C74" s="18">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="D74" s="15">
+        <v>1.1200000000000001</v>
+      </c>
+      <c r="F74">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="75" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A75" s="19" t="s">
+        <v>99</v>
+      </c>
+      <c r="B75" s="17" t="s">
+        <v>100</v>
+      </c>
+      <c r="C75" s="18">
+        <v>1</v>
+      </c>
+      <c r="D75" s="15">
         <v>0</v>
       </c>
-      <c r="F74">
+      <c r="F75">
         <v>73</v>
-      </c>
-    </row>
-    <row r="75" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A75" s="19"/>
-      <c r="B75" s="17" t="s">
-        <v>102</v>
-      </c>
-      <c r="C75" s="18">
-        <v>4</v>
-      </c>
-      <c r="D75" s="15">
-        <v>1</v>
-      </c>
-      <c r="F75">
-        <v>74</v>
       </c>
     </row>
     <row r="76" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A76" s="19"/>
       <c r="B76" s="17" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="C76" s="18">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="D76" s="15">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F76">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="77" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A77" s="19"/>
+      <c r="B77" s="17" t="s">
+        <v>100</v>
+      </c>
+      <c r="C77" s="18">
+        <v>3</v>
+      </c>
+      <c r="D77" s="15">
+        <v>0</v>
+      </c>
+      <c r="F77">
         <v>75</v>
-      </c>
-    </row>
-    <row r="77" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A77" s="19" t="s">
-        <v>103</v>
-      </c>
-      <c r="B77" s="17" t="s">
-        <v>104</v>
-      </c>
-      <c r="C77" s="18">
-        <v>1</v>
-      </c>
-      <c r="D77" s="15">
-        <v>500</v>
-      </c>
-      <c r="F77">
-        <v>76</v>
       </c>
     </row>
     <row r="78" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A78" s="19"/>
       <c r="B78" s="17" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="C78" s="18">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="D78" s="15">
-        <v>300</v>
+        <v>1</v>
       </c>
       <c r="F78">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="79" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A79" s="19"/>
       <c r="B79" s="17" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="C79" s="18">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="D79" s="15">
-        <v>200</v>
+        <v>1</v>
       </c>
       <c r="F79">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="80" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A80" s="19" t="s">
+        <v>101</v>
+      </c>
+      <c r="B80" s="17" t="s">
+        <v>102</v>
+      </c>
+      <c r="C80" s="18">
+        <v>1</v>
+      </c>
+      <c r="D80" s="15">
+        <v>500</v>
+      </c>
+      <c r="F80">
         <v>78</v>
-      </c>
-    </row>
-    <row r="80" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A80" s="19"/>
-      <c r="B80" s="17" t="s">
-        <v>104</v>
-      </c>
-      <c r="C80" s="18">
-        <v>4</v>
-      </c>
-      <c r="D80" s="15">
-        <v>200</v>
-      </c>
-      <c r="F80">
-        <v>79</v>
       </c>
     </row>
     <row r="81" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A81" s="19"/>
       <c r="B81" s="17" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="C81" s="18">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="D81" s="15">
         <v>300</v>
       </c>
       <c r="F81">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="82" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A82" s="19"/>
+      <c r="B82" s="17" t="s">
+        <v>102</v>
+      </c>
+      <c r="C82" s="18">
+        <v>3</v>
+      </c>
+      <c r="D82" s="15">
+        <v>200</v>
+      </c>
+      <c r="F82">
         <v>80</v>
       </c>
     </row>
-    <row r="82" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A82" s="20"/>
-      <c r="B82" s="21"/>
-      <c r="C82" s="22"/>
-    </row>
     <row r="83" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A83" s="20"/>
-      <c r="B83" s="21"/>
-      <c r="C83" s="22"/>
+      <c r="A83" s="19"/>
+      <c r="B83" s="17" t="s">
+        <v>102</v>
+      </c>
+      <c r="C83" s="18">
+        <v>4</v>
+      </c>
+      <c r="D83" s="15">
+        <v>200</v>
+      </c>
+      <c r="F83">
+        <v>81</v>
+      </c>
     </row>
     <row r="84" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A84" s="20"/>
-      <c r="B84" s="21"/>
-      <c r="C84" s="22"/>
+      <c r="A84" s="19"/>
+      <c r="B84" s="17" t="s">
+        <v>102</v>
+      </c>
+      <c r="C84" s="18">
+        <v>5</v>
+      </c>
+      <c r="D84" s="15">
+        <v>300</v>
+      </c>
+      <c r="F84">
+        <v>82</v>
+      </c>
     </row>
     <row r="85" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A85" s="20"/>
@@ -2889,14 +2943,29 @@
       <c r="B201" s="21"/>
       <c r="C201" s="22"/>
     </row>
+    <row r="202" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A202" s="20"/>
+      <c r="B202" s="21"/>
+      <c r="C202" s="22"/>
+    </row>
+    <row r="203" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A203" s="20"/>
+      <c r="B203" s="21"/>
+      <c r="C203" s="22"/>
+    </row>
+    <row r="204" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A204" s="20"/>
+      <c r="B204" s="21"/>
+      <c r="C204" s="22"/>
+    </row>
   </sheetData>
   <mergeCells count="4">
-    <mergeCell ref="A13:A15"/>
     <mergeCell ref="A16:A18"/>
-    <mergeCell ref="A22:A27"/>
-    <mergeCell ref="A28:A30"/>
+    <mergeCell ref="A19:A21"/>
+    <mergeCell ref="A25:A30"/>
+    <mergeCell ref="A31:A33"/>
   </mergeCells>
-  <dataValidations count="9">
+  <dataValidations count="12">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D4" xr:uid="{CDBB5640-3705-4524-A12C-18C0BA89A391}">
       <formula1>"graminoid, forb/herb, shrub, tree, nonvascular"</formula1>
     </dataValidation>
@@ -2906,25 +2975,34 @@
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D6" xr:uid="{FCAB33B4-E22D-416A-9EE8-1B6629F4B7A9}">
       <formula1>"angiosperm, gymnosperm"</formula1>
     </dataValidation>
-    <dataValidation type="whole" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D43" xr:uid="{2A9331BB-EEBF-40CD-B47D-E4013CB2D0AD}">
+    <dataValidation type="whole" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D46" xr:uid="{2A9331BB-EEBF-40CD-B47D-E4013CB2D0AD}">
       <formula1>0</formula1>
     </dataValidation>
-    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D19 D39:D42 D44:D47" xr:uid="{C20F82BC-B9F3-4514-8D12-0BF659884D61}">
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D22 D42:D45 D47:D50" xr:uid="{C20F82BC-B9F3-4514-8D12-0BF659884D61}">
       <formula1>0</formula1>
       <formula2>1</formula2>
     </dataValidation>
-    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D10:D12" xr:uid="{89511D6B-7806-4594-AA02-B0D66F3A6A50}">
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D13:D15" xr:uid="{89511D6B-7806-4594-AA02-B0D66F3A6A50}">
       <formula1>1</formula1>
       <formula2>366</formula2>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D8" xr:uid="{5620C1FF-B28B-4556-ADEF-5FA98FE67CB9}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D11" xr:uid="{5620C1FF-B28B-4556-ADEF-5FA98FE67CB9}">
       <formula1>"C3, C4, CAM"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D9" xr:uid="{D43B937F-2CE8-47D9-A978-7D336015DF11}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D12" xr:uid="{D43B937F-2CE8-47D9-A978-7D336015DF11}">
       <formula1>"Annual, Herbaceous perennial, Woody perennial"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D7:D8" xr:uid="{6E5E4A37-6A5B-480B-8E8F-63973FC4A36F}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D7 D11" xr:uid="{6E5E4A37-6A5B-480B-8E8F-63973FC4A36F}">
       <formula1>"annual, perennial"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D10" xr:uid="{9C2C3F79-B79E-49D3-96C9-4B893A4F4CBC}">
+      <formula1>"climbing,columnar,conical,decumbent,erect,irregular,oval,prostrate,rounded,semi_erect,vase"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D9" xr:uid="{E22474F0-0264-4C55-99F3-1F4582999007}">
+      <formula1>"bunch, colonizing, multiple_stems, rhizomatous,single_crown,single_stem,stoloniferous,thicket_forming"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D8" xr:uid="{793E17DF-C558-4DAF-B608-9E20297CD619}">
+      <formula1>"evergreen, deciduous"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2933,10 +3011,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7A5B2ED1-E60A-481E-A183-520033C5AF7F}">
-  <dimension ref="A1:G201"/>
+  <dimension ref="A1:G204"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="E30" sqref="E30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2989,7 +3067,7 @@
       </c>
       <c r="C3" s="11"/>
       <c r="D3" s="12" t="s">
-        <v>108</v>
+        <v>119</v>
       </c>
       <c r="F3">
         <v>2</v>
@@ -3000,7 +3078,7 @@
         <v>8</v>
       </c>
       <c r="B4" s="10" t="s">
-        <v>9</v>
+        <v>117</v>
       </c>
       <c r="C4" s="11"/>
       <c r="D4" s="12" t="s">
@@ -3045,11 +3123,11 @@
         <v>17</v>
       </c>
       <c r="B7" s="10" t="s">
-        <v>18</v>
+        <v>116</v>
       </c>
       <c r="C7" s="11"/>
       <c r="D7" s="12" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="F7">
         <v>6</v>
@@ -3057,41 +3135,44 @@
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="9" t="s">
-        <v>19</v>
+        <v>108</v>
       </c>
       <c r="B8" s="10" t="s">
-        <v>20</v>
+        <v>118</v>
       </c>
       <c r="C8" s="11"/>
       <c r="D8" s="12" t="s">
-        <v>21</v>
+        <v>112</v>
       </c>
       <c r="F8">
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="18" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="B9" s="6"/>
-      <c r="C9" s="7"/>
-      <c r="D9" s="14"/>
-      <c r="E9" s="8"/>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" s="9" t="s">
+        <v>109</v>
+      </c>
+      <c r="B9" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="C9" s="11"/>
+      <c r="D9" s="12" t="s">
+        <v>115</v>
+      </c>
       <c r="F9">
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="9" t="s">
-        <v>23</v>
+        <v>110</v>
       </c>
       <c r="B10" s="10" t="s">
-        <v>24</v>
+        <v>111</v>
       </c>
       <c r="C10" s="11"/>
-      <c r="D10" s="15">
-        <v>244</v>
+      <c r="D10" s="12" t="s">
+        <v>114</v>
       </c>
       <c r="F10">
         <v>9</v>
@@ -3099,76 +3180,71 @@
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="9" t="s">
-        <v>25</v>
+        <v>18</v>
       </c>
       <c r="B11" s="10" t="s">
-        <v>26</v>
+        <v>19</v>
       </c>
       <c r="C11" s="11"/>
-      <c r="D11" s="15">
-        <v>305</v>
+      <c r="D11" s="12" t="s">
+        <v>105</v>
       </c>
       <c r="F11">
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12" s="9" t="s">
-        <v>27</v>
-      </c>
-      <c r="B12" s="10" t="s">
-        <v>28</v>
-      </c>
-      <c r="C12" s="11"/>
-      <c r="D12" s="15">
-        <v>273</v>
-      </c>
+    <row r="12" spans="1:6" ht="18" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A12" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="B12" s="6"/>
+      <c r="C12" s="7"/>
+      <c r="D12" s="14"/>
+      <c r="E12" s="8"/>
       <c r="F12">
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A13" s="25" t="s">
-        <v>29</v>
+    <row r="13" spans="1:6" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="9" t="s">
+        <v>21</v>
       </c>
       <c r="B13" s="10" t="s">
-        <v>110</v>
-      </c>
-      <c r="C13" s="11" t="s">
-        <v>30</v>
-      </c>
+        <v>22</v>
+      </c>
+      <c r="C13" s="11"/>
       <c r="D13" s="15">
-        <v>1.4999999999999999E-2</v>
+        <v>144</v>
       </c>
       <c r="F13">
         <v>12</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A14" s="25"/>
+      <c r="A14" s="9" t="s">
+        <v>23</v>
+      </c>
       <c r="B14" s="10" t="s">
-        <v>110</v>
-      </c>
-      <c r="C14" s="11" t="s">
-        <v>31</v>
-      </c>
+        <v>24</v>
+      </c>
+      <c r="C14" s="11"/>
       <c r="D14" s="15">
-        <v>1.4999999999999999E-2</v>
+        <v>305</v>
       </c>
       <c r="F14">
         <v>13</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A15" s="25"/>
+      <c r="A15" s="9" t="s">
+        <v>25</v>
+      </c>
       <c r="B15" s="10" t="s">
-        <v>110</v>
-      </c>
-      <c r="C15" s="11" t="s">
-        <v>32</v>
-      </c>
+        <v>26</v>
+      </c>
+      <c r="C15" s="11"/>
       <c r="D15" s="15">
-        <v>0.03</v>
+        <v>273</v>
       </c>
       <c r="F15">
         <v>14</v>
@@ -3176,16 +3252,16 @@
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="25" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="B16" s="10" t="s">
-        <v>34</v>
+        <v>107</v>
       </c>
       <c r="C16" s="11" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="D16" s="15">
-        <v>1.444</v>
+        <v>1.4999999999999999E-2</v>
       </c>
       <c r="F16">
         <v>15</v>
@@ -3194,13 +3270,13 @@
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="25"/>
       <c r="B17" s="10" t="s">
-        <v>34</v>
+        <v>107</v>
       </c>
       <c r="C17" s="11" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="D17" s="15">
-        <v>1.5129999999999999</v>
+        <v>1.4999999999999999E-2</v>
       </c>
       <c r="F17">
         <v>16</v>
@@ -3209,133 +3285,141 @@
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" s="25"/>
       <c r="B18" s="10" t="s">
-        <v>34</v>
+        <v>107</v>
       </c>
       <c r="C18" s="11" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="D18" s="15">
-        <v>1.4630000000000001</v>
+        <v>0.03</v>
       </c>
       <c r="F18">
         <v>17</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A19" s="9" t="s">
-        <v>35</v>
+      <c r="A19" s="25" t="s">
+        <v>31</v>
       </c>
       <c r="B19" s="10" t="s">
-        <v>36</v>
-      </c>
-      <c r="C19" s="11"/>
+        <v>32</v>
+      </c>
+      <c r="C19" s="11" t="s">
+        <v>28</v>
+      </c>
       <c r="D19" s="15">
-        <v>0.48</v>
+        <v>1.444</v>
       </c>
       <c r="F19">
         <v>18</v>
       </c>
     </row>
-    <row r="20" spans="1:7" ht="32.25" x14ac:dyDescent="0.25">
-      <c r="A20" s="9" t="s">
-        <v>37</v>
-      </c>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A20" s="25"/>
       <c r="B20" s="10" t="s">
-        <v>38</v>
-      </c>
-      <c r="C20" s="11"/>
+        <v>32</v>
+      </c>
+      <c r="C20" s="11" t="s">
+        <v>29</v>
+      </c>
       <c r="D20" s="15">
-        <v>100</v>
-      </c>
-      <c r="E20" t="s">
-        <v>109</v>
+        <v>1.5129999999999999</v>
       </c>
       <c r="F20">
         <v>19</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A21" s="9" t="s">
-        <v>39</v>
-      </c>
+      <c r="A21" s="25"/>
       <c r="B21" s="10" t="s">
-        <v>40</v>
-      </c>
-      <c r="C21" s="11"/>
+        <v>32</v>
+      </c>
+      <c r="C21" s="11" t="s">
+        <v>30</v>
+      </c>
       <c r="D21" s="15">
-        <v>0.5</v>
+        <v>1.4630000000000001</v>
       </c>
       <c r="F21">
         <v>20</v>
       </c>
     </row>
-    <row r="22" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A22" s="26" t="s">
-        <v>41</v>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A22" s="9" t="s">
+        <v>33</v>
       </c>
       <c r="B22" s="10" t="s">
-        <v>42</v>
-      </c>
-      <c r="C22" s="11" t="s">
-        <v>43</v>
-      </c>
-      <c r="D22" s="15"/>
-      <c r="E22" s="16" t="s">
-        <v>44</v>
+        <v>34</v>
+      </c>
+      <c r="C22" s="11"/>
+      <c r="D22" s="15">
+        <v>0.48</v>
       </c>
       <c r="F22">
         <v>21</v>
       </c>
-      <c r="G22" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A23" s="26"/>
+    </row>
+    <row r="23" spans="1:7" ht="32.25" x14ac:dyDescent="0.25">
+      <c r="A23" s="9" t="s">
+        <v>35</v>
+      </c>
       <c r="B23" s="10" t="s">
-        <v>42</v>
-      </c>
-      <c r="C23" s="11" t="s">
-        <v>46</v>
-      </c>
-      <c r="D23" s="15"/>
+        <v>36</v>
+      </c>
+      <c r="C23" s="11"/>
+      <c r="D23" s="15">
+        <v>100</v>
+      </c>
+      <c r="E23" t="s">
+        <v>106</v>
+      </c>
       <c r="F23">
         <v>22</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A24" s="26"/>
+      <c r="A24" s="9" t="s">
+        <v>37</v>
+      </c>
       <c r="B24" s="10" t="s">
-        <v>42</v>
-      </c>
-      <c r="C24" s="11" t="s">
-        <v>47</v>
-      </c>
-      <c r="D24" s="15"/>
+        <v>38</v>
+      </c>
+      <c r="C24" s="11"/>
+      <c r="D24" s="15">
+        <v>0.05</v>
+      </c>
       <c r="F24">
         <v>23</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A25" s="26"/>
+    <row r="25" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A25" s="26" t="s">
+        <v>39</v>
+      </c>
       <c r="B25" s="10" t="s">
-        <v>48</v>
+        <v>40</v>
       </c>
       <c r="C25" s="11" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="D25" s="15"/>
+      <c r="E25" s="16" t="s">
+        <v>42</v>
+      </c>
       <c r="F25">
         <v>24</v>
+      </c>
+      <c r="G25" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" s="26"/>
       <c r="B26" s="10" t="s">
-        <v>48</v>
+        <v>40</v>
       </c>
       <c r="C26" s="11" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="D26" s="15"/>
       <c r="F26">
@@ -3345,10 +3429,10 @@
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" s="26"/>
       <c r="B27" s="10" t="s">
-        <v>48</v>
+        <v>40</v>
       </c>
       <c r="C27" s="11" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="D27" s="15"/>
       <c r="F27">
@@ -3356,233 +3440,230 @@
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A28" s="27" t="s">
-        <v>49</v>
-      </c>
-      <c r="B28" s="17" t="s">
-        <v>50</v>
-      </c>
-      <c r="C28" s="18" t="s">
-        <v>30</v>
-      </c>
-      <c r="D28" s="15">
-        <v>0.01</v>
-      </c>
+      <c r="A28" s="26"/>
+      <c r="B28" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="C28" s="11" t="s">
+        <v>41</v>
+      </c>
+      <c r="D28" s="15"/>
       <c r="F28">
         <v>27</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A29" s="27"/>
-      <c r="B29" s="17" t="s">
-        <v>50</v>
-      </c>
-      <c r="C29" s="18" t="s">
-        <v>31</v>
-      </c>
-      <c r="D29" s="15">
-        <v>0.1</v>
-      </c>
+      <c r="A29" s="26"/>
+      <c r="B29" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="C29" s="11" t="s">
+        <v>44</v>
+      </c>
+      <c r="D29" s="15"/>
       <c r="F29">
         <v>28</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A30" s="27"/>
-      <c r="B30" s="17" t="s">
-        <v>50</v>
-      </c>
-      <c r="C30" s="18" t="s">
-        <v>32</v>
-      </c>
-      <c r="D30" s="15">
-        <v>0.5</v>
-      </c>
+      <c r="A30" s="26"/>
+      <c r="B30" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="C30" s="11" t="s">
+        <v>45</v>
+      </c>
+      <c r="D30" s="15"/>
       <c r="F30">
         <v>29</v>
       </c>
     </row>
-    <row r="31" spans="1:7" ht="18" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A31" s="5" t="s">
-        <v>51</v>
-      </c>
-      <c r="B31" s="6"/>
-      <c r="C31" s="7"/>
-      <c r="D31" s="6"/>
-      <c r="E31" s="8"/>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A31" s="27" t="s">
+        <v>47</v>
+      </c>
+      <c r="B31" s="17" t="s">
+        <v>48</v>
+      </c>
+      <c r="C31" s="18" t="s">
+        <v>28</v>
+      </c>
+      <c r="D31" s="15">
+        <v>0.01</v>
+      </c>
       <c r="F31">
         <v>30</v>
       </c>
     </row>
-    <row r="32" spans="1:7" ht="18" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="19" t="s">
-        <v>52</v>
-      </c>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A32" s="27"/>
       <c r="B32" s="17" t="s">
-        <v>53</v>
-      </c>
-      <c r="C32" s="18"/>
+        <v>48</v>
+      </c>
+      <c r="C32" s="18" t="s">
+        <v>29</v>
+      </c>
       <c r="D32" s="15">
-        <v>34</v>
+        <v>0.1</v>
       </c>
       <c r="F32">
         <v>31</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A33" s="19" t="s">
-        <v>54</v>
-      </c>
+      <c r="A33" s="27"/>
       <c r="B33" s="17" t="s">
-        <v>55</v>
-      </c>
-      <c r="C33" s="18"/>
+        <v>48</v>
+      </c>
+      <c r="C33" s="18" t="s">
+        <v>30</v>
+      </c>
       <c r="D33" s="15">
-        <v>3</v>
+        <v>0.5</v>
       </c>
       <c r="F33">
         <v>32</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A34" s="19" t="s">
-        <v>56</v>
-      </c>
-      <c r="B34" s="17" t="s">
-        <v>57</v>
-      </c>
-      <c r="C34" s="18"/>
-      <c r="D34" s="15">
-        <v>1</v>
-      </c>
+    <row r="34" spans="1:6" ht="18" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A34" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="B34" s="6"/>
+      <c r="C34" s="7"/>
+      <c r="D34" s="6"/>
+      <c r="E34" s="8"/>
       <c r="F34">
         <v>33</v>
       </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:6" ht="18" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A35" s="19" t="s">
-        <v>58</v>
+        <v>50</v>
       </c>
       <c r="B35" s="17" t="s">
-        <v>59</v>
+        <v>51</v>
       </c>
       <c r="C35" s="18"/>
       <c r="D35" s="15">
-        <v>1.45</v>
+        <v>34</v>
       </c>
       <c r="F35">
         <v>34</v>
       </c>
     </row>
-    <row r="36" spans="1:6" ht="17.25" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36" s="19" t="s">
-        <v>60</v>
+        <v>52</v>
       </c>
       <c r="B36" s="17" t="s">
-        <v>61</v>
+        <v>53</v>
       </c>
       <c r="C36" s="18"/>
       <c r="D36" s="15">
-        <v>0.23100000000000001</v>
+        <v>3</v>
       </c>
       <c r="F36">
         <v>35</v>
       </c>
     </row>
-    <row r="37" spans="1:6" ht="18" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A37" s="5" t="s">
-        <v>62</v>
-      </c>
-      <c r="B37" s="6"/>
-      <c r="C37" s="7"/>
-      <c r="D37" s="6"/>
-      <c r="E37" s="8"/>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A37" s="19" t="s">
+        <v>54</v>
+      </c>
+      <c r="B37" s="17" t="s">
+        <v>55</v>
+      </c>
+      <c r="C37" s="18"/>
+      <c r="D37" s="15">
+        <v>1</v>
+      </c>
       <c r="F37">
         <v>36</v>
       </c>
     </row>
-    <row r="38" spans="1:6" ht="30.75" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38" s="19" t="s">
-        <v>63</v>
+        <v>56</v>
       </c>
       <c r="B38" s="17" t="s">
-        <v>64</v>
+        <v>57</v>
       </c>
       <c r="C38" s="18"/>
       <c r="D38" s="15">
-        <v>4</v>
+        <v>1.45</v>
       </c>
       <c r="F38">
         <v>37</v>
       </c>
     </row>
-    <row r="39" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:6" ht="17.25" x14ac:dyDescent="0.25">
       <c r="A39" s="19" t="s">
-        <v>65</v>
+        <v>58</v>
       </c>
       <c r="B39" s="17" t="s">
-        <v>66</v>
+        <v>59</v>
       </c>
       <c r="C39" s="18"/>
       <c r="D39" s="15">
-        <v>0.5</v>
+        <v>0.23100000000000001</v>
       </c>
       <c r="F39">
         <v>38</v>
       </c>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A40" s="19" t="s">
-        <v>67</v>
-      </c>
-      <c r="B40" s="17" t="s">
-        <v>68</v>
-      </c>
-      <c r="C40" s="18"/>
-      <c r="D40" s="15">
-        <v>0</v>
-      </c>
+    <row r="40" spans="1:6" ht="18" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A40" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="B40" s="6"/>
+      <c r="C40" s="7"/>
+      <c r="D40" s="6"/>
+      <c r="E40" s="8"/>
       <c r="F40">
         <v>39</v>
       </c>
     </row>
-    <row r="41" spans="1:6" ht="18" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A41" s="5" t="s">
-        <v>69</v>
-      </c>
-      <c r="B41" s="6"/>
-      <c r="C41" s="7"/>
-      <c r="D41" s="6"/>
-      <c r="E41" s="8"/>
+    <row r="41" spans="1:6" ht="30.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A41" s="19" t="s">
+        <v>61</v>
+      </c>
+      <c r="B41" s="17" t="s">
+        <v>62</v>
+      </c>
+      <c r="C41" s="18"/>
+      <c r="D41" s="15">
+        <v>4</v>
+      </c>
       <c r="F41">
         <v>40</v>
       </c>
     </row>
-    <row r="42" spans="1:6" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A42" s="19" t="s">
-        <v>70</v>
+        <v>63</v>
       </c>
       <c r="B42" s="17" t="s">
-        <v>71</v>
+        <v>64</v>
       </c>
       <c r="C42" s="18"/>
       <c r="D42" s="15">
-        <v>0.01</v>
+        <v>0.5</v>
       </c>
       <c r="F42">
         <v>41</v>
       </c>
     </row>
-    <row r="43" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A43" s="19" t="s">
-        <v>72</v>
+        <v>65</v>
       </c>
       <c r="B43" s="17" t="s">
-        <v>73</v>
+        <v>66</v>
       </c>
       <c r="C43" s="18"/>
       <c r="D43" s="15">
-        <v>365</v>
+        <v>0</v>
       </c>
       <c r="F43">
         <v>42</v>
@@ -3590,7 +3671,7 @@
     </row>
     <row r="44" spans="1:6" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A44" s="5" t="s">
-        <v>74</v>
+        <v>67</v>
       </c>
       <c r="B44" s="6"/>
       <c r="C44" s="7"/>
@@ -3600,19 +3681,16 @@
         <v>43</v>
       </c>
     </row>
-    <row r="45" spans="1:6" ht="30.75" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:6" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A45" s="19" t="s">
-        <v>75</v>
+        <v>68</v>
       </c>
       <c r="B45" s="17" t="s">
-        <v>76</v>
+        <v>69</v>
       </c>
       <c r="C45" s="18"/>
       <c r="D45" s="15">
-        <v>0.25</v>
-      </c>
-      <c r="E45" t="s">
-        <v>77</v>
+        <v>0.01</v>
       </c>
       <c r="F45">
         <v>44</v>
@@ -3620,14 +3698,14 @@
     </row>
     <row r="46" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A46" s="19" t="s">
-        <v>78</v>
+        <v>70</v>
       </c>
       <c r="B46" s="17" t="s">
-        <v>79</v>
+        <v>71</v>
       </c>
       <c r="C46" s="18"/>
       <c r="D46" s="15">
-        <v>0.25</v>
+        <v>365</v>
       </c>
       <c r="F46">
         <v>45</v>
@@ -3635,107 +3713,109 @@
     </row>
     <row r="47" spans="1:6" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A47" s="5" t="s">
-        <v>80</v>
+        <v>72</v>
       </c>
       <c r="B47" s="6"/>
       <c r="C47" s="7"/>
       <c r="D47" s="6"/>
-      <c r="E47" s="8" t="s">
-        <v>81</v>
-      </c>
+      <c r="E47" s="8"/>
       <c r="F47">
         <v>46</v>
       </c>
     </row>
-    <row r="48" spans="1:6" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:6" ht="30.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A48" s="19" t="s">
-        <v>82</v>
+        <v>73</v>
       </c>
       <c r="B48" s="17" t="s">
-        <v>83</v>
+        <v>74</v>
       </c>
       <c r="C48" s="18"/>
-      <c r="D48" s="12" t="s">
-        <v>84</v>
+      <c r="D48" s="15">
+        <v>0.25</v>
       </c>
       <c r="E48" t="s">
-        <v>85</v>
+        <v>75</v>
       </c>
       <c r="F48">
         <v>47</v>
       </c>
     </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A49" s="19" t="s">
-        <v>86</v>
+        <v>76</v>
       </c>
       <c r="B49" s="17" t="s">
-        <v>87</v>
+        <v>77</v>
       </c>
       <c r="C49" s="18"/>
       <c r="D49" s="15">
-        <v>207</v>
+        <v>0.25</v>
       </c>
       <c r="F49">
         <v>48</v>
       </c>
     </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A50" s="19" t="s">
-        <v>88</v>
-      </c>
-      <c r="B50" s="17" t="s">
-        <v>89</v>
-      </c>
-      <c r="C50" s="18">
-        <v>1</v>
-      </c>
-      <c r="D50" s="15">
-        <v>30</v>
+    <row r="50" spans="1:6" ht="18" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A50" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="B50" s="6"/>
+      <c r="C50" s="7"/>
+      <c r="D50" s="6"/>
+      <c r="E50" s="8" t="s">
+        <v>79</v>
       </c>
       <c r="F50">
         <v>49</v>
       </c>
     </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A51" s="19"/>
+    <row r="51" spans="1:6" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A51" s="19" t="s">
+        <v>80</v>
+      </c>
       <c r="B51" s="17" t="s">
-        <v>89</v>
-      </c>
-      <c r="C51" s="18">
-        <v>2</v>
-      </c>
-      <c r="D51" s="15">
-        <v>40</v>
+        <v>81</v>
+      </c>
+      <c r="C51" s="18"/>
+      <c r="D51" s="12" t="s">
+        <v>82</v>
+      </c>
+      <c r="E51" t="s">
+        <v>83</v>
       </c>
       <c r="F51">
         <v>50</v>
       </c>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A52" s="19"/>
+      <c r="A52" s="19" t="s">
+        <v>84</v>
+      </c>
       <c r="B52" s="17" t="s">
-        <v>89</v>
-      </c>
-      <c r="C52" s="18">
-        <v>3</v>
-      </c>
+        <v>85</v>
+      </c>
+      <c r="C52" s="18"/>
       <c r="D52" s="15">
-        <v>50</v>
+        <v>207</v>
       </c>
       <c r="F52">
         <v>51</v>
       </c>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A53" s="19"/>
+      <c r="A53" s="19" t="s">
+        <v>86</v>
+      </c>
       <c r="B53" s="17" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="C53" s="18">
-        <v>4</v>
-      </c>
-      <c r="D53" s="15"/>
+        <v>1</v>
+      </c>
+      <c r="D53" s="15">
+        <v>30</v>
+      </c>
       <c r="F53">
         <v>52</v>
       </c>
@@ -3743,28 +3823,28 @@
     <row r="54" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A54" s="19"/>
       <c r="B54" s="17" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="C54" s="18">
-        <v>5</v>
-      </c>
-      <c r="D54" s="15"/>
+        <v>2</v>
+      </c>
+      <c r="D54" s="15">
+        <v>40</v>
+      </c>
       <c r="F54">
         <v>53</v>
       </c>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A55" s="19" t="s">
-        <v>90</v>
-      </c>
+      <c r="A55" s="19"/>
       <c r="B55" s="17" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="C55" s="18">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D55" s="15">
-        <v>0.01</v>
+        <v>50</v>
       </c>
       <c r="F55">
         <v>54</v>
@@ -3773,14 +3853,12 @@
     <row r="56" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A56" s="19"/>
       <c r="B56" s="17" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="C56" s="18">
-        <v>2</v>
-      </c>
-      <c r="D56" s="15">
-        <v>0.25</v>
-      </c>
+        <v>4</v>
+      </c>
+      <c r="D56" s="15"/>
       <c r="F56">
         <v>55</v>
       </c>
@@ -3788,27 +3866,29 @@
     <row r="57" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A57" s="19"/>
       <c r="B57" s="17" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="C57" s="18">
-        <v>3</v>
-      </c>
-      <c r="D57" s="15">
-        <v>0.67</v>
-      </c>
+        <v>5</v>
+      </c>
+      <c r="D57" s="15"/>
       <c r="F57">
         <v>56</v>
       </c>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A58" s="19"/>
+      <c r="A58" s="19" t="s">
+        <v>88</v>
+      </c>
       <c r="B58" s="17" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="C58" s="18">
-        <v>4</v>
-      </c>
-      <c r="D58" s="15"/>
+        <v>1</v>
+      </c>
+      <c r="D58" s="15">
+        <v>0.01</v>
+      </c>
       <c r="F58">
         <v>57</v>
       </c>
@@ -3816,28 +3896,28 @@
     <row r="59" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A59" s="19"/>
       <c r="B59" s="17" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="C59" s="18">
-        <v>5</v>
-      </c>
-      <c r="D59" s="15"/>
+        <v>2</v>
+      </c>
+      <c r="D59" s="15">
+        <v>0.25</v>
+      </c>
       <c r="F59">
         <v>58</v>
       </c>
     </row>
-    <row r="60" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A60" s="19" t="s">
-        <v>92</v>
-      </c>
+    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A60" s="19"/>
       <c r="B60" s="17" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="C60" s="18">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D60" s="15">
-        <v>1</v>
+        <v>0.67</v>
       </c>
       <c r="F60">
         <v>59</v>
@@ -3846,14 +3926,12 @@
     <row r="61" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A61" s="19"/>
       <c r="B61" s="17" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="C61" s="18">
-        <v>2</v>
-      </c>
-      <c r="D61" s="15">
-        <v>1</v>
-      </c>
+        <v>4</v>
+      </c>
+      <c r="D61" s="15"/>
       <c r="F61">
         <v>60</v>
       </c>
@@ -3861,27 +3939,29 @@
     <row r="62" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A62" s="19"/>
       <c r="B62" s="17" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="C62" s="18">
-        <v>3</v>
-      </c>
-      <c r="D62" s="15">
-        <v>1</v>
-      </c>
+        <v>5</v>
+      </c>
+      <c r="D62" s="15"/>
       <c r="F62">
         <v>61</v>
       </c>
     </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A63" s="19"/>
+    <row r="63" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A63" s="19" t="s">
+        <v>90</v>
+      </c>
       <c r="B63" s="17" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="C63" s="18">
-        <v>4</v>
-      </c>
-      <c r="D63" s="15"/>
+        <v>1</v>
+      </c>
+      <c r="D63" s="15">
+        <v>1</v>
+      </c>
       <c r="F63">
         <v>62</v>
       </c>
@@ -3889,103 +3969,101 @@
     <row r="64" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A64" s="19"/>
       <c r="B64" s="17" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="C64" s="18">
-        <v>5</v>
-      </c>
-      <c r="D64" s="15"/>
+        <v>2</v>
+      </c>
+      <c r="D64" s="15">
+        <v>1</v>
+      </c>
       <c r="F64">
         <v>63</v>
       </c>
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A65" s="19" t="s">
-        <v>94</v>
-      </c>
+      <c r="A65" s="19"/>
       <c r="B65" s="17" t="s">
-        <v>95</v>
-      </c>
-      <c r="C65" s="18"/>
-      <c r="D65" s="12" t="s">
-        <v>96</v>
+        <v>91</v>
+      </c>
+      <c r="C65" s="18">
+        <v>3</v>
+      </c>
+      <c r="D65" s="15">
+        <v>1</v>
       </c>
       <c r="F65">
         <v>64</v>
       </c>
     </row>
     <row r="66" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A66" s="19" t="s">
-        <v>97</v>
-      </c>
+      <c r="A66" s="19"/>
       <c r="B66" s="17" t="s">
-        <v>98</v>
-      </c>
-      <c r="C66" s="18"/>
-      <c r="D66" s="15">
-        <v>365</v>
-      </c>
+        <v>91</v>
+      </c>
+      <c r="C66" s="18">
+        <v>4</v>
+      </c>
+      <c r="D66" s="15"/>
       <c r="F66">
         <v>65</v>
       </c>
     </row>
     <row r="67" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A67" s="19" t="s">
-        <v>99</v>
-      </c>
+      <c r="A67" s="19"/>
       <c r="B67" s="17" t="s">
-        <v>100</v>
+        <v>91</v>
       </c>
       <c r="C67" s="18">
-        <v>1</v>
-      </c>
-      <c r="D67" s="15">
-        <v>0</v>
-      </c>
+        <v>5</v>
+      </c>
+      <c r="D67" s="15"/>
       <c r="F67">
         <v>66</v>
       </c>
     </row>
     <row r="68" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A68" s="19"/>
+      <c r="A68" s="19" t="s">
+        <v>92</v>
+      </c>
       <c r="B68" s="17" t="s">
-        <v>100</v>
-      </c>
-      <c r="C68" s="18">
-        <v>2</v>
-      </c>
-      <c r="D68" s="15">
-        <v>0.2</v>
+        <v>93</v>
+      </c>
+      <c r="C68" s="18"/>
+      <c r="D68" s="12" t="s">
+        <v>94</v>
       </c>
       <c r="F68">
         <v>67</v>
       </c>
     </row>
     <row r="69" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A69" s="19"/>
+      <c r="A69" s="19" t="s">
+        <v>95</v>
+      </c>
       <c r="B69" s="17" t="s">
-        <v>100</v>
-      </c>
-      <c r="C69" s="18">
-        <v>3</v>
-      </c>
+        <v>96</v>
+      </c>
+      <c r="C69" s="18"/>
       <c r="D69" s="15">
-        <v>0.5</v>
+        <v>365</v>
       </c>
       <c r="F69">
         <v>68</v>
       </c>
     </row>
     <row r="70" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A70" s="19"/>
+      <c r="A70" s="19" t="s">
+        <v>97</v>
+      </c>
       <c r="B70" s="17" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="C70" s="18">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="D70" s="15">
-        <v>0.68</v>
+        <v>0</v>
       </c>
       <c r="F70">
         <v>69</v>
@@ -3994,30 +4072,28 @@
     <row r="71" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A71" s="19"/>
       <c r="B71" s="17" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="C71" s="18">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="D71" s="15">
-        <v>1.1200000000000001</v>
+        <v>0.2</v>
       </c>
       <c r="F71">
         <v>70</v>
       </c>
     </row>
     <row r="72" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A72" s="19" t="s">
-        <v>101</v>
-      </c>
+      <c r="A72" s="19"/>
       <c r="B72" s="17" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="C72" s="18">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D72" s="15">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="F72">
         <v>71</v>
@@ -4026,13 +4102,13 @@
     <row r="73" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A73" s="19"/>
       <c r="B73" s="17" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="C73" s="18">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="D73" s="15">
-        <v>0</v>
+        <v>0.68</v>
       </c>
       <c r="F73">
         <v>72</v>
@@ -4041,28 +4117,30 @@
     <row r="74" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A74" s="19"/>
       <c r="B74" s="17" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="C74" s="18">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="D74" s="15">
-        <v>0</v>
+        <v>1.1200000000000001</v>
       </c>
       <c r="F74">
         <v>73</v>
       </c>
     </row>
     <row r="75" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A75" s="19"/>
+      <c r="A75" s="19" t="s">
+        <v>99</v>
+      </c>
       <c r="B75" s="17" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="C75" s="18">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="D75" s="15">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F75">
         <v>74</v>
@@ -4071,30 +4149,28 @@
     <row r="76" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A76" s="19"/>
       <c r="B76" s="17" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="C76" s="18">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="D76" s="15">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F76">
         <v>75</v>
       </c>
     </row>
-    <row r="77" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A77" s="19" t="s">
-        <v>103</v>
-      </c>
+    <row r="77" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A77" s="19"/>
       <c r="B77" s="17" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="C77" s="18">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D77" s="15">
-        <v>500</v>
+        <v>0</v>
       </c>
       <c r="F77">
         <v>76</v>
@@ -4103,13 +4179,13 @@
     <row r="78" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A78" s="19"/>
       <c r="B78" s="17" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="C78" s="18">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="D78" s="15">
-        <v>300</v>
+        <v>1</v>
       </c>
       <c r="F78">
         <v>77</v>
@@ -4118,28 +4194,30 @@
     <row r="79" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A79" s="19"/>
       <c r="B79" s="17" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="C79" s="18">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="D79" s="15">
-        <v>200</v>
+        <v>1</v>
       </c>
       <c r="F79">
         <v>78</v>
       </c>
     </row>
-    <row r="80" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A80" s="19"/>
+    <row r="80" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A80" s="19" t="s">
+        <v>101</v>
+      </c>
       <c r="B80" s="17" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="C80" s="18">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="D80" s="15">
-        <v>200</v>
+        <v>500</v>
       </c>
       <c r="F80">
         <v>79</v>
@@ -4148,10 +4226,10 @@
     <row r="81" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A81" s="19"/>
       <c r="B81" s="17" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="C81" s="18">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="D81" s="15">
         <v>300</v>
@@ -4161,19 +4239,49 @@
       </c>
     </row>
     <row r="82" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A82" s="20"/>
-      <c r="B82" s="21"/>
-      <c r="C82" s="22"/>
+      <c r="A82" s="19"/>
+      <c r="B82" s="17" t="s">
+        <v>102</v>
+      </c>
+      <c r="C82" s="18">
+        <v>3</v>
+      </c>
+      <c r="D82" s="15">
+        <v>200</v>
+      </c>
+      <c r="F82">
+        <v>81</v>
+      </c>
     </row>
     <row r="83" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A83" s="20"/>
-      <c r="B83" s="21"/>
-      <c r="C83" s="22"/>
+      <c r="A83" s="19"/>
+      <c r="B83" s="17" t="s">
+        <v>102</v>
+      </c>
+      <c r="C83" s="18">
+        <v>4</v>
+      </c>
+      <c r="D83" s="15">
+        <v>200</v>
+      </c>
+      <c r="F83">
+        <v>82</v>
+      </c>
     </row>
     <row r="84" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A84" s="20"/>
-      <c r="B84" s="21"/>
-      <c r="C84" s="22"/>
+      <c r="A84" s="19"/>
+      <c r="B84" s="17" t="s">
+        <v>102</v>
+      </c>
+      <c r="C84" s="18">
+        <v>5</v>
+      </c>
+      <c r="D84" s="15">
+        <v>300</v>
+      </c>
+      <c r="F84">
+        <v>83</v>
+      </c>
     </row>
     <row r="85" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A85" s="20"/>
@@ -4760,32 +4868,47 @@
       <c r="B201" s="21"/>
       <c r="C201" s="22"/>
     </row>
+    <row r="202" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A202" s="20"/>
+      <c r="B202" s="21"/>
+      <c r="C202" s="22"/>
+    </row>
+    <row r="203" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A203" s="20"/>
+      <c r="B203" s="21"/>
+      <c r="C203" s="22"/>
+    </row>
+    <row r="204" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A204" s="20"/>
+      <c r="B204" s="21"/>
+      <c r="C204" s="22"/>
+    </row>
   </sheetData>
   <mergeCells count="4">
-    <mergeCell ref="A13:A15"/>
     <mergeCell ref="A16:A18"/>
-    <mergeCell ref="A22:A27"/>
-    <mergeCell ref="A28:A30"/>
+    <mergeCell ref="A19:A21"/>
+    <mergeCell ref="A25:A30"/>
+    <mergeCell ref="A31:A33"/>
   </mergeCells>
-  <dataValidations count="10">
+  <dataValidations count="13">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D7" xr:uid="{76366DFC-F994-4B24-8F58-3C475A37D29A}">
       <formula1>"annual, perennial"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D9" xr:uid="{FEC1871F-0B63-45CE-84E2-697ABFCCA571}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D12" xr:uid="{FEC1871F-0B63-45CE-84E2-697ABFCCA571}">
       <formula1>"Annual, Herbaceous perennial, Woody perennial"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D8" xr:uid="{BF09F0A8-DEDC-4564-B7AE-B6347D314DF5}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D11" xr:uid="{BF09F0A8-DEDC-4564-B7AE-B6347D314DF5}">
       <formula1>"C3, C4, CAM"</formula1>
     </dataValidation>
-    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D10:D12" xr:uid="{2135F1C0-D38D-4F5D-8EF7-81232862BF29}">
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D13:D15" xr:uid="{2135F1C0-D38D-4F5D-8EF7-81232862BF29}">
       <formula1>1</formula1>
       <formula2>366</formula2>
     </dataValidation>
-    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D19 D39:D42 D44:D47" xr:uid="{99673017-9BA7-4007-B122-EE6B62E8329F}">
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D22 D42:D45 D47:D50" xr:uid="{99673017-9BA7-4007-B122-EE6B62E8329F}">
       <formula1>0</formula1>
       <formula2>1</formula2>
     </dataValidation>
-    <dataValidation type="whole" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D43" xr:uid="{AD51276E-9E22-4C8A-A243-458D6265E1F0}">
+    <dataValidation type="whole" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D46" xr:uid="{AD51276E-9E22-4C8A-A243-458D6265E1F0}">
       <formula1>0</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D6" xr:uid="{9966BE53-3AF7-47D9-9DC3-79C6924CF42E}">
@@ -4795,12 +4918,22 @@
       <formula1>"monocot, dicot"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D4" xr:uid="{4695B65F-F242-4655-9983-F7931FCFC7A1}">
-      <formula1>"graminoid, forb/herb, shrub, tree, nonvascular"</formula1>
+      <formula1>"graminoid, forb_herb, shrub, tree"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D8" xr:uid="{0112A41A-9292-4030-8737-C126C38A2DAA}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D11" xr:uid="{0112A41A-9292-4030-8737-C126C38A2DAA}">
       <formula1>"C3, C4"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D8" xr:uid="{91D25E75-68D5-4C64-BABF-5FDC6B6EC5E0}">
+      <formula1>"evergreen, deciduous"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D9" xr:uid="{49CF716A-5412-4AD4-9944-2EC89E33B7C3}">
+      <formula1>"bunch, colonizing, multiple_stems, rhizomatous,single_crown,single_stem,stoloniferous,thicket_forming"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D10" xr:uid="{82D88EBD-3D9A-4158-A9B3-F883994282C6}">
+      <formula1>"climbing,columnar,conical,decumbent,erect,irregular,oval,prostrate,rounded,semi_erect,vase"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Updated class attribute and method names
</commit_message>
<xml_diff>
--- a/notebooks/GenVeg/GenVeg_Example_Simulation.xlsx
+++ b/notebooks/GenVeg/GenVeg_Example_Simulation.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Python\landlab\notebooks\GenVeg\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36748BE5-7A68-4415-B0BC-E113603454ED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49F768FB-C773-44C4-9A2C-22A8711447C4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{4FA2BB3E-4334-4C54-90D8-DFF869504B66}"/>
+    <workbookView xWindow="2745" yWindow="2745" windowWidth="21600" windowHeight="11385" xr2:uid="{4FA2BB3E-4334-4C54-90D8-DFF869504B66}"/>
   </bookViews>
   <sheets>
     <sheet name="Corn" sheetId="1" r:id="rId1"/>
@@ -92,9 +92,6 @@
   </si>
   <si>
     <t>Photosynthesis type</t>
-  </si>
-  <si>
-    <t>ptype</t>
   </si>
   <si>
     <t>Photosythesis variables</t>
@@ -556,6 +553,9 @@
   </si>
   <si>
     <t>Wheat</t>
+  </si>
+  <si>
+    <t>p_type</t>
   </si>
 </sst>
 </file>
@@ -1091,8 +1091,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{59430052-850A-4E52-8B29-0C7825B169C3}">
   <dimension ref="A1:G204"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D24" sqref="D24"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1142,7 +1142,7 @@
       </c>
       <c r="C3" s="11"/>
       <c r="D3" s="12" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="F3">
         <v>1</v>
@@ -1153,7 +1153,7 @@
         <v>8</v>
       </c>
       <c r="B4" s="10" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C4" s="11"/>
       <c r="D4" s="12" t="s">
@@ -1198,11 +1198,11 @@
         <v>17</v>
       </c>
       <c r="B7" s="10" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C7" s="11"/>
       <c r="D7" s="12" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="F7">
         <v>5</v>
@@ -1210,14 +1210,14 @@
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="9" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B8" s="10" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C8" s="11"/>
       <c r="D8" s="12" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="F8">
         <v>6</v>
@@ -1225,14 +1225,14 @@
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="9" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B9" s="10" t="s">
         <v>9</v>
       </c>
       <c r="C9" s="11"/>
       <c r="D9" s="12" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="F9">
         <v>7</v>
@@ -1240,14 +1240,14 @@
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="9" t="s">
+        <v>109</v>
+      </c>
+      <c r="B10" s="10" t="s">
         <v>110</v>
-      </c>
-      <c r="B10" s="10" t="s">
-        <v>111</v>
       </c>
       <c r="C10" s="11"/>
       <c r="D10" s="12" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="F10">
         <v>8</v>
@@ -1258,11 +1258,11 @@
         <v>18</v>
       </c>
       <c r="B11" s="10" t="s">
-        <v>19</v>
+        <v>119</v>
       </c>
       <c r="C11" s="11"/>
       <c r="D11" s="12" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="F11">
         <v>9</v>
@@ -1270,7 +1270,7 @@
     </row>
     <row r="12" spans="1:6" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A12" s="5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B12" s="6"/>
       <c r="C12" s="7"/>
@@ -1282,10 +1282,10 @@
     </row>
     <row r="13" spans="1:6" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A13" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="B13" s="10" t="s">
         <v>21</v>
-      </c>
-      <c r="B13" s="10" t="s">
-        <v>22</v>
       </c>
       <c r="C13" s="11"/>
       <c r="D13" s="15">
@@ -1297,10 +1297,10 @@
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="B14" s="10" t="s">
         <v>23</v>
-      </c>
-      <c r="B14" s="10" t="s">
-        <v>24</v>
       </c>
       <c r="C14" s="11"/>
       <c r="D14" s="15">
@@ -1312,10 +1312,10 @@
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="B15" s="10" t="s">
         <v>25</v>
-      </c>
-      <c r="B15" s="10" t="s">
-        <v>26</v>
       </c>
       <c r="C15" s="11"/>
       <c r="D15" s="15">
@@ -1327,13 +1327,13 @@
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="25" t="s">
+        <v>26</v>
+      </c>
+      <c r="B16" s="10" t="s">
+        <v>106</v>
+      </c>
+      <c r="C16" s="11" t="s">
         <v>27</v>
-      </c>
-      <c r="B16" s="10" t="s">
-        <v>107</v>
-      </c>
-      <c r="C16" s="11" t="s">
-        <v>28</v>
       </c>
       <c r="D16" s="15">
         <v>1.4999999999999999E-2</v>
@@ -1345,10 +1345,10 @@
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="25"/>
       <c r="B17" s="10" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C17" s="11" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D17" s="15">
         <v>1.4999999999999999E-2</v>
@@ -1360,10 +1360,10 @@
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" s="25"/>
       <c r="B18" s="10" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C18" s="11" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D18" s="15">
         <v>0.03</v>
@@ -1374,13 +1374,13 @@
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" s="25" t="s">
+        <v>30</v>
+      </c>
+      <c r="B19" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="B19" s="10" t="s">
-        <v>32</v>
-      </c>
       <c r="C19" s="11" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D19" s="15">
         <v>1.444</v>
@@ -1392,10 +1392,10 @@
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" s="25"/>
       <c r="B20" s="10" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C20" s="11" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D20" s="15">
         <v>1.5129999999999999</v>
@@ -1407,10 +1407,10 @@
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" s="25"/>
       <c r="B21" s="10" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C21" s="11" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D21" s="15">
         <v>1.4630000000000001</v>
@@ -1421,10 +1421,10 @@
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="B22" s="10" t="s">
         <v>33</v>
-      </c>
-      <c r="B22" s="10" t="s">
-        <v>34</v>
       </c>
       <c r="C22" s="11"/>
       <c r="D22" s="15">
@@ -1436,17 +1436,17 @@
     </row>
     <row r="23" spans="1:7" ht="32.25" x14ac:dyDescent="0.25">
       <c r="A23" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="B23" s="10" t="s">
         <v>35</v>
-      </c>
-      <c r="B23" s="10" t="s">
-        <v>36</v>
       </c>
       <c r="C23" s="11"/>
       <c r="D23" s="15">
         <v>100</v>
       </c>
       <c r="E23" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="F23">
         <v>21</v>
@@ -1454,10 +1454,10 @@
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="B24" s="10" t="s">
         <v>37</v>
-      </c>
-      <c r="B24" s="10" t="s">
-        <v>38</v>
       </c>
       <c r="C24" s="11"/>
       <c r="D24" s="15">
@@ -1469,32 +1469,32 @@
     </row>
     <row r="25" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A25" s="26" t="s">
+        <v>38</v>
+      </c>
+      <c r="B25" s="10" t="s">
         <v>39</v>
       </c>
-      <c r="B25" s="10" t="s">
+      <c r="C25" s="11" t="s">
         <v>40</v>
-      </c>
-      <c r="C25" s="11" t="s">
-        <v>41</v>
       </c>
       <c r="D25" s="15"/>
       <c r="E25" s="16" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F25">
         <v>23</v>
       </c>
       <c r="G25" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" s="26"/>
       <c r="B26" s="10" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C26" s="11" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D26" s="15"/>
       <c r="F26">
@@ -1504,10 +1504,10 @@
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" s="26"/>
       <c r="B27" s="10" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C27" s="11" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D27" s="15"/>
       <c r="F27">
@@ -1517,10 +1517,10 @@
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" s="26"/>
       <c r="B28" s="10" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C28" s="11" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D28" s="15"/>
       <c r="F28">
@@ -1530,10 +1530,10 @@
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" s="26"/>
       <c r="B29" s="10" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C29" s="11" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D29" s="15"/>
       <c r="F29">
@@ -1543,10 +1543,10 @@
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" s="26"/>
       <c r="B30" s="10" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C30" s="11" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D30" s="15"/>
       <c r="F30">
@@ -1555,13 +1555,13 @@
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" s="27" t="s">
+        <v>46</v>
+      </c>
+      <c r="B31" s="17" t="s">
         <v>47</v>
       </c>
-      <c r="B31" s="17" t="s">
-        <v>48</v>
-      </c>
       <c r="C31" s="18" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D31" s="15">
         <v>0.01</v>
@@ -1573,10 +1573,10 @@
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32" s="27"/>
       <c r="B32" s="17" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C32" s="18" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D32" s="15">
         <v>0.1</v>
@@ -1588,10 +1588,10 @@
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" s="27"/>
       <c r="B33" s="17" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C33" s="18" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D33" s="15">
         <v>0.5</v>
@@ -1602,7 +1602,7 @@
     </row>
     <row r="34" spans="1:6" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A34" s="5" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B34" s="6"/>
       <c r="C34" s="7"/>
@@ -1614,10 +1614,10 @@
     </row>
     <row r="35" spans="1:6" ht="18" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A35" s="19" t="s">
+        <v>49</v>
+      </c>
+      <c r="B35" s="17" t="s">
         <v>50</v>
-      </c>
-      <c r="B35" s="17" t="s">
-        <v>51</v>
       </c>
       <c r="C35" s="18"/>
       <c r="D35" s="15">
@@ -1629,10 +1629,10 @@
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36" s="19" t="s">
+        <v>51</v>
+      </c>
+      <c r="B36" s="17" t="s">
         <v>52</v>
-      </c>
-      <c r="B36" s="17" t="s">
-        <v>53</v>
       </c>
       <c r="C36" s="18"/>
       <c r="D36" s="15">
@@ -1644,10 +1644,10 @@
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37" s="19" t="s">
+        <v>53</v>
+      </c>
+      <c r="B37" s="17" t="s">
         <v>54</v>
-      </c>
-      <c r="B37" s="17" t="s">
-        <v>55</v>
       </c>
       <c r="C37" s="18"/>
       <c r="D37" s="15">
@@ -1659,10 +1659,10 @@
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38" s="19" t="s">
+        <v>55</v>
+      </c>
+      <c r="B38" s="17" t="s">
         <v>56</v>
-      </c>
-      <c r="B38" s="17" t="s">
-        <v>57</v>
       </c>
       <c r="C38" s="18"/>
       <c r="D38" s="15">
@@ -1674,10 +1674,10 @@
     </row>
     <row r="39" spans="1:6" ht="17.25" x14ac:dyDescent="0.25">
       <c r="A39" s="19" t="s">
+        <v>57</v>
+      </c>
+      <c r="B39" s="17" t="s">
         <v>58</v>
-      </c>
-      <c r="B39" s="17" t="s">
-        <v>59</v>
       </c>
       <c r="C39" s="18"/>
       <c r="D39" s="15">
@@ -1689,7 +1689,7 @@
     </row>
     <row r="40" spans="1:6" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A40" s="5" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B40" s="6"/>
       <c r="C40" s="7"/>
@@ -1701,10 +1701,10 @@
     </row>
     <row r="41" spans="1:6" ht="30.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A41" s="19" t="s">
+        <v>60</v>
+      </c>
+      <c r="B41" s="17" t="s">
         <v>61</v>
-      </c>
-      <c r="B41" s="17" t="s">
-        <v>62</v>
       </c>
       <c r="C41" s="18"/>
       <c r="D41" s="15">
@@ -1716,10 +1716,10 @@
     </row>
     <row r="42" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A42" s="19" t="s">
+        <v>62</v>
+      </c>
+      <c r="B42" s="17" t="s">
         <v>63</v>
-      </c>
-      <c r="B42" s="17" t="s">
-        <v>64</v>
       </c>
       <c r="C42" s="18"/>
       <c r="D42" s="15">
@@ -1731,10 +1731,10 @@
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A43" s="19" t="s">
+        <v>64</v>
+      </c>
+      <c r="B43" s="17" t="s">
         <v>65</v>
-      </c>
-      <c r="B43" s="17" t="s">
-        <v>66</v>
       </c>
       <c r="C43" s="18"/>
       <c r="D43" s="15">
@@ -1746,7 +1746,7 @@
     </row>
     <row r="44" spans="1:6" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A44" s="5" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B44" s="6"/>
       <c r="C44" s="7"/>
@@ -1758,10 +1758,10 @@
     </row>
     <row r="45" spans="1:6" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A45" s="19" t="s">
+        <v>67</v>
+      </c>
+      <c r="B45" s="17" t="s">
         <v>68</v>
-      </c>
-      <c r="B45" s="17" t="s">
-        <v>69</v>
       </c>
       <c r="C45" s="18"/>
       <c r="D45" s="15">
@@ -1773,10 +1773,10 @@
     </row>
     <row r="46" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A46" s="19" t="s">
+        <v>69</v>
+      </c>
+      <c r="B46" s="17" t="s">
         <v>70</v>
-      </c>
-      <c r="B46" s="17" t="s">
-        <v>71</v>
       </c>
       <c r="C46" s="18"/>
       <c r="D46" s="15">
@@ -1788,7 +1788,7 @@
     </row>
     <row r="47" spans="1:6" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A47" s="5" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B47" s="6"/>
       <c r="C47" s="7"/>
@@ -1800,17 +1800,17 @@
     </row>
     <row r="48" spans="1:6" ht="30.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A48" s="19" t="s">
+        <v>72</v>
+      </c>
+      <c r="B48" s="17" t="s">
         <v>73</v>
-      </c>
-      <c r="B48" s="17" t="s">
-        <v>74</v>
       </c>
       <c r="C48" s="18"/>
       <c r="D48" s="15">
         <v>0.25</v>
       </c>
       <c r="E48" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="F48">
         <v>46</v>
@@ -1818,10 +1818,10 @@
     </row>
     <row r="49" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A49" s="19" t="s">
+        <v>75</v>
+      </c>
+      <c r="B49" s="17" t="s">
         <v>76</v>
-      </c>
-      <c r="B49" s="17" t="s">
-        <v>77</v>
       </c>
       <c r="C49" s="18"/>
       <c r="D49" s="15">
@@ -1833,13 +1833,13 @@
     </row>
     <row r="50" spans="1:6" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A50" s="5" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B50" s="6"/>
       <c r="C50" s="7"/>
       <c r="D50" s="6"/>
       <c r="E50" s="8" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="F50">
         <v>48</v>
@@ -1847,17 +1847,17 @@
     </row>
     <row r="51" spans="1:6" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A51" s="19" t="s">
+        <v>79</v>
+      </c>
+      <c r="B51" s="17" t="s">
         <v>80</v>
-      </c>
-      <c r="B51" s="17" t="s">
-        <v>81</v>
       </c>
       <c r="C51" s="18"/>
       <c r="D51" s="12" t="s">
+        <v>81</v>
+      </c>
+      <c r="E51" t="s">
         <v>82</v>
-      </c>
-      <c r="E51" t="s">
-        <v>83</v>
       </c>
       <c r="F51">
         <v>49</v>
@@ -1865,10 +1865,10 @@
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A52" s="19" t="s">
+        <v>83</v>
+      </c>
+      <c r="B52" s="17" t="s">
         <v>84</v>
-      </c>
-      <c r="B52" s="17" t="s">
-        <v>85</v>
       </c>
       <c r="C52" s="18"/>
       <c r="D52" s="15">
@@ -1880,10 +1880,10 @@
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A53" s="19" t="s">
+        <v>85</v>
+      </c>
+      <c r="B53" s="17" t="s">
         <v>86</v>
-      </c>
-      <c r="B53" s="17" t="s">
-        <v>87</v>
       </c>
       <c r="C53" s="18">
         <v>1</v>
@@ -1898,7 +1898,7 @@
     <row r="54" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A54" s="19"/>
       <c r="B54" s="17" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C54" s="18">
         <v>2</v>
@@ -1913,7 +1913,7 @@
     <row r="55" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A55" s="19"/>
       <c r="B55" s="17" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C55" s="18">
         <v>3</v>
@@ -1928,7 +1928,7 @@
     <row r="56" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A56" s="19"/>
       <c r="B56" s="17" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C56" s="18">
         <v>4</v>
@@ -1941,7 +1941,7 @@
     <row r="57" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A57" s="19"/>
       <c r="B57" s="17" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C57" s="18">
         <v>5</v>
@@ -1953,10 +1953,10 @@
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A58" s="19" t="s">
+        <v>87</v>
+      </c>
+      <c r="B58" s="17" t="s">
         <v>88</v>
-      </c>
-      <c r="B58" s="17" t="s">
-        <v>89</v>
       </c>
       <c r="C58" s="18">
         <v>1</v>
@@ -1971,7 +1971,7 @@
     <row r="59" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A59" s="19"/>
       <c r="B59" s="17" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C59" s="18">
         <v>2</v>
@@ -1986,7 +1986,7 @@
     <row r="60" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A60" s="19"/>
       <c r="B60" s="17" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C60" s="18">
         <v>3</v>
@@ -2001,7 +2001,7 @@
     <row r="61" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A61" s="19"/>
       <c r="B61" s="17" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C61" s="18">
         <v>4</v>
@@ -2014,7 +2014,7 @@
     <row r="62" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A62" s="19"/>
       <c r="B62" s="17" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C62" s="18">
         <v>5</v>
@@ -2026,10 +2026,10 @@
     </row>
     <row r="63" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A63" s="19" t="s">
+        <v>89</v>
+      </c>
+      <c r="B63" s="17" t="s">
         <v>90</v>
-      </c>
-      <c r="B63" s="17" t="s">
-        <v>91</v>
       </c>
       <c r="C63" s="18">
         <v>1</v>
@@ -2044,7 +2044,7 @@
     <row r="64" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A64" s="19"/>
       <c r="B64" s="17" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C64" s="18">
         <v>2</v>
@@ -2059,7 +2059,7 @@
     <row r="65" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A65" s="19"/>
       <c r="B65" s="17" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C65" s="18">
         <v>3</v>
@@ -2074,7 +2074,7 @@
     <row r="66" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A66" s="19"/>
       <c r="B66" s="17" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C66" s="18">
         <v>4</v>
@@ -2087,7 +2087,7 @@
     <row r="67" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A67" s="19"/>
       <c r="B67" s="17" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C67" s="18">
         <v>5</v>
@@ -2099,14 +2099,14 @@
     </row>
     <row r="68" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A68" s="19" t="s">
+        <v>91</v>
+      </c>
+      <c r="B68" s="17" t="s">
         <v>92</v>
-      </c>
-      <c r="B68" s="17" t="s">
-        <v>93</v>
       </c>
       <c r="C68" s="18"/>
       <c r="D68" s="12" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="F68">
         <v>66</v>
@@ -2114,10 +2114,10 @@
     </row>
     <row r="69" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A69" s="19" t="s">
+        <v>94</v>
+      </c>
+      <c r="B69" s="17" t="s">
         <v>95</v>
-      </c>
-      <c r="B69" s="17" t="s">
-        <v>96</v>
       </c>
       <c r="C69" s="18"/>
       <c r="D69" s="15">
@@ -2129,10 +2129,10 @@
     </row>
     <row r="70" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A70" s="19" t="s">
+        <v>96</v>
+      </c>
+      <c r="B70" s="17" t="s">
         <v>97</v>
-      </c>
-      <c r="B70" s="17" t="s">
-        <v>98</v>
       </c>
       <c r="C70" s="18">
         <v>1</v>
@@ -2147,7 +2147,7 @@
     <row r="71" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A71" s="19"/>
       <c r="B71" s="17" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C71" s="18">
         <v>2</v>
@@ -2162,7 +2162,7 @@
     <row r="72" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A72" s="19"/>
       <c r="B72" s="17" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C72" s="18">
         <v>3</v>
@@ -2177,7 +2177,7 @@
     <row r="73" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A73" s="19"/>
       <c r="B73" s="17" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C73" s="18">
         <v>4</v>
@@ -2192,7 +2192,7 @@
     <row r="74" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A74" s="19"/>
       <c r="B74" s="17" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C74" s="18">
         <v>5</v>
@@ -2206,10 +2206,10 @@
     </row>
     <row r="75" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A75" s="19" t="s">
+        <v>98</v>
+      </c>
+      <c r="B75" s="17" t="s">
         <v>99</v>
-      </c>
-      <c r="B75" s="17" t="s">
-        <v>100</v>
       </c>
       <c r="C75" s="18">
         <v>1</v>
@@ -2224,7 +2224,7 @@
     <row r="76" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A76" s="19"/>
       <c r="B76" s="17" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C76" s="18">
         <v>2</v>
@@ -2239,7 +2239,7 @@
     <row r="77" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A77" s="19"/>
       <c r="B77" s="17" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C77" s="18">
         <v>3</v>
@@ -2254,7 +2254,7 @@
     <row r="78" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A78" s="19"/>
       <c r="B78" s="17" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C78" s="18">
         <v>4</v>
@@ -2269,7 +2269,7 @@
     <row r="79" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A79" s="19"/>
       <c r="B79" s="17" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C79" s="18">
         <v>5</v>
@@ -2283,10 +2283,10 @@
     </row>
     <row r="80" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A80" s="19" t="s">
+        <v>100</v>
+      </c>
+      <c r="B80" s="17" t="s">
         <v>101</v>
-      </c>
-      <c r="B80" s="17" t="s">
-        <v>102</v>
       </c>
       <c r="C80" s="18">
         <v>1</v>
@@ -2301,7 +2301,7 @@
     <row r="81" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A81" s="19"/>
       <c r="B81" s="17" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C81" s="18">
         <v>2</v>
@@ -2316,7 +2316,7 @@
     <row r="82" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A82" s="19"/>
       <c r="B82" s="17" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C82" s="18">
         <v>3</v>
@@ -2331,7 +2331,7 @@
     <row r="83" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A83" s="19"/>
       <c r="B83" s="17" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C83" s="18">
         <v>4</v>
@@ -2346,7 +2346,7 @@
     <row r="84" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A84" s="19"/>
       <c r="B84" s="17" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C84" s="18">
         <v>5</v>
@@ -3013,8 +3013,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7A5B2ED1-E60A-481E-A183-520033C5AF7F}">
   <dimension ref="A1:G204"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="E30" sqref="E30"/>
+    <sheetView topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3067,7 +3067,7 @@
       </c>
       <c r="C3" s="11"/>
       <c r="D3" s="12" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="F3">
         <v>2</v>
@@ -3078,7 +3078,7 @@
         <v>8</v>
       </c>
       <c r="B4" s="10" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C4" s="11"/>
       <c r="D4" s="12" t="s">
@@ -3123,11 +3123,11 @@
         <v>17</v>
       </c>
       <c r="B7" s="10" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C7" s="11"/>
       <c r="D7" s="12" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="F7">
         <v>6</v>
@@ -3135,14 +3135,14 @@
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="9" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B8" s="10" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C8" s="11"/>
       <c r="D8" s="12" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="F8">
         <v>7</v>
@@ -3150,14 +3150,14 @@
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="9" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B9" s="10" t="s">
         <v>9</v>
       </c>
       <c r="C9" s="11"/>
       <c r="D9" s="12" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="F9">
         <v>8</v>
@@ -3165,14 +3165,14 @@
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="9" t="s">
+        <v>109</v>
+      </c>
+      <c r="B10" s="10" t="s">
         <v>110</v>
-      </c>
-      <c r="B10" s="10" t="s">
-        <v>111</v>
       </c>
       <c r="C10" s="11"/>
       <c r="D10" s="12" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="F10">
         <v>9</v>
@@ -3183,11 +3183,11 @@
         <v>18</v>
       </c>
       <c r="B11" s="10" t="s">
-        <v>19</v>
+        <v>119</v>
       </c>
       <c r="C11" s="11"/>
       <c r="D11" s="12" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="F11">
         <v>10</v>
@@ -3195,7 +3195,7 @@
     </row>
     <row r="12" spans="1:6" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A12" s="5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B12" s="6"/>
       <c r="C12" s="7"/>
@@ -3207,10 +3207,10 @@
     </row>
     <row r="13" spans="1:6" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A13" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="B13" s="10" t="s">
         <v>21</v>
-      </c>
-      <c r="B13" s="10" t="s">
-        <v>22</v>
       </c>
       <c r="C13" s="11"/>
       <c r="D13" s="15">
@@ -3222,10 +3222,10 @@
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="B14" s="10" t="s">
         <v>23</v>
-      </c>
-      <c r="B14" s="10" t="s">
-        <v>24</v>
       </c>
       <c r="C14" s="11"/>
       <c r="D14" s="15">
@@ -3237,10 +3237,10 @@
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="B15" s="10" t="s">
         <v>25</v>
-      </c>
-      <c r="B15" s="10" t="s">
-        <v>26</v>
       </c>
       <c r="C15" s="11"/>
       <c r="D15" s="15">
@@ -3252,13 +3252,13 @@
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="25" t="s">
+        <v>26</v>
+      </c>
+      <c r="B16" s="10" t="s">
+        <v>106</v>
+      </c>
+      <c r="C16" s="11" t="s">
         <v>27</v>
-      </c>
-      <c r="B16" s="10" t="s">
-        <v>107</v>
-      </c>
-      <c r="C16" s="11" t="s">
-        <v>28</v>
       </c>
       <c r="D16" s="15">
         <v>1.4999999999999999E-2</v>
@@ -3270,10 +3270,10 @@
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="25"/>
       <c r="B17" s="10" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C17" s="11" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D17" s="15">
         <v>1.4999999999999999E-2</v>
@@ -3285,10 +3285,10 @@
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" s="25"/>
       <c r="B18" s="10" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C18" s="11" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D18" s="15">
         <v>0.03</v>
@@ -3299,13 +3299,13 @@
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" s="25" t="s">
+        <v>30</v>
+      </c>
+      <c r="B19" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="B19" s="10" t="s">
-        <v>32</v>
-      </c>
       <c r="C19" s="11" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D19" s="15">
         <v>1.444</v>
@@ -3317,10 +3317,10 @@
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" s="25"/>
       <c r="B20" s="10" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C20" s="11" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D20" s="15">
         <v>1.5129999999999999</v>
@@ -3332,10 +3332,10 @@
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" s="25"/>
       <c r="B21" s="10" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C21" s="11" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D21" s="15">
         <v>1.4630000000000001</v>
@@ -3346,10 +3346,10 @@
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="B22" s="10" t="s">
         <v>33</v>
-      </c>
-      <c r="B22" s="10" t="s">
-        <v>34</v>
       </c>
       <c r="C22" s="11"/>
       <c r="D22" s="15">
@@ -3361,17 +3361,17 @@
     </row>
     <row r="23" spans="1:7" ht="32.25" x14ac:dyDescent="0.25">
       <c r="A23" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="B23" s="10" t="s">
         <v>35</v>
-      </c>
-      <c r="B23" s="10" t="s">
-        <v>36</v>
       </c>
       <c r="C23" s="11"/>
       <c r="D23" s="15">
         <v>100</v>
       </c>
       <c r="E23" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="F23">
         <v>22</v>
@@ -3379,10 +3379,10 @@
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="B24" s="10" t="s">
         <v>37</v>
-      </c>
-      <c r="B24" s="10" t="s">
-        <v>38</v>
       </c>
       <c r="C24" s="11"/>
       <c r="D24" s="15">
@@ -3394,32 +3394,32 @@
     </row>
     <row r="25" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A25" s="26" t="s">
+        <v>38</v>
+      </c>
+      <c r="B25" s="10" t="s">
         <v>39</v>
       </c>
-      <c r="B25" s="10" t="s">
+      <c r="C25" s="11" t="s">
         <v>40</v>
-      </c>
-      <c r="C25" s="11" t="s">
-        <v>41</v>
       </c>
       <c r="D25" s="15"/>
       <c r="E25" s="16" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F25">
         <v>24</v>
       </c>
       <c r="G25" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" s="26"/>
       <c r="B26" s="10" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C26" s="11" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D26" s="15"/>
       <c r="F26">
@@ -3429,10 +3429,10 @@
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" s="26"/>
       <c r="B27" s="10" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C27" s="11" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D27" s="15"/>
       <c r="F27">
@@ -3442,10 +3442,10 @@
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" s="26"/>
       <c r="B28" s="10" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C28" s="11" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D28" s="15"/>
       <c r="F28">
@@ -3455,10 +3455,10 @@
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" s="26"/>
       <c r="B29" s="10" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C29" s="11" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D29" s="15"/>
       <c r="F29">
@@ -3468,10 +3468,10 @@
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" s="26"/>
       <c r="B30" s="10" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C30" s="11" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D30" s="15"/>
       <c r="F30">
@@ -3480,13 +3480,13 @@
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" s="27" t="s">
+        <v>46</v>
+      </c>
+      <c r="B31" s="17" t="s">
         <v>47</v>
       </c>
-      <c r="B31" s="17" t="s">
-        <v>48</v>
-      </c>
       <c r="C31" s="18" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D31" s="15">
         <v>0.01</v>
@@ -3498,10 +3498,10 @@
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32" s="27"/>
       <c r="B32" s="17" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C32" s="18" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D32" s="15">
         <v>0.1</v>
@@ -3513,10 +3513,10 @@
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" s="27"/>
       <c r="B33" s="17" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C33" s="18" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D33" s="15">
         <v>0.5</v>
@@ -3527,7 +3527,7 @@
     </row>
     <row r="34" spans="1:6" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A34" s="5" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B34" s="6"/>
       <c r="C34" s="7"/>
@@ -3539,10 +3539,10 @@
     </row>
     <row r="35" spans="1:6" ht="18" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A35" s="19" t="s">
+        <v>49</v>
+      </c>
+      <c r="B35" s="17" t="s">
         <v>50</v>
-      </c>
-      <c r="B35" s="17" t="s">
-        <v>51</v>
       </c>
       <c r="C35" s="18"/>
       <c r="D35" s="15">
@@ -3554,10 +3554,10 @@
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36" s="19" t="s">
+        <v>51</v>
+      </c>
+      <c r="B36" s="17" t="s">
         <v>52</v>
-      </c>
-      <c r="B36" s="17" t="s">
-        <v>53</v>
       </c>
       <c r="C36" s="18"/>
       <c r="D36" s="15">
@@ -3569,10 +3569,10 @@
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37" s="19" t="s">
+        <v>53</v>
+      </c>
+      <c r="B37" s="17" t="s">
         <v>54</v>
-      </c>
-      <c r="B37" s="17" t="s">
-        <v>55</v>
       </c>
       <c r="C37" s="18"/>
       <c r="D37" s="15">
@@ -3584,10 +3584,10 @@
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38" s="19" t="s">
+        <v>55</v>
+      </c>
+      <c r="B38" s="17" t="s">
         <v>56</v>
-      </c>
-      <c r="B38" s="17" t="s">
-        <v>57</v>
       </c>
       <c r="C38" s="18"/>
       <c r="D38" s="15">
@@ -3599,10 +3599,10 @@
     </row>
     <row r="39" spans="1:6" ht="17.25" x14ac:dyDescent="0.25">
       <c r="A39" s="19" t="s">
+        <v>57</v>
+      </c>
+      <c r="B39" s="17" t="s">
         <v>58</v>
-      </c>
-      <c r="B39" s="17" t="s">
-        <v>59</v>
       </c>
       <c r="C39" s="18"/>
       <c r="D39" s="15">
@@ -3614,7 +3614,7 @@
     </row>
     <row r="40" spans="1:6" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A40" s="5" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B40" s="6"/>
       <c r="C40" s="7"/>
@@ -3626,10 +3626,10 @@
     </row>
     <row r="41" spans="1:6" ht="30.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A41" s="19" t="s">
+        <v>60</v>
+      </c>
+      <c r="B41" s="17" t="s">
         <v>61</v>
-      </c>
-      <c r="B41" s="17" t="s">
-        <v>62</v>
       </c>
       <c r="C41" s="18"/>
       <c r="D41" s="15">
@@ -3641,10 +3641,10 @@
     </row>
     <row r="42" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A42" s="19" t="s">
+        <v>62</v>
+      </c>
+      <c r="B42" s="17" t="s">
         <v>63</v>
-      </c>
-      <c r="B42" s="17" t="s">
-        <v>64</v>
       </c>
       <c r="C42" s="18"/>
       <c r="D42" s="15">
@@ -3656,10 +3656,10 @@
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A43" s="19" t="s">
+        <v>64</v>
+      </c>
+      <c r="B43" s="17" t="s">
         <v>65</v>
-      </c>
-      <c r="B43" s="17" t="s">
-        <v>66</v>
       </c>
       <c r="C43" s="18"/>
       <c r="D43" s="15">
@@ -3671,7 +3671,7 @@
     </row>
     <row r="44" spans="1:6" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A44" s="5" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B44" s="6"/>
       <c r="C44" s="7"/>
@@ -3683,10 +3683,10 @@
     </row>
     <row r="45" spans="1:6" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A45" s="19" t="s">
+        <v>67</v>
+      </c>
+      <c r="B45" s="17" t="s">
         <v>68</v>
-      </c>
-      <c r="B45" s="17" t="s">
-        <v>69</v>
       </c>
       <c r="C45" s="18"/>
       <c r="D45" s="15">
@@ -3698,10 +3698,10 @@
     </row>
     <row r="46" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A46" s="19" t="s">
+        <v>69</v>
+      </c>
+      <c r="B46" s="17" t="s">
         <v>70</v>
-      </c>
-      <c r="B46" s="17" t="s">
-        <v>71</v>
       </c>
       <c r="C46" s="18"/>
       <c r="D46" s="15">
@@ -3713,7 +3713,7 @@
     </row>
     <row r="47" spans="1:6" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A47" s="5" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B47" s="6"/>
       <c r="C47" s="7"/>
@@ -3725,17 +3725,17 @@
     </row>
     <row r="48" spans="1:6" ht="30.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A48" s="19" t="s">
+        <v>72</v>
+      </c>
+      <c r="B48" s="17" t="s">
         <v>73</v>
-      </c>
-      <c r="B48" s="17" t="s">
-        <v>74</v>
       </c>
       <c r="C48" s="18"/>
       <c r="D48" s="15">
         <v>0.25</v>
       </c>
       <c r="E48" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="F48">
         <v>47</v>
@@ -3743,10 +3743,10 @@
     </row>
     <row r="49" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A49" s="19" t="s">
+        <v>75</v>
+      </c>
+      <c r="B49" s="17" t="s">
         <v>76</v>
-      </c>
-      <c r="B49" s="17" t="s">
-        <v>77</v>
       </c>
       <c r="C49" s="18"/>
       <c r="D49" s="15">
@@ -3758,13 +3758,13 @@
     </row>
     <row r="50" spans="1:6" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A50" s="5" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B50" s="6"/>
       <c r="C50" s="7"/>
       <c r="D50" s="6"/>
       <c r="E50" s="8" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="F50">
         <v>49</v>
@@ -3772,17 +3772,17 @@
     </row>
     <row r="51" spans="1:6" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A51" s="19" t="s">
+        <v>79</v>
+      </c>
+      <c r="B51" s="17" t="s">
         <v>80</v>
-      </c>
-      <c r="B51" s="17" t="s">
-        <v>81</v>
       </c>
       <c r="C51" s="18"/>
       <c r="D51" s="12" t="s">
+        <v>81</v>
+      </c>
+      <c r="E51" t="s">
         <v>82</v>
-      </c>
-      <c r="E51" t="s">
-        <v>83</v>
       </c>
       <c r="F51">
         <v>50</v>
@@ -3790,10 +3790,10 @@
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A52" s="19" t="s">
+        <v>83</v>
+      </c>
+      <c r="B52" s="17" t="s">
         <v>84</v>
-      </c>
-      <c r="B52" s="17" t="s">
-        <v>85</v>
       </c>
       <c r="C52" s="18"/>
       <c r="D52" s="15">
@@ -3805,10 +3805,10 @@
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A53" s="19" t="s">
+        <v>85</v>
+      </c>
+      <c r="B53" s="17" t="s">
         <v>86</v>
-      </c>
-      <c r="B53" s="17" t="s">
-        <v>87</v>
       </c>
       <c r="C53" s="18">
         <v>1</v>
@@ -3823,7 +3823,7 @@
     <row r="54" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A54" s="19"/>
       <c r="B54" s="17" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C54" s="18">
         <v>2</v>
@@ -3838,7 +3838,7 @@
     <row r="55" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A55" s="19"/>
       <c r="B55" s="17" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C55" s="18">
         <v>3</v>
@@ -3853,7 +3853,7 @@
     <row r="56" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A56" s="19"/>
       <c r="B56" s="17" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C56" s="18">
         <v>4</v>
@@ -3866,7 +3866,7 @@
     <row r="57" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A57" s="19"/>
       <c r="B57" s="17" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C57" s="18">
         <v>5</v>
@@ -3878,10 +3878,10 @@
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A58" s="19" t="s">
+        <v>87</v>
+      </c>
+      <c r="B58" s="17" t="s">
         <v>88</v>
-      </c>
-      <c r="B58" s="17" t="s">
-        <v>89</v>
       </c>
       <c r="C58" s="18">
         <v>1</v>
@@ -3896,7 +3896,7 @@
     <row r="59" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A59" s="19"/>
       <c r="B59" s="17" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C59" s="18">
         <v>2</v>
@@ -3911,7 +3911,7 @@
     <row r="60" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A60" s="19"/>
       <c r="B60" s="17" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C60" s="18">
         <v>3</v>
@@ -3926,7 +3926,7 @@
     <row r="61" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A61" s="19"/>
       <c r="B61" s="17" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C61" s="18">
         <v>4</v>
@@ -3939,7 +3939,7 @@
     <row r="62" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A62" s="19"/>
       <c r="B62" s="17" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C62" s="18">
         <v>5</v>
@@ -3951,10 +3951,10 @@
     </row>
     <row r="63" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A63" s="19" t="s">
+        <v>89</v>
+      </c>
+      <c r="B63" s="17" t="s">
         <v>90</v>
-      </c>
-      <c r="B63" s="17" t="s">
-        <v>91</v>
       </c>
       <c r="C63" s="18">
         <v>1</v>
@@ -3969,7 +3969,7 @@
     <row r="64" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A64" s="19"/>
       <c r="B64" s="17" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C64" s="18">
         <v>2</v>
@@ -3984,7 +3984,7 @@
     <row r="65" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A65" s="19"/>
       <c r="B65" s="17" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C65" s="18">
         <v>3</v>
@@ -3999,7 +3999,7 @@
     <row r="66" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A66" s="19"/>
       <c r="B66" s="17" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C66" s="18">
         <v>4</v>
@@ -4012,7 +4012,7 @@
     <row r="67" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A67" s="19"/>
       <c r="B67" s="17" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C67" s="18">
         <v>5</v>
@@ -4024,14 +4024,14 @@
     </row>
     <row r="68" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A68" s="19" t="s">
+        <v>91</v>
+      </c>
+      <c r="B68" s="17" t="s">
         <v>92</v>
-      </c>
-      <c r="B68" s="17" t="s">
-        <v>93</v>
       </c>
       <c r="C68" s="18"/>
       <c r="D68" s="12" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="F68">
         <v>67</v>
@@ -4039,10 +4039,10 @@
     </row>
     <row r="69" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A69" s="19" t="s">
+        <v>94</v>
+      </c>
+      <c r="B69" s="17" t="s">
         <v>95</v>
-      </c>
-      <c r="B69" s="17" t="s">
-        <v>96</v>
       </c>
       <c r="C69" s="18"/>
       <c r="D69" s="15">
@@ -4054,10 +4054,10 @@
     </row>
     <row r="70" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A70" s="19" t="s">
+        <v>96</v>
+      </c>
+      <c r="B70" s="17" t="s">
         <v>97</v>
-      </c>
-      <c r="B70" s="17" t="s">
-        <v>98</v>
       </c>
       <c r="C70" s="18">
         <v>1</v>
@@ -4072,7 +4072,7 @@
     <row r="71" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A71" s="19"/>
       <c r="B71" s="17" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C71" s="18">
         <v>2</v>
@@ -4087,7 +4087,7 @@
     <row r="72" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A72" s="19"/>
       <c r="B72" s="17" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C72" s="18">
         <v>3</v>
@@ -4102,7 +4102,7 @@
     <row r="73" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A73" s="19"/>
       <c r="B73" s="17" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C73" s="18">
         <v>4</v>
@@ -4117,7 +4117,7 @@
     <row r="74" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A74" s="19"/>
       <c r="B74" s="17" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C74" s="18">
         <v>5</v>
@@ -4131,10 +4131,10 @@
     </row>
     <row r="75" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A75" s="19" t="s">
+        <v>98</v>
+      </c>
+      <c r="B75" s="17" t="s">
         <v>99</v>
-      </c>
-      <c r="B75" s="17" t="s">
-        <v>100</v>
       </c>
       <c r="C75" s="18">
         <v>1</v>
@@ -4149,7 +4149,7 @@
     <row r="76" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A76" s="19"/>
       <c r="B76" s="17" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C76" s="18">
         <v>2</v>
@@ -4164,7 +4164,7 @@
     <row r="77" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A77" s="19"/>
       <c r="B77" s="17" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C77" s="18">
         <v>3</v>
@@ -4179,7 +4179,7 @@
     <row r="78" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A78" s="19"/>
       <c r="B78" s="17" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C78" s="18">
         <v>4</v>
@@ -4194,7 +4194,7 @@
     <row r="79" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A79" s="19"/>
       <c r="B79" s="17" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C79" s="18">
         <v>5</v>
@@ -4208,10 +4208,10 @@
     </row>
     <row r="80" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A80" s="19" t="s">
+        <v>100</v>
+      </c>
+      <c r="B80" s="17" t="s">
         <v>101</v>
-      </c>
-      <c r="B80" s="17" t="s">
-        <v>102</v>
       </c>
       <c r="C80" s="18">
         <v>1</v>
@@ -4226,7 +4226,7 @@
     <row r="81" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A81" s="19"/>
       <c r="B81" s="17" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C81" s="18">
         <v>2</v>
@@ -4241,7 +4241,7 @@
     <row r="82" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A82" s="19"/>
       <c r="B82" s="17" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C82" s="18">
         <v>3</v>
@@ -4256,7 +4256,7 @@
     <row r="83" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A83" s="19"/>
       <c r="B83" s="17" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C83" s="18">
         <v>4</v>
@@ -4271,7 +4271,7 @@
     <row r="84" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A84" s="19"/>
       <c r="B84" s="17" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C84" s="18">
         <v>5</v>

</xml_diff>

<commit_message>
Implemented storage/repro biomass, size checks
</commit_message>
<xml_diff>
--- a/notebooks/GenVeg/GenVeg_Example_Simulation.xlsx
+++ b/notebooks/GenVeg/GenVeg_Example_Simulation.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25601"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Python\landlab\notebooks\GenVeg\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49F768FB-C773-44C4-9A2C-22A8711447C4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A69C6B99-D6C7-42DA-B9DC-D9A4C803A581}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2745" yWindow="2745" windowWidth="21600" windowHeight="11385" xr2:uid="{4FA2BB3E-4334-4C54-90D8-DFF869504B66}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{4FA2BB3E-4334-4C54-90D8-DFF869504B66}"/>
   </bookViews>
   <sheets>
     <sheet name="Corn" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="322" uniqueCount="120">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="360" uniqueCount="123">
   <si>
     <t>Parameter</t>
   </si>
@@ -375,27 +375,15 @@
     <t>total_cs_area_stems</t>
   </si>
   <si>
-    <t>Dispersion</t>
-  </si>
-  <si>
     <t>Growing season maximum dispersion distance (m)</t>
   </si>
   <si>
-    <t>max_dist_dispersion</t>
-  </si>
-  <si>
     <t>Minimum plant size for dispersion (proportion of maximum)</t>
   </si>
   <si>
-    <t>min_size_dispersion</t>
-  </si>
-  <si>
     <t>Dispersion carbohydrate cost (g)</t>
   </si>
   <si>
-    <t>carb_cost_dispersion</t>
-  </si>
-  <si>
     <t>Colonization</t>
   </si>
   <si>
@@ -411,151 +399,172 @@
     <t>time_to_colonization</t>
   </si>
   <si>
+    <t>Mortality and survival</t>
+  </si>
+  <si>
+    <t>*This will need to be updated so the user identifies if this is a mortality factor or a growth factor</t>
+  </si>
+  <si>
+    <t>Survival factor 1 name</t>
+  </si>
+  <si>
+    <t>mort_factor_1</t>
+  </si>
+  <si>
+    <t>Distance to shore</t>
+  </si>
+  <si>
+    <t>*Not sure if we should allow user to provide manual weighting for fit function or if we should force it in the code</t>
+  </si>
+  <si>
+    <t>Survival factor 1 time (days)</t>
+  </si>
+  <si>
+    <t>mort_factor_1_duration</t>
+  </si>
+  <si>
+    <t>Survival factor 1 predictor</t>
+  </si>
+  <si>
+    <t>mort_factor_1_predictor</t>
+  </si>
+  <si>
+    <t>Survival factor 1 survival rates (0-1)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">mort_factor_1_response </t>
+  </si>
+  <si>
+    <t>Survival factor 1 survival weights (0-1000)</t>
+  </si>
+  <si>
+    <t>mort_factor_1_weight</t>
+  </si>
+  <si>
+    <t>Survival factor 2 name</t>
+  </si>
+  <si>
+    <t>mort_factor_2</t>
+  </si>
+  <si>
+    <t>Minimum elevation</t>
+  </si>
+  <si>
+    <t>Survival factor 2 time (days)</t>
+  </si>
+  <si>
+    <t>mort_factor_2_duration</t>
+  </si>
+  <si>
+    <t>Survival factor 2 predictor</t>
+  </si>
+  <si>
+    <t>mort_factor_2_predictor</t>
+  </si>
+  <si>
+    <t>Survival factor 2 survival rates (0-1)</t>
+  </si>
+  <si>
+    <t>mort_factor_2_response</t>
+  </si>
+  <si>
+    <t>Survival factor 2 survival weights (0-1000)</t>
+  </si>
+  <si>
+    <t>mort_factor_2_weight</t>
+  </si>
+  <si>
+    <t>Corn</t>
+  </si>
+  <si>
+    <t>annual</t>
+  </si>
+  <si>
+    <t>C4</t>
+  </si>
+  <si>
+    <t>per file:///C:/Users/RDEL1CMC/Downloads/Charisma-a_simulation_model_of_the_dynamics_of_submerged_plants.PDF.pdf</t>
+  </si>
+  <si>
+    <t>respiration_coefficient</t>
+  </si>
+  <si>
+    <t>Leaf retention</t>
+  </si>
+  <si>
+    <t>Growth form</t>
+  </si>
+  <si>
+    <t>Shape and orientation</t>
+  </si>
+  <si>
+    <t>shape</t>
+  </si>
+  <si>
+    <t>deciduous</t>
+  </si>
+  <si>
+    <t>single_stem</t>
+  </si>
+  <si>
+    <t>erect</t>
+  </si>
+  <si>
+    <t>bunch</t>
+  </si>
+  <si>
+    <t>duration</t>
+  </si>
+  <si>
+    <t>growth_habit</t>
+  </si>
+  <si>
+    <t>leaf_retention</t>
+  </si>
+  <si>
+    <t>Wheat</t>
+  </si>
+  <si>
+    <t>p_type</t>
+  </si>
+  <si>
+    <t>Maximum mass (g)</t>
+  </si>
+  <si>
+    <t>plant_part_max</t>
+  </si>
+  <si>
+    <t>perennial</t>
+  </si>
+  <si>
+    <t>C3</t>
+  </si>
+  <si>
     <t>Storage</t>
   </si>
   <si>
-    <t>Winter dieoff (proportion of root loss for winter)</t>
-  </si>
-  <si>
-    <t>wint_dieoff_roots</t>
-  </si>
-  <si>
-    <t>*Should we look at this daily? I could foresee this changing as emergence dates change with rising temperatures</t>
-  </si>
-  <si>
-    <t>Winter storage (proportion of biomass to send to roots for winter)</t>
-  </si>
-  <si>
-    <t>wint_store_to_roots</t>
-  </si>
-  <si>
-    <t>Mortality and survival</t>
-  </si>
-  <si>
-    <t>*This will need to be updated so the user identifies if this is a mortality factor or a growth factor</t>
-  </si>
-  <si>
-    <t>Survival factor 1 name</t>
-  </si>
-  <si>
-    <t>mort_factor_1</t>
-  </si>
-  <si>
-    <t>Distance to shore</t>
-  </si>
-  <si>
-    <t>*Not sure if we should allow user to provide manual weighting for fit function or if we should force it in the code</t>
-  </si>
-  <si>
-    <t>Survival factor 1 time (days)</t>
-  </si>
-  <si>
-    <t>mort_factor_1_duration</t>
-  </si>
-  <si>
-    <t>Survival factor 1 predictor</t>
-  </si>
-  <si>
-    <t>mort_factor_1_predictor</t>
-  </si>
-  <si>
-    <t>Survival factor 1 survival rates (0-1)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">mort_factor_1_response </t>
-  </si>
-  <si>
-    <t>Survival factor 1 survival weights (0-1000)</t>
-  </si>
-  <si>
-    <t>mort_factor_1_weight</t>
-  </si>
-  <si>
-    <t>Survival factor 2 name</t>
-  </si>
-  <si>
-    <t>mort_factor_2</t>
-  </si>
-  <si>
-    <t>Minimum elevation</t>
-  </si>
-  <si>
-    <t>Survival factor 2 time (days)</t>
-  </si>
-  <si>
-    <t>mort_factor_2_duration</t>
-  </si>
-  <si>
-    <t>Survival factor 2 predictor</t>
-  </si>
-  <si>
-    <t>mort_factor_2_predictor</t>
-  </si>
-  <si>
-    <t>Survival factor 2 survival rates (0-1)</t>
-  </si>
-  <si>
-    <t>mort_factor_2_response</t>
-  </si>
-  <si>
-    <t>Survival factor 2 survival weights (0-1000)</t>
-  </si>
-  <si>
-    <t>mort_factor_2_weight</t>
-  </si>
-  <si>
-    <t>Corn</t>
-  </si>
-  <si>
-    <t>annual</t>
-  </si>
-  <si>
-    <t>C4</t>
-  </si>
-  <si>
-    <t>per file:///C:/Users/RDEL1CMC/Downloads/Charisma-a_simulation_model_of_the_dynamics_of_submerged_plants.PDF.pdf</t>
-  </si>
-  <si>
-    <t>respiration_coefficient</t>
-  </si>
-  <si>
-    <t>Leaf retention</t>
-  </si>
-  <si>
-    <t>Growth form</t>
-  </si>
-  <si>
-    <t>Shape and orientation</t>
-  </si>
-  <si>
-    <t>shape</t>
-  </si>
-  <si>
-    <t>deciduous</t>
-  </si>
-  <si>
-    <t>single_stem</t>
-  </si>
-  <si>
-    <t>erect</t>
-  </si>
-  <si>
-    <t>bunch</t>
-  </si>
-  <si>
-    <t>duration</t>
-  </si>
-  <si>
-    <t>growth_habit</t>
-  </si>
-  <si>
-    <t>leaf_retention</t>
-  </si>
-  <si>
-    <t>Wheat</t>
-  </si>
-  <si>
-    <t>p_type</t>
+    <t>Reproductive</t>
+  </si>
+  <si>
+    <t>Dispersal</t>
+  </si>
+  <si>
+    <t>Reproduction period begins (day-of-year)</t>
+  </si>
+  <si>
+    <t>reproduction_start</t>
+  </si>
+  <si>
+    <t>Dispesal</t>
+  </si>
+  <si>
+    <t>max_dist_dispersal</t>
+  </si>
+  <si>
+    <t>min_size_dispersal</t>
+  </si>
+  <si>
+    <t>carb_cost_dispersal</t>
   </si>
 </sst>
 </file>
@@ -693,7 +702,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -762,6 +771,12 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="3" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="3" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -1089,10 +1104,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{59430052-850A-4E52-8B29-0C7825B169C3}">
-  <dimension ref="A1:G204"/>
+  <dimension ref="A1:G213"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+    <sheetView topLeftCell="A32" workbookViewId="0">
+      <selection activeCell="B44" sqref="B44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1142,7 +1157,7 @@
       </c>
       <c r="C3" s="11"/>
       <c r="D3" s="12" t="s">
-        <v>102</v>
+        <v>92</v>
       </c>
       <c r="F3">
         <v>1</v>
@@ -1153,7 +1168,7 @@
         <v>8</v>
       </c>
       <c r="B4" s="10" t="s">
-        <v>116</v>
+        <v>106</v>
       </c>
       <c r="C4" s="11"/>
       <c r="D4" s="12" t="s">
@@ -1198,11 +1213,11 @@
         <v>17</v>
       </c>
       <c r="B7" s="10" t="s">
-        <v>115</v>
+        <v>105</v>
       </c>
       <c r="C7" s="11"/>
       <c r="D7" s="12" t="s">
-        <v>103</v>
+        <v>93</v>
       </c>
       <c r="F7">
         <v>5</v>
@@ -1210,14 +1225,14 @@
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="9" t="s">
+        <v>97</v>
+      </c>
+      <c r="B8" s="10" t="s">
         <v>107</v>
-      </c>
-      <c r="B8" s="10" t="s">
-        <v>117</v>
       </c>
       <c r="C8" s="11"/>
       <c r="D8" s="12" t="s">
-        <v>111</v>
+        <v>101</v>
       </c>
       <c r="F8">
         <v>6</v>
@@ -1225,14 +1240,14 @@
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="9" t="s">
-        <v>108</v>
+        <v>98</v>
       </c>
       <c r="B9" s="10" t="s">
         <v>9</v>
       </c>
       <c r="C9" s="11"/>
       <c r="D9" s="12" t="s">
-        <v>112</v>
+        <v>102</v>
       </c>
       <c r="F9">
         <v>7</v>
@@ -1240,14 +1255,14 @@
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="9" t="s">
-        <v>109</v>
+        <v>99</v>
       </c>
       <c r="B10" s="10" t="s">
-        <v>110</v>
+        <v>100</v>
       </c>
       <c r="C10" s="11"/>
       <c r="D10" s="12" t="s">
-        <v>113</v>
+        <v>103</v>
       </c>
       <c r="F10">
         <v>8</v>
@@ -1258,11 +1273,11 @@
         <v>18</v>
       </c>
       <c r="B11" s="10" t="s">
-        <v>119</v>
+        <v>109</v>
       </c>
       <c r="C11" s="11"/>
       <c r="D11" s="12" t="s">
-        <v>104</v>
+        <v>94</v>
       </c>
       <c r="F11">
         <v>9</v>
@@ -1326,11 +1341,11 @@
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A16" s="25" t="s">
+      <c r="A16" s="27" t="s">
         <v>26</v>
       </c>
       <c r="B16" s="10" t="s">
-        <v>106</v>
+        <v>96</v>
       </c>
       <c r="C16" s="11" t="s">
         <v>27</v>
@@ -1343,9 +1358,9 @@
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A17" s="25"/>
+      <c r="A17" s="27"/>
       <c r="B17" s="10" t="s">
-        <v>106</v>
+        <v>96</v>
       </c>
       <c r="C17" s="11" t="s">
         <v>28</v>
@@ -1358,9 +1373,9 @@
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A18" s="25"/>
+      <c r="A18" s="27"/>
       <c r="B18" s="10" t="s">
-        <v>106</v>
+        <v>96</v>
       </c>
       <c r="C18" s="11" t="s">
         <v>29</v>
@@ -1373,17 +1388,15 @@
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A19" s="25" t="s">
-        <v>30</v>
-      </c>
+      <c r="A19" s="27"/>
       <c r="B19" s="10" t="s">
-        <v>31</v>
+        <v>96</v>
       </c>
       <c r="C19" s="11" t="s">
-        <v>27</v>
+        <v>114</v>
       </c>
       <c r="D19" s="15">
-        <v>1.444</v>
+        <v>0.01</v>
       </c>
       <c r="F19">
         <v>17</v>
@@ -1392,161 +1405,171 @@
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" s="25"/>
       <c r="B20" s="10" t="s">
-        <v>31</v>
+        <v>96</v>
       </c>
       <c r="C20" s="11" t="s">
-        <v>28</v>
+        <v>115</v>
       </c>
       <c r="D20" s="15">
-        <v>1.5129999999999999</v>
+        <v>0.01</v>
       </c>
       <c r="F20">
         <v>18</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A21" s="25"/>
+      <c r="A21" s="27" t="s">
+        <v>30</v>
+      </c>
       <c r="B21" s="10" t="s">
         <v>31</v>
       </c>
       <c r="C21" s="11" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="D21" s="15">
-        <v>1.4630000000000001</v>
+        <v>1.444</v>
       </c>
       <c r="F21">
         <v>19</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A22" s="9" t="s">
-        <v>32</v>
-      </c>
+      <c r="A22" s="27"/>
       <c r="B22" s="10" t="s">
-        <v>33</v>
-      </c>
-      <c r="C22" s="11"/>
+        <v>31</v>
+      </c>
+      <c r="C22" s="11" t="s">
+        <v>28</v>
+      </c>
       <c r="D22" s="15">
-        <v>0.51</v>
+        <v>1.5129999999999999</v>
       </c>
       <c r="F22">
         <v>20</v>
       </c>
     </row>
-    <row r="23" spans="1:7" ht="32.25" x14ac:dyDescent="0.25">
-      <c r="A23" s="9" t="s">
-        <v>34</v>
-      </c>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A23" s="27"/>
       <c r="B23" s="10" t="s">
-        <v>35</v>
-      </c>
-      <c r="C23" s="11"/>
+        <v>31</v>
+      </c>
+      <c r="C23" s="11" t="s">
+        <v>29</v>
+      </c>
       <c r="D23" s="15">
-        <v>100</v>
-      </c>
-      <c r="E23" t="s">
-        <v>105</v>
+        <v>1.4630000000000001</v>
       </c>
       <c r="F23">
         <v>21</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A24" s="9" t="s">
-        <v>36</v>
-      </c>
+      <c r="A24" s="27"/>
       <c r="B24" s="10" t="s">
-        <v>37</v>
-      </c>
-      <c r="C24" s="11"/>
+        <v>31</v>
+      </c>
+      <c r="C24" s="11" t="s">
+        <v>114</v>
+      </c>
       <c r="D24" s="15">
-        <v>3.7199999999999997E-2</v>
+        <v>1.415</v>
       </c>
       <c r="F24">
         <v>22</v>
       </c>
     </row>
-    <row r="25" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A25" s="26" t="s">
-        <v>38</v>
-      </c>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A25" s="27"/>
       <c r="B25" s="10" t="s">
-        <v>39</v>
+        <v>31</v>
       </c>
       <c r="C25" s="11" t="s">
-        <v>40</v>
-      </c>
-      <c r="D25" s="15"/>
-      <c r="E25" s="16" t="s">
-        <v>41</v>
+        <v>115</v>
+      </c>
+      <c r="D25" s="15">
+        <v>1.4139999999999999</v>
       </c>
       <c r="F25">
         <v>23</v>
       </c>
-      <c r="G25" t="s">
-        <v>42</v>
-      </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A26" s="26"/>
+      <c r="A26" s="9" t="s">
+        <v>32</v>
+      </c>
       <c r="B26" s="10" t="s">
-        <v>39</v>
-      </c>
-      <c r="C26" s="11" t="s">
-        <v>43</v>
-      </c>
-      <c r="D26" s="15"/>
+        <v>33</v>
+      </c>
+      <c r="C26" s="11"/>
+      <c r="D26" s="15">
+        <v>0.51</v>
+      </c>
       <c r="F26">
         <v>24</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A27" s="26"/>
+    <row r="27" spans="1:7" ht="32.25" x14ac:dyDescent="0.25">
+      <c r="A27" s="9" t="s">
+        <v>34</v>
+      </c>
       <c r="B27" s="10" t="s">
-        <v>39</v>
-      </c>
-      <c r="C27" s="11" t="s">
-        <v>44</v>
-      </c>
-      <c r="D27" s="15"/>
+        <v>35</v>
+      </c>
+      <c r="C27" s="11"/>
+      <c r="D27" s="15">
+        <v>100</v>
+      </c>
+      <c r="E27" t="s">
+        <v>95</v>
+      </c>
       <c r="F27">
         <v>25</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A28" s="26"/>
+      <c r="A28" s="9" t="s">
+        <v>36</v>
+      </c>
       <c r="B28" s="10" t="s">
-        <v>45</v>
-      </c>
-      <c r="C28" s="11" t="s">
-        <v>40</v>
-      </c>
-      <c r="D28" s="15"/>
+        <v>37</v>
+      </c>
+      <c r="C28" s="11"/>
+      <c r="D28" s="15">
+        <v>3.7199999999999997E-2</v>
+      </c>
       <c r="F28">
         <v>26</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A29" s="26"/>
+    <row r="29" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A29" s="28" t="s">
+        <v>38</v>
+      </c>
       <c r="B29" s="10" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="C29" s="11" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="D29" s="15"/>
+      <c r="E29" s="16" t="s">
+        <v>41</v>
+      </c>
       <c r="F29">
         <v>27</v>
       </c>
+      <c r="G29" t="s">
+        <v>42</v>
+      </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A30" s="26"/>
+      <c r="A30" s="28"/>
       <c r="B30" s="10" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="C30" s="11" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D30" s="15"/>
       <c r="F30">
@@ -1554,488 +1577,486 @@
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A31" s="27" t="s">
-        <v>46</v>
-      </c>
-      <c r="B31" s="17" t="s">
-        <v>47</v>
-      </c>
-      <c r="C31" s="18" t="s">
-        <v>27</v>
-      </c>
-      <c r="D31" s="15">
-        <v>0.01</v>
-      </c>
+      <c r="A31" s="28"/>
+      <c r="B31" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="C31" s="11" t="s">
+        <v>44</v>
+      </c>
+      <c r="D31" s="15"/>
       <c r="F31">
         <v>29</v>
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A32" s="27"/>
-      <c r="B32" s="17" t="s">
-        <v>47</v>
-      </c>
-      <c r="C32" s="18" t="s">
-        <v>28</v>
-      </c>
-      <c r="D32" s="15">
-        <v>0.1</v>
-      </c>
+      <c r="A32" s="28"/>
+      <c r="B32" s="10" t="s">
+        <v>45</v>
+      </c>
+      <c r="C32" s="11" t="s">
+        <v>40</v>
+      </c>
+      <c r="D32" s="15"/>
       <c r="F32">
         <v>30</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A33" s="27"/>
-      <c r="B33" s="17" t="s">
-        <v>47</v>
-      </c>
-      <c r="C33" s="18" t="s">
-        <v>29</v>
-      </c>
-      <c r="D33" s="15">
-        <v>0.5</v>
-      </c>
+      <c r="A33" s="28"/>
+      <c r="B33" s="10" t="s">
+        <v>45</v>
+      </c>
+      <c r="C33" s="11" t="s">
+        <v>43</v>
+      </c>
+      <c r="D33" s="15"/>
       <c r="F33">
         <v>31</v>
       </c>
     </row>
-    <row r="34" spans="1:6" ht="18" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A34" s="5" t="s">
-        <v>48</v>
-      </c>
-      <c r="B34" s="6"/>
-      <c r="C34" s="7"/>
-      <c r="D34" s="6"/>
-      <c r="E34" s="8"/>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A34" s="28"/>
+      <c r="B34" s="10" t="s">
+        <v>45</v>
+      </c>
+      <c r="C34" s="11" t="s">
+        <v>44</v>
+      </c>
+      <c r="D34" s="15"/>
       <c r="F34">
         <v>32</v>
       </c>
     </row>
-    <row r="35" spans="1:6" ht="18" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="19" t="s">
-        <v>49</v>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A35" s="29" t="s">
+        <v>46</v>
       </c>
       <c r="B35" s="17" t="s">
-        <v>50</v>
-      </c>
-      <c r="C35" s="18"/>
+        <v>47</v>
+      </c>
+      <c r="C35" s="18" t="s">
+        <v>27</v>
+      </c>
       <c r="D35" s="15">
-        <v>34</v>
+        <v>0.01</v>
       </c>
       <c r="F35">
         <v>33</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A36" s="19" t="s">
-        <v>51</v>
-      </c>
+      <c r="A36" s="29"/>
       <c r="B36" s="17" t="s">
-        <v>52</v>
-      </c>
-      <c r="C36" s="18"/>
+        <v>47</v>
+      </c>
+      <c r="C36" s="18" t="s">
+        <v>28</v>
+      </c>
       <c r="D36" s="15">
-        <v>3</v>
+        <v>0.1</v>
       </c>
       <c r="F36">
         <v>34</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A37" s="19" t="s">
-        <v>53</v>
-      </c>
+      <c r="A37" s="29"/>
       <c r="B37" s="17" t="s">
-        <v>54</v>
-      </c>
-      <c r="C37" s="18"/>
+        <v>47</v>
+      </c>
+      <c r="C37" s="18" t="s">
+        <v>29</v>
+      </c>
       <c r="D37" s="15">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="F37">
         <v>35</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A38" s="19" t="s">
-        <v>55</v>
-      </c>
+      <c r="A38" s="26"/>
       <c r="B38" s="17" t="s">
-        <v>56</v>
-      </c>
-      <c r="C38" s="18"/>
+        <v>47</v>
+      </c>
+      <c r="C38" s="18" t="s">
+        <v>114</v>
+      </c>
       <c r="D38" s="15">
-        <v>1.45</v>
+        <v>0</v>
       </c>
       <c r="F38">
         <v>36</v>
       </c>
     </row>
-    <row r="39" spans="1:6" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="A39" s="19" t="s">
-        <v>57</v>
-      </c>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A39" s="26"/>
       <c r="B39" s="17" t="s">
-        <v>58</v>
-      </c>
-      <c r="C39" s="18"/>
+        <v>47</v>
+      </c>
+      <c r="C39" s="18" t="s">
+        <v>115</v>
+      </c>
       <c r="D39" s="15">
-        <v>0.23100000000000001</v>
+        <v>0</v>
       </c>
       <c r="F39">
         <v>37</v>
       </c>
     </row>
-    <row r="40" spans="1:6" ht="18" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A40" s="5" t="s">
-        <v>59</v>
-      </c>
-      <c r="B40" s="6"/>
-      <c r="C40" s="7"/>
-      <c r="D40" s="6"/>
-      <c r="E40" s="8"/>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A40" s="29" t="s">
+        <v>110</v>
+      </c>
+      <c r="B40" s="17" t="s">
+        <v>111</v>
+      </c>
+      <c r="C40" s="18" t="s">
+        <v>27</v>
+      </c>
+      <c r="D40" s="15">
+        <v>6</v>
+      </c>
       <c r="F40">
         <v>38</v>
       </c>
     </row>
-    <row r="41" spans="1:6" ht="30.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="19" t="s">
-        <v>60</v>
-      </c>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A41" s="29"/>
       <c r="B41" s="17" t="s">
-        <v>61</v>
-      </c>
-      <c r="C41" s="18"/>
+        <v>111</v>
+      </c>
+      <c r="C41" s="18" t="s">
+        <v>28</v>
+      </c>
       <c r="D41" s="15">
-        <v>4</v>
+        <v>25</v>
       </c>
       <c r="F41">
         <v>39</v>
       </c>
     </row>
-    <row r="42" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A42" s="19" t="s">
-        <v>62</v>
-      </c>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A42" s="29"/>
       <c r="B42" s="17" t="s">
-        <v>63</v>
-      </c>
-      <c r="C42" s="18"/>
+        <v>111</v>
+      </c>
+      <c r="C42" s="18" t="s">
+        <v>29</v>
+      </c>
       <c r="D42" s="15">
-        <v>0.5</v>
+        <v>30</v>
       </c>
       <c r="F42">
         <v>40</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A43" s="19" t="s">
-        <v>64</v>
-      </c>
+      <c r="A43" s="29"/>
       <c r="B43" s="17" t="s">
-        <v>65</v>
-      </c>
-      <c r="C43" s="18"/>
+        <v>111</v>
+      </c>
+      <c r="C43" s="18" t="s">
+        <v>114</v>
+      </c>
       <c r="D43" s="15">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="F43">
         <v>41</v>
       </c>
     </row>
-    <row r="44" spans="1:6" ht="18" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A44" s="5" t="s">
-        <v>66</v>
-      </c>
-      <c r="B44" s="6"/>
-      <c r="C44" s="7"/>
-      <c r="D44" s="6"/>
-      <c r="E44" s="8"/>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A44" s="29"/>
+      <c r="B44" s="17" t="s">
+        <v>111</v>
+      </c>
+      <c r="C44" s="18" t="s">
+        <v>115</v>
+      </c>
+      <c r="D44" s="15">
+        <v>30</v>
+      </c>
       <c r="F44">
         <v>42</v>
       </c>
     </row>
-    <row r="45" spans="1:6" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="19" t="s">
-        <v>67</v>
-      </c>
-      <c r="B45" s="17" t="s">
-        <v>68</v>
-      </c>
-      <c r="C45" s="18"/>
-      <c r="D45" s="15">
-        <v>0.01</v>
-      </c>
+    <row r="45" spans="1:6" ht="18" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A45" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="B45" s="6"/>
+      <c r="C45" s="7"/>
+      <c r="D45" s="6"/>
+      <c r="E45" s="8"/>
       <c r="F45">
         <v>43</v>
       </c>
     </row>
-    <row r="46" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:6" ht="18" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A46" s="19" t="s">
-        <v>69</v>
+        <v>49</v>
       </c>
       <c r="B46" s="17" t="s">
-        <v>70</v>
+        <v>50</v>
       </c>
       <c r="C46" s="18"/>
       <c r="D46" s="15">
-        <v>365</v>
+        <v>34</v>
       </c>
       <c r="F46">
         <v>44</v>
       </c>
     </row>
-    <row r="47" spans="1:6" ht="18" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A47" s="5" t="s">
-        <v>71</v>
-      </c>
-      <c r="B47" s="6"/>
-      <c r="C47" s="7"/>
-      <c r="D47" s="6"/>
-      <c r="E47" s="8"/>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A47" s="19" t="s">
+        <v>51</v>
+      </c>
+      <c r="B47" s="17" t="s">
+        <v>52</v>
+      </c>
+      <c r="C47" s="18"/>
+      <c r="D47" s="15">
+        <v>3</v>
+      </c>
       <c r="F47">
         <v>45</v>
       </c>
     </row>
-    <row r="48" spans="1:6" ht="30.75" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A48" s="19" t="s">
-        <v>72</v>
+        <v>53</v>
       </c>
       <c r="B48" s="17" t="s">
-        <v>73</v>
+        <v>54</v>
       </c>
       <c r="C48" s="18"/>
       <c r="D48" s="15">
-        <v>0.25</v>
-      </c>
-      <c r="E48" t="s">
-        <v>74</v>
+        <v>1</v>
       </c>
       <c r="F48">
         <v>46</v>
       </c>
     </row>
-    <row r="49" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A49" s="19" t="s">
-        <v>75</v>
+        <v>55</v>
       </c>
       <c r="B49" s="17" t="s">
-        <v>76</v>
+        <v>56</v>
       </c>
       <c r="C49" s="18"/>
       <c r="D49" s="15">
-        <v>0.25</v>
+        <v>1.45</v>
       </c>
       <c r="F49">
         <v>47</v>
       </c>
     </row>
-    <row r="50" spans="1:6" ht="18" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A50" s="5" t="s">
-        <v>77</v>
-      </c>
-      <c r="B50" s="6"/>
-      <c r="C50" s="7"/>
-      <c r="D50" s="6"/>
-      <c r="E50" s="8" t="s">
-        <v>78</v>
+    <row r="50" spans="1:6" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="A50" s="19" t="s">
+        <v>57</v>
+      </c>
+      <c r="B50" s="17" t="s">
+        <v>58</v>
+      </c>
+      <c r="C50" s="18"/>
+      <c r="D50" s="15">
+        <v>0.23100000000000001</v>
       </c>
       <c r="F50">
         <v>48</v>
       </c>
     </row>
-    <row r="51" spans="1:6" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A51" s="19" t="s">
-        <v>79</v>
-      </c>
-      <c r="B51" s="17" t="s">
-        <v>80</v>
-      </c>
-      <c r="C51" s="18"/>
-      <c r="D51" s="12" t="s">
-        <v>81</v>
-      </c>
-      <c r="E51" t="s">
-        <v>82</v>
-      </c>
+    <row r="51" spans="1:6" ht="18" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A51" s="5" t="s">
+        <v>119</v>
+      </c>
+      <c r="B51" s="6"/>
+      <c r="C51" s="7"/>
+      <c r="D51" s="6"/>
+      <c r="E51" s="8"/>
       <c r="F51">
         <v>49</v>
       </c>
     </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:6" ht="18.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A52" s="19" t="s">
-        <v>83</v>
+        <v>117</v>
       </c>
       <c r="B52" s="17" t="s">
-        <v>84</v>
+        <v>118</v>
       </c>
       <c r="C52" s="18"/>
       <c r="D52" s="15">
-        <v>207</v>
+        <v>180</v>
       </c>
       <c r="F52">
         <v>50</v>
       </c>
     </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A53" s="19" t="s">
-        <v>85</v>
+        <v>59</v>
       </c>
       <c r="B53" s="17" t="s">
-        <v>86</v>
-      </c>
-      <c r="C53" s="18">
-        <v>1</v>
-      </c>
+        <v>120</v>
+      </c>
+      <c r="C53" s="18"/>
       <c r="D53" s="15">
-        <v>30</v>
+        <v>4</v>
       </c>
       <c r="F53">
         <v>51</v>
       </c>
     </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A54" s="19"/>
+    <row r="54" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A54" s="19" t="s">
+        <v>60</v>
+      </c>
       <c r="B54" s="17" t="s">
-        <v>86</v>
-      </c>
-      <c r="C54" s="18">
-        <v>2</v>
-      </c>
+        <v>121</v>
+      </c>
+      <c r="C54" s="18"/>
       <c r="D54" s="15">
-        <v>40</v>
+        <v>0.5</v>
       </c>
       <c r="F54">
         <v>52</v>
       </c>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A55" s="19"/>
+      <c r="A55" s="19" t="s">
+        <v>61</v>
+      </c>
       <c r="B55" s="17" t="s">
-        <v>86</v>
-      </c>
-      <c r="C55" s="18">
-        <v>3</v>
-      </c>
+        <v>122</v>
+      </c>
+      <c r="C55" s="18"/>
       <c r="D55" s="15">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="F55">
         <v>53</v>
       </c>
     </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A56" s="19"/>
-      <c r="B56" s="17" t="s">
-        <v>86</v>
-      </c>
-      <c r="C56" s="18">
-        <v>4</v>
-      </c>
-      <c r="D56" s="15"/>
+    <row r="56" spans="1:6" ht="18" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A56" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="B56" s="6"/>
+      <c r="C56" s="7"/>
+      <c r="D56" s="6"/>
+      <c r="E56" s="8"/>
       <c r="F56">
         <v>54</v>
       </c>
     </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A57" s="19"/>
+    <row r="57" spans="1:6" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A57" s="19" t="s">
+        <v>63</v>
+      </c>
       <c r="B57" s="17" t="s">
-        <v>86</v>
-      </c>
-      <c r="C57" s="18">
-        <v>5</v>
-      </c>
-      <c r="D57" s="15"/>
+        <v>64</v>
+      </c>
+      <c r="C57" s="18"/>
+      <c r="D57" s="15">
+        <v>0.01</v>
+      </c>
       <c r="F57">
         <v>55</v>
       </c>
     </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A58" s="19" t="s">
-        <v>87</v>
+        <v>65</v>
       </c>
       <c r="B58" s="17" t="s">
-        <v>88</v>
-      </c>
-      <c r="C58" s="18">
-        <v>1</v>
-      </c>
+        <v>66</v>
+      </c>
+      <c r="C58" s="18"/>
       <c r="D58" s="15">
-        <v>0.01</v>
+        <v>365</v>
       </c>
       <c r="F58">
         <v>56</v>
       </c>
     </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A59" s="19"/>
-      <c r="B59" s="17" t="s">
-        <v>88</v>
-      </c>
-      <c r="C59" s="18">
-        <v>2</v>
-      </c>
-      <c r="D59" s="15">
-        <v>0.25</v>
+    <row r="59" spans="1:6" ht="18" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A59" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="B59" s="6"/>
+      <c r="C59" s="7"/>
+      <c r="D59" s="6"/>
+      <c r="E59" s="8" t="s">
+        <v>68</v>
       </c>
       <c r="F59">
         <v>57</v>
       </c>
     </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A60" s="19"/>
+    <row r="60" spans="1:6" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A60" s="19" t="s">
+        <v>69</v>
+      </c>
       <c r="B60" s="17" t="s">
-        <v>88</v>
-      </c>
-      <c r="C60" s="18">
-        <v>3</v>
-      </c>
-      <c r="D60" s="15">
-        <v>0.67</v>
+        <v>70</v>
+      </c>
+      <c r="C60" s="18"/>
+      <c r="D60" s="12" t="s">
+        <v>71</v>
+      </c>
+      <c r="E60" t="s">
+        <v>72</v>
       </c>
       <c r="F60">
         <v>58</v>
       </c>
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A61" s="19"/>
+      <c r="A61" s="19" t="s">
+        <v>73</v>
+      </c>
       <c r="B61" s="17" t="s">
-        <v>88</v>
-      </c>
-      <c r="C61" s="18">
-        <v>4</v>
-      </c>
-      <c r="D61" s="15"/>
+        <v>74</v>
+      </c>
+      <c r="C61" s="18"/>
+      <c r="D61" s="15">
+        <v>207</v>
+      </c>
       <c r="F61">
         <v>59</v>
       </c>
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A62" s="19"/>
+      <c r="A62" s="19" t="s">
+        <v>75</v>
+      </c>
       <c r="B62" s="17" t="s">
-        <v>88</v>
+        <v>76</v>
       </c>
       <c r="C62" s="18">
-        <v>5</v>
-      </c>
-      <c r="D62" s="15"/>
+        <v>1</v>
+      </c>
+      <c r="D62" s="15">
+        <v>30</v>
+      </c>
       <c r="F62">
         <v>60</v>
       </c>
     </row>
-    <row r="63" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A63" s="19" t="s">
-        <v>89</v>
-      </c>
+    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A63" s="19"/>
       <c r="B63" s="17" t="s">
-        <v>90</v>
+        <v>76</v>
       </c>
       <c r="C63" s="18">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D63" s="15">
-        <v>1</v>
+        <v>40</v>
       </c>
       <c r="F63">
         <v>61</v>
@@ -2044,13 +2065,13 @@
     <row r="64" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A64" s="19"/>
       <c r="B64" s="17" t="s">
-        <v>90</v>
+        <v>76</v>
       </c>
       <c r="C64" s="18">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D64" s="15">
-        <v>1</v>
+        <v>50</v>
       </c>
       <c r="F64">
         <v>62</v>
@@ -2059,14 +2080,12 @@
     <row r="65" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A65" s="19"/>
       <c r="B65" s="17" t="s">
-        <v>90</v>
+        <v>76</v>
       </c>
       <c r="C65" s="18">
-        <v>3</v>
-      </c>
-      <c r="D65" s="15">
-        <v>1</v>
-      </c>
+        <v>4</v>
+      </c>
+      <c r="D65" s="15"/>
       <c r="F65">
         <v>63</v>
       </c>
@@ -2074,10 +2093,10 @@
     <row r="66" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A66" s="19"/>
       <c r="B66" s="17" t="s">
-        <v>90</v>
+        <v>76</v>
       </c>
       <c r="C66" s="18">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D66" s="15"/>
       <c r="F66">
@@ -2085,61 +2104,61 @@
       </c>
     </row>
     <row r="67" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A67" s="19"/>
+      <c r="A67" s="19" t="s">
+        <v>77</v>
+      </c>
       <c r="B67" s="17" t="s">
-        <v>90</v>
+        <v>78</v>
       </c>
       <c r="C67" s="18">
-        <v>5</v>
-      </c>
-      <c r="D67" s="15"/>
+        <v>1</v>
+      </c>
+      <c r="D67" s="15">
+        <v>0.01</v>
+      </c>
       <c r="F67">
         <v>65</v>
       </c>
     </row>
     <row r="68" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A68" s="19" t="s">
-        <v>91</v>
-      </c>
+      <c r="A68" s="19"/>
       <c r="B68" s="17" t="s">
-        <v>92</v>
-      </c>
-      <c r="C68" s="18"/>
-      <c r="D68" s="12" t="s">
-        <v>93</v>
+        <v>78</v>
+      </c>
+      <c r="C68" s="18">
+        <v>2</v>
+      </c>
+      <c r="D68" s="15">
+        <v>0.25</v>
       </c>
       <c r="F68">
         <v>66</v>
       </c>
     </row>
     <row r="69" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A69" s="19" t="s">
-        <v>94</v>
-      </c>
+      <c r="A69" s="19"/>
       <c r="B69" s="17" t="s">
-        <v>95</v>
-      </c>
-      <c r="C69" s="18"/>
+        <v>78</v>
+      </c>
+      <c r="C69" s="18">
+        <v>3</v>
+      </c>
       <c r="D69" s="15">
-        <v>365</v>
+        <v>0.67</v>
       </c>
       <c r="F69">
         <v>67</v>
       </c>
     </row>
     <row r="70" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A70" s="19" t="s">
-        <v>96</v>
-      </c>
+      <c r="A70" s="19"/>
       <c r="B70" s="17" t="s">
-        <v>97</v>
+        <v>78</v>
       </c>
       <c r="C70" s="18">
-        <v>1</v>
-      </c>
-      <c r="D70" s="15">
-        <v>0</v>
-      </c>
+        <v>4</v>
+      </c>
+      <c r="D70" s="15"/>
       <c r="F70">
         <v>68</v>
       </c>
@@ -2147,28 +2166,28 @@
     <row r="71" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A71" s="19"/>
       <c r="B71" s="17" t="s">
-        <v>97</v>
+        <v>78</v>
       </c>
       <c r="C71" s="18">
-        <v>2</v>
-      </c>
-      <c r="D71" s="15">
-        <v>0.2</v>
-      </c>
+        <v>5</v>
+      </c>
+      <c r="D71" s="15"/>
       <c r="F71">
         <v>69</v>
       </c>
     </row>
-    <row r="72" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A72" s="19"/>
+    <row r="72" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A72" s="19" t="s">
+        <v>79</v>
+      </c>
       <c r="B72" s="17" t="s">
-        <v>97</v>
+        <v>80</v>
       </c>
       <c r="C72" s="18">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D72" s="15">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="F72">
         <v>70</v>
@@ -2177,13 +2196,13 @@
     <row r="73" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A73" s="19"/>
       <c r="B73" s="17" t="s">
-        <v>97</v>
+        <v>80</v>
       </c>
       <c r="C73" s="18">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="D73" s="15">
-        <v>0.68</v>
+        <v>1</v>
       </c>
       <c r="F73">
         <v>71</v>
@@ -2192,31 +2211,27 @@
     <row r="74" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A74" s="19"/>
       <c r="B74" s="17" t="s">
-        <v>97</v>
+        <v>80</v>
       </c>
       <c r="C74" s="18">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D74" s="15">
-        <v>1.1200000000000001</v>
+        <v>1</v>
       </c>
       <c r="F74">
         <v>72</v>
       </c>
     </row>
     <row r="75" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A75" s="19" t="s">
-        <v>98</v>
-      </c>
+      <c r="A75" s="19"/>
       <c r="B75" s="17" t="s">
-        <v>99</v>
+        <v>80</v>
       </c>
       <c r="C75" s="18">
-        <v>1</v>
-      </c>
-      <c r="D75" s="15">
-        <v>0</v>
-      </c>
+        <v>4</v>
+      </c>
+      <c r="D75" s="15"/>
       <c r="F75">
         <v>73</v>
       </c>
@@ -2224,75 +2239,73 @@
     <row r="76" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A76" s="19"/>
       <c r="B76" s="17" t="s">
-        <v>99</v>
+        <v>80</v>
       </c>
       <c r="C76" s="18">
-        <v>2</v>
-      </c>
-      <c r="D76" s="15">
-        <v>0</v>
-      </c>
+        <v>5</v>
+      </c>
+      <c r="D76" s="15"/>
       <c r="F76">
         <v>74</v>
       </c>
     </row>
     <row r="77" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A77" s="19"/>
+      <c r="A77" s="19" t="s">
+        <v>81</v>
+      </c>
       <c r="B77" s="17" t="s">
-        <v>99</v>
-      </c>
-      <c r="C77" s="18">
-        <v>3</v>
-      </c>
-      <c r="D77" s="15">
-        <v>0</v>
+        <v>82</v>
+      </c>
+      <c r="C77" s="18"/>
+      <c r="D77" s="12" t="s">
+        <v>83</v>
       </c>
       <c r="F77">
         <v>75</v>
       </c>
     </row>
     <row r="78" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A78" s="19"/>
+      <c r="A78" s="19" t="s">
+        <v>84</v>
+      </c>
       <c r="B78" s="17" t="s">
-        <v>99</v>
-      </c>
-      <c r="C78" s="18">
-        <v>4</v>
-      </c>
+        <v>85</v>
+      </c>
+      <c r="C78" s="18"/>
       <c r="D78" s="15">
-        <v>1</v>
+        <v>365</v>
       </c>
       <c r="F78">
         <v>76</v>
       </c>
     </row>
     <row r="79" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A79" s="19"/>
+      <c r="A79" s="19" t="s">
+        <v>86</v>
+      </c>
       <c r="B79" s="17" t="s">
-        <v>99</v>
+        <v>87</v>
       </c>
       <c r="C79" s="18">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="D79" s="15">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F79">
         <v>77</v>
       </c>
     </row>
-    <row r="80" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A80" s="19" t="s">
-        <v>100</v>
-      </c>
+    <row r="80" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A80" s="19"/>
       <c r="B80" s="17" t="s">
-        <v>101</v>
+        <v>87</v>
       </c>
       <c r="C80" s="18">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D80" s="15">
-        <v>500</v>
+        <v>0.2</v>
       </c>
       <c r="F80">
         <v>78</v>
@@ -2301,13 +2314,13 @@
     <row r="81" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A81" s="19"/>
       <c r="B81" s="17" t="s">
-        <v>101</v>
+        <v>87</v>
       </c>
       <c r="C81" s="18">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D81" s="15">
-        <v>300</v>
+        <v>0.5</v>
       </c>
       <c r="F81">
         <v>79</v>
@@ -2316,13 +2329,13 @@
     <row r="82" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A82" s="19"/>
       <c r="B82" s="17" t="s">
-        <v>101</v>
+        <v>87</v>
       </c>
       <c r="C82" s="18">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D82" s="15">
-        <v>200</v>
+        <v>0.68</v>
       </c>
       <c r="F82">
         <v>80</v>
@@ -2331,77 +2344,171 @@
     <row r="83" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A83" s="19"/>
       <c r="B83" s="17" t="s">
-        <v>101</v>
+        <v>87</v>
       </c>
       <c r="C83" s="18">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D83" s="15">
-        <v>200</v>
+        <v>1.1200000000000001</v>
       </c>
       <c r="F83">
         <v>81</v>
       </c>
     </row>
     <row r="84" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A84" s="19"/>
+      <c r="A84" s="19" t="s">
+        <v>88</v>
+      </c>
       <c r="B84" s="17" t="s">
-        <v>101</v>
+        <v>89</v>
       </c>
       <c r="C84" s="18">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="D84" s="15">
-        <v>300</v>
+        <v>0</v>
       </c>
       <c r="F84">
         <v>82</v>
       </c>
     </row>
     <row r="85" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A85" s="20"/>
-      <c r="B85" s="21"/>
-      <c r="C85" s="22"/>
+      <c r="A85" s="19"/>
+      <c r="B85" s="17" t="s">
+        <v>89</v>
+      </c>
+      <c r="C85" s="18">
+        <v>2</v>
+      </c>
+      <c r="D85" s="15">
+        <v>0</v>
+      </c>
+      <c r="F85">
+        <v>83</v>
+      </c>
     </row>
     <row r="86" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A86" s="20"/>
-      <c r="B86" s="21"/>
-      <c r="C86" s="22"/>
+      <c r="A86" s="19"/>
+      <c r="B86" s="17" t="s">
+        <v>89</v>
+      </c>
+      <c r="C86" s="18">
+        <v>3</v>
+      </c>
+      <c r="D86" s="15">
+        <v>0</v>
+      </c>
+      <c r="F86">
+        <v>84</v>
+      </c>
     </row>
     <row r="87" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A87" s="20"/>
-      <c r="B87" s="21"/>
-      <c r="C87" s="22"/>
+      <c r="A87" s="19"/>
+      <c r="B87" s="17" t="s">
+        <v>89</v>
+      </c>
+      <c r="C87" s="18">
+        <v>4</v>
+      </c>
+      <c r="D87" s="15">
+        <v>1</v>
+      </c>
+      <c r="F87">
+        <v>85</v>
+      </c>
     </row>
     <row r="88" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A88" s="20"/>
-      <c r="B88" s="21"/>
-      <c r="C88" s="22"/>
-    </row>
-    <row r="89" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A89" s="20"/>
-      <c r="B89" s="21"/>
-      <c r="C89" s="22"/>
+      <c r="A88" s="19"/>
+      <c r="B88" s="17" t="s">
+        <v>89</v>
+      </c>
+      <c r="C88" s="18">
+        <v>5</v>
+      </c>
+      <c r="D88" s="15">
+        <v>1</v>
+      </c>
+      <c r="F88">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="89" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A89" s="19" t="s">
+        <v>90</v>
+      </c>
+      <c r="B89" s="17" t="s">
+        <v>91</v>
+      </c>
+      <c r="C89" s="18">
+        <v>1</v>
+      </c>
+      <c r="D89" s="15">
+        <v>500</v>
+      </c>
+      <c r="F89">
+        <v>87</v>
+      </c>
     </row>
     <row r="90" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A90" s="20"/>
-      <c r="B90" s="21"/>
-      <c r="C90" s="22"/>
+      <c r="A90" s="19"/>
+      <c r="B90" s="17" t="s">
+        <v>91</v>
+      </c>
+      <c r="C90" s="18">
+        <v>2</v>
+      </c>
+      <c r="D90" s="15">
+        <v>300</v>
+      </c>
+      <c r="F90">
+        <v>88</v>
+      </c>
     </row>
     <row r="91" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A91" s="20"/>
-      <c r="B91" s="21"/>
-      <c r="C91" s="22"/>
+      <c r="A91" s="19"/>
+      <c r="B91" s="17" t="s">
+        <v>91</v>
+      </c>
+      <c r="C91" s="18">
+        <v>3</v>
+      </c>
+      <c r="D91" s="15">
+        <v>200</v>
+      </c>
+      <c r="F91">
+        <v>89</v>
+      </c>
     </row>
     <row r="92" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A92" s="20"/>
-      <c r="B92" s="21"/>
-      <c r="C92" s="22"/>
+      <c r="A92" s="19"/>
+      <c r="B92" s="17" t="s">
+        <v>91</v>
+      </c>
+      <c r="C92" s="18">
+        <v>4</v>
+      </c>
+      <c r="D92" s="15">
+        <v>200</v>
+      </c>
+      <c r="F92">
+        <v>90</v>
+      </c>
     </row>
     <row r="93" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A93" s="20"/>
-      <c r="B93" s="21"/>
-      <c r="C93" s="22"/>
+      <c r="A93" s="19"/>
+      <c r="B93" s="17" t="s">
+        <v>91</v>
+      </c>
+      <c r="C93" s="18">
+        <v>5</v>
+      </c>
+      <c r="D93" s="15">
+        <v>300</v>
+      </c>
+      <c r="F93">
+        <v>91</v>
+      </c>
     </row>
     <row r="94" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A94" s="20"/>
@@ -2958,12 +3065,58 @@
       <c r="B204" s="21"/>
       <c r="C204" s="22"/>
     </row>
+    <row r="205" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A205" s="20"/>
+      <c r="B205" s="21"/>
+      <c r="C205" s="22"/>
+    </row>
+    <row r="206" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A206" s="20"/>
+      <c r="B206" s="21"/>
+      <c r="C206" s="22"/>
+    </row>
+    <row r="207" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A207" s="20"/>
+      <c r="B207" s="21"/>
+      <c r="C207" s="22"/>
+    </row>
+    <row r="208" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A208" s="20"/>
+      <c r="B208" s="21"/>
+      <c r="C208" s="22"/>
+    </row>
+    <row r="209" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A209" s="20"/>
+      <c r="B209" s="21"/>
+      <c r="C209" s="22"/>
+    </row>
+    <row r="210" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A210" s="20"/>
+      <c r="B210" s="21"/>
+      <c r="C210" s="22"/>
+    </row>
+    <row r="211" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A211" s="20"/>
+      <c r="B211" s="21"/>
+      <c r="C211" s="22"/>
+    </row>
+    <row r="212" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A212" s="20"/>
+      <c r="B212" s="21"/>
+      <c r="C212" s="22"/>
+    </row>
+    <row r="213" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A213" s="20"/>
+      <c r="B213" s="21"/>
+      <c r="C213" s="22"/>
+    </row>
   </sheetData>
-  <mergeCells count="4">
-    <mergeCell ref="A16:A18"/>
-    <mergeCell ref="A19:A21"/>
-    <mergeCell ref="A25:A30"/>
-    <mergeCell ref="A31:A33"/>
+  <mergeCells count="5">
+    <mergeCell ref="A16:A19"/>
+    <mergeCell ref="A21:A25"/>
+    <mergeCell ref="A29:A34"/>
+    <mergeCell ref="A40:A44"/>
+    <mergeCell ref="A35:A37"/>
   </mergeCells>
   <dataValidations count="12">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D4" xr:uid="{CDBB5640-3705-4524-A12C-18C0BA89A391}">
@@ -2975,10 +3128,10 @@
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D6" xr:uid="{FCAB33B4-E22D-416A-9EE8-1B6629F4B7A9}">
       <formula1>"angiosperm, gymnosperm"</formula1>
     </dataValidation>
-    <dataValidation type="whole" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D46" xr:uid="{2A9331BB-EEBF-40CD-B47D-E4013CB2D0AD}">
+    <dataValidation type="whole" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D58" xr:uid="{2A9331BB-EEBF-40CD-B47D-E4013CB2D0AD}">
       <formula1>0</formula1>
     </dataValidation>
-    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D22 D42:D45 D47:D50" xr:uid="{C20F82BC-B9F3-4514-8D12-0BF659884D61}">
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D26 D54:D57 D59" xr:uid="{C20F82BC-B9F3-4514-8D12-0BF659884D61}">
       <formula1>0</formula1>
       <formula2>1</formula2>
     </dataValidation>
@@ -3011,10 +3164,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7A5B2ED1-E60A-481E-A183-520033C5AF7F}">
-  <dimension ref="A1:G204"/>
+  <dimension ref="A1:G213"/>
   <sheetViews>
-    <sheetView topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+    <sheetView tabSelected="1" topLeftCell="A38" workbookViewId="0">
+      <selection activeCell="J54" sqref="J54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3042,9 +3195,6 @@
       <c r="E1" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="F1">
-        <v>0</v>
-      </c>
     </row>
     <row r="2" spans="1:6" ht="18.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="5" t="s">
@@ -3055,7 +3205,7 @@
       <c r="D2" s="8"/>
       <c r="E2" s="8"/>
       <c r="F2">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
@@ -3067,10 +3217,10 @@
       </c>
       <c r="C3" s="11"/>
       <c r="D3" s="12" t="s">
-        <v>118</v>
+        <v>108</v>
       </c>
       <c r="F3">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
@@ -3078,14 +3228,14 @@
         <v>8</v>
       </c>
       <c r="B4" s="10" t="s">
-        <v>116</v>
+        <v>106</v>
       </c>
       <c r="C4" s="11"/>
       <c r="D4" s="12" t="s">
         <v>10</v>
       </c>
       <c r="F4">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
@@ -3100,7 +3250,7 @@
         <v>13</v>
       </c>
       <c r="F5">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
@@ -3115,7 +3265,7 @@
         <v>16</v>
       </c>
       <c r="F6">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
@@ -3123,59 +3273,59 @@
         <v>17</v>
       </c>
       <c r="B7" s="10" t="s">
-        <v>115</v>
+        <v>105</v>
       </c>
       <c r="C7" s="11"/>
       <c r="D7" s="12" t="s">
-        <v>103</v>
+        <v>112</v>
       </c>
       <c r="F7">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="9" t="s">
+        <v>97</v>
+      </c>
+      <c r="B8" s="10" t="s">
         <v>107</v>
-      </c>
-      <c r="B8" s="10" t="s">
-        <v>117</v>
       </c>
       <c r="C8" s="11"/>
       <c r="D8" s="12" t="s">
-        <v>111</v>
+        <v>101</v>
       </c>
       <c r="F8">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="9" t="s">
-        <v>108</v>
+        <v>98</v>
       </c>
       <c r="B9" s="10" t="s">
         <v>9</v>
       </c>
       <c r="C9" s="11"/>
       <c r="D9" s="12" t="s">
-        <v>114</v>
+        <v>104</v>
       </c>
       <c r="F9">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="9" t="s">
-        <v>109</v>
+        <v>99</v>
       </c>
       <c r="B10" s="10" t="s">
-        <v>110</v>
+        <v>100</v>
       </c>
       <c r="C10" s="11"/>
       <c r="D10" s="12" t="s">
-        <v>113</v>
+        <v>103</v>
       </c>
       <c r="F10">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
@@ -3183,14 +3333,14 @@
         <v>18</v>
       </c>
       <c r="B11" s="10" t="s">
-        <v>119</v>
+        <v>109</v>
       </c>
       <c r="C11" s="11"/>
       <c r="D11" s="12" t="s">
-        <v>104</v>
+        <v>113</v>
       </c>
       <c r="F11">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="12" spans="1:6" ht="18" thickBot="1" x14ac:dyDescent="0.35">
@@ -3202,7 +3352,7 @@
       <c r="D12" s="14"/>
       <c r="E12" s="8"/>
       <c r="F12">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="13" spans="1:6" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
@@ -3217,7 +3367,7 @@
         <v>144</v>
       </c>
       <c r="F13">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
@@ -3232,7 +3382,7 @@
         <v>305</v>
       </c>
       <c r="F14">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
@@ -3247,15 +3397,15 @@
         <v>273</v>
       </c>
       <c r="F15">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A16" s="25" t="s">
+      <c r="A16" s="27" t="s">
         <v>26</v>
       </c>
       <c r="B16" s="10" t="s">
-        <v>106</v>
+        <v>96</v>
       </c>
       <c r="C16" s="11" t="s">
         <v>27</v>
@@ -3264,13 +3414,13 @@
         <v>1.4999999999999999E-2</v>
       </c>
       <c r="F16">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A17" s="25"/>
+      <c r="A17" s="27"/>
       <c r="B17" s="10" t="s">
-        <v>106</v>
+        <v>96</v>
       </c>
       <c r="C17" s="11" t="s">
         <v>28</v>
@@ -3279,13 +3429,13 @@
         <v>1.4999999999999999E-2</v>
       </c>
       <c r="F17">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A18" s="25"/>
+      <c r="A18" s="27"/>
       <c r="B18" s="10" t="s">
-        <v>106</v>
+        <v>96</v>
       </c>
       <c r="C18" s="11" t="s">
         <v>29</v>
@@ -3294,1039 +3444,1131 @@
         <v>0.03</v>
       </c>
       <c r="F18">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A19" s="27"/>
+      <c r="B19" s="10" t="s">
+        <v>96</v>
+      </c>
+      <c r="C19" s="11" t="s">
+        <v>114</v>
+      </c>
+      <c r="D19" s="15">
+        <v>0.01</v>
+      </c>
+      <c r="F19">
         <v>17</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A19" s="25" t="s">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A20" s="27"/>
+      <c r="B20" s="10" t="s">
+        <v>96</v>
+      </c>
+      <c r="C20" s="11" t="s">
+        <v>115</v>
+      </c>
+      <c r="D20" s="15">
+        <v>0.01</v>
+      </c>
+      <c r="F20">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A21" s="27" t="s">
         <v>30</v>
       </c>
-      <c r="B19" s="10" t="s">
-        <v>31</v>
-      </c>
-      <c r="C19" s="11" t="s">
-        <v>27</v>
-      </c>
-      <c r="D19" s="15">
-        <v>1.444</v>
-      </c>
-      <c r="F19">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A20" s="25"/>
-      <c r="B20" s="10" t="s">
-        <v>31</v>
-      </c>
-      <c r="C20" s="11" t="s">
-        <v>28</v>
-      </c>
-      <c r="D20" s="15">
-        <v>1.5129999999999999</v>
-      </c>
-      <c r="F20">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A21" s="25"/>
       <c r="B21" s="10" t="s">
         <v>31</v>
       </c>
       <c r="C21" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="D21" s="15">
+        <v>1.444</v>
+      </c>
+      <c r="F21">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A22" s="27"/>
+      <c r="B22" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="C22" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="D22" s="15">
+        <v>1.5129999999999999</v>
+      </c>
+      <c r="F22">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A23" s="27"/>
+      <c r="B23" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="C23" s="11" t="s">
         <v>29</v>
       </c>
-      <c r="D21" s="15">
+      <c r="D23" s="15">
         <v>1.4630000000000001</v>
       </c>
-      <c r="F21">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A22" s="9" t="s">
+      <c r="F23">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A24" s="27"/>
+      <c r="B24" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="C24" s="11" t="s">
+        <v>114</v>
+      </c>
+      <c r="D24" s="15">
+        <v>1.415</v>
+      </c>
+      <c r="F24">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A25" s="27"/>
+      <c r="B25" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="C25" s="11" t="s">
+        <v>115</v>
+      </c>
+      <c r="D25" s="15">
+        <v>1.4139999999999999</v>
+      </c>
+      <c r="F25">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A26" s="9" t="s">
         <v>32</v>
       </c>
-      <c r="B22" s="10" t="s">
+      <c r="B26" s="10" t="s">
         <v>33</v>
       </c>
-      <c r="C22" s="11"/>
-      <c r="D22" s="15">
+      <c r="C26" s="11"/>
+      <c r="D26" s="15">
         <v>0.48</v>
       </c>
-      <c r="F22">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7" ht="32.25" x14ac:dyDescent="0.25">
-      <c r="A23" s="9" t="s">
+      <c r="F26">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" ht="32.25" x14ac:dyDescent="0.25">
+      <c r="A27" s="9" t="s">
         <v>34</v>
       </c>
-      <c r="B23" s="10" t="s">
+      <c r="B27" s="10" t="s">
         <v>35</v>
       </c>
-      <c r="C23" s="11"/>
-      <c r="D23" s="15">
+      <c r="C27" s="11"/>
+      <c r="D27" s="15">
         <v>100</v>
       </c>
-      <c r="E23" t="s">
-        <v>105</v>
-      </c>
-      <c r="F23">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A24" s="9" t="s">
+      <c r="E27" t="s">
+        <v>95</v>
+      </c>
+      <c r="F27">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A28" s="9" t="s">
         <v>36</v>
       </c>
-      <c r="B24" s="10" t="s">
+      <c r="B28" s="10" t="s">
         <v>37</v>
       </c>
-      <c r="C24" s="11"/>
-      <c r="D24" s="15">
+      <c r="C28" s="11"/>
+      <c r="D28" s="15">
         <v>0.05</v>
       </c>
-      <c r="F24">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A25" s="26" t="s">
+      <c r="F28">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A29" s="28" t="s">
         <v>38</v>
       </c>
-      <c r="B25" s="10" t="s">
+      <c r="B29" s="10" t="s">
         <v>39</v>
       </c>
-      <c r="C25" s="11" t="s">
+      <c r="C29" s="11" t="s">
         <v>40</v>
       </c>
-      <c r="D25" s="15"/>
-      <c r="E25" s="16" t="s">
+      <c r="D29" s="15"/>
+      <c r="E29" s="16" t="s">
         <v>41</v>
       </c>
-      <c r="F25">
-        <v>24</v>
-      </c>
-      <c r="G25" t="s">
+      <c r="F29">
+        <v>27</v>
+      </c>
+      <c r="G29" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A26" s="26"/>
-      <c r="B26" s="10" t="s">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A30" s="28"/>
+      <c r="B30" s="10" t="s">
         <v>39</v>
       </c>
-      <c r="C26" s="11" t="s">
+      <c r="C30" s="11" t="s">
         <v>43</v>
-      </c>
-      <c r="D26" s="15"/>
-      <c r="F26">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A27" s="26"/>
-      <c r="B27" s="10" t="s">
-        <v>39</v>
-      </c>
-      <c r="C27" s="11" t="s">
-        <v>44</v>
-      </c>
-      <c r="D27" s="15"/>
-      <c r="F27">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A28" s="26"/>
-      <c r="B28" s="10" t="s">
-        <v>45</v>
-      </c>
-      <c r="C28" s="11" t="s">
-        <v>40</v>
-      </c>
-      <c r="D28" s="15"/>
-      <c r="F28">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A29" s="26"/>
-      <c r="B29" s="10" t="s">
-        <v>45</v>
-      </c>
-      <c r="C29" s="11" t="s">
-        <v>43</v>
-      </c>
-      <c r="D29" s="15"/>
-      <c r="F29">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A30" s="26"/>
-      <c r="B30" s="10" t="s">
-        <v>45</v>
-      </c>
-      <c r="C30" s="11" t="s">
-        <v>44</v>
       </c>
       <c r="D30" s="15"/>
       <c r="F30">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A31" s="28"/>
+      <c r="B31" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="C31" s="11" t="s">
+        <v>44</v>
+      </c>
+      <c r="D31" s="15"/>
+      <c r="F31">
         <v>29</v>
       </c>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A31" s="27" t="s">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A32" s="28"/>
+      <c r="B32" s="10" t="s">
+        <v>45</v>
+      </c>
+      <c r="C32" s="11" t="s">
+        <v>40</v>
+      </c>
+      <c r="D32" s="15"/>
+      <c r="F32">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A33" s="28"/>
+      <c r="B33" s="10" t="s">
+        <v>45</v>
+      </c>
+      <c r="C33" s="11" t="s">
+        <v>43</v>
+      </c>
+      <c r="D33" s="15"/>
+      <c r="F33">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A34" s="28"/>
+      <c r="B34" s="10" t="s">
+        <v>45</v>
+      </c>
+      <c r="C34" s="11" t="s">
+        <v>44</v>
+      </c>
+      <c r="D34" s="15"/>
+      <c r="F34">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A35" s="29" t="s">
         <v>46</v>
       </c>
-      <c r="B31" s="17" t="s">
+      <c r="B35" s="17" t="s">
         <v>47</v>
       </c>
-      <c r="C31" s="18" t="s">
+      <c r="C35" s="18" t="s">
         <v>27</v>
       </c>
-      <c r="D31" s="15">
+      <c r="D35" s="15">
         <v>0.01</v>
       </c>
-      <c r="F31">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A32" s="27"/>
-      <c r="B32" s="17" t="s">
+      <c r="F35">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A36" s="29"/>
+      <c r="B36" s="17" t="s">
         <v>47</v>
       </c>
-      <c r="C32" s="18" t="s">
+      <c r="C36" s="18" t="s">
         <v>28</v>
       </c>
-      <c r="D32" s="15">
+      <c r="D36" s="15">
         <v>0.1</v>
       </c>
-      <c r="F32">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A33" s="27"/>
-      <c r="B33" s="17" t="s">
+      <c r="F36">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A37" s="29"/>
+      <c r="B37" s="17" t="s">
         <v>47</v>
       </c>
-      <c r="C33" s="18" t="s">
+      <c r="C37" s="18" t="s">
         <v>29</v>
       </c>
-      <c r="D33" s="15">
+      <c r="D37" s="15">
         <v>0.5</v>
       </c>
-      <c r="F33">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="34" spans="1:6" ht="18" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A34" s="5" t="s">
+      <c r="F37">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A38" s="29"/>
+      <c r="B38" s="17" t="s">
+        <v>47</v>
+      </c>
+      <c r="C38" s="18" t="s">
+        <v>114</v>
+      </c>
+      <c r="D38" s="15">
+        <v>0</v>
+      </c>
+      <c r="F38">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A39" s="29"/>
+      <c r="B39" s="17" t="s">
+        <v>47</v>
+      </c>
+      <c r="C39" s="18" t="s">
+        <v>115</v>
+      </c>
+      <c r="D39" s="15">
+        <v>0</v>
+      </c>
+      <c r="F39">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A40" s="29" t="s">
+        <v>110</v>
+      </c>
+      <c r="B40" s="17" t="s">
+        <v>111</v>
+      </c>
+      <c r="C40" s="18" t="s">
+        <v>27</v>
+      </c>
+      <c r="D40" s="15">
+        <v>1.23</v>
+      </c>
+      <c r="F40">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A41" s="29"/>
+      <c r="B41" s="17" t="s">
+        <v>111</v>
+      </c>
+      <c r="C41" s="18" t="s">
+        <v>28</v>
+      </c>
+      <c r="D41" s="15">
+        <v>5</v>
+      </c>
+      <c r="F41">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A42" s="29"/>
+      <c r="B42" s="17" t="s">
+        <v>111</v>
+      </c>
+      <c r="C42" s="18" t="s">
+        <v>29</v>
+      </c>
+      <c r="D42" s="15">
+        <v>4</v>
+      </c>
+      <c r="F42">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A43" s="29"/>
+      <c r="B43" s="17" t="s">
+        <v>111</v>
+      </c>
+      <c r="C43" s="18" t="s">
+        <v>114</v>
+      </c>
+      <c r="D43" s="15">
+        <v>1</v>
+      </c>
+      <c r="F43">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A44" s="29"/>
+      <c r="B44" s="17" t="s">
+        <v>111</v>
+      </c>
+      <c r="C44" s="18" t="s">
+        <v>115</v>
+      </c>
+      <c r="D44" s="15">
+        <v>4</v>
+      </c>
+      <c r="F44">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" ht="18" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A45" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="B34" s="6"/>
-      <c r="C34" s="7"/>
-      <c r="D34" s="6"/>
-      <c r="E34" s="8"/>
-      <c r="F34">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="35" spans="1:6" ht="18" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="19" t="s">
+      <c r="B45" s="6"/>
+      <c r="C45" s="7"/>
+      <c r="D45" s="6"/>
+      <c r="E45" s="8"/>
+      <c r="F45">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" ht="18" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A46" s="19" t="s">
         <v>49</v>
       </c>
-      <c r="B35" s="17" t="s">
+      <c r="B46" s="17" t="s">
         <v>50</v>
-      </c>
-      <c r="C35" s="18"/>
-      <c r="D35" s="15">
-        <v>34</v>
-      </c>
-      <c r="F35">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A36" s="19" t="s">
-        <v>51</v>
-      </c>
-      <c r="B36" s="17" t="s">
-        <v>52</v>
-      </c>
-      <c r="C36" s="18"/>
-      <c r="D36" s="15">
-        <v>3</v>
-      </c>
-      <c r="F36">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A37" s="19" t="s">
-        <v>53</v>
-      </c>
-      <c r="B37" s="17" t="s">
-        <v>54</v>
-      </c>
-      <c r="C37" s="18"/>
-      <c r="D37" s="15">
-        <v>1</v>
-      </c>
-      <c r="F37">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A38" s="19" t="s">
-        <v>55</v>
-      </c>
-      <c r="B38" s="17" t="s">
-        <v>56</v>
-      </c>
-      <c r="C38" s="18"/>
-      <c r="D38" s="15">
-        <v>1.45</v>
-      </c>
-      <c r="F38">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="39" spans="1:6" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="A39" s="19" t="s">
-        <v>57</v>
-      </c>
-      <c r="B39" s="17" t="s">
-        <v>58</v>
-      </c>
-      <c r="C39" s="18"/>
-      <c r="D39" s="15">
-        <v>0.23100000000000001</v>
-      </c>
-      <c r="F39">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="40" spans="1:6" ht="18" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A40" s="5" t="s">
-        <v>59</v>
-      </c>
-      <c r="B40" s="6"/>
-      <c r="C40" s="7"/>
-      <c r="D40" s="6"/>
-      <c r="E40" s="8"/>
-      <c r="F40">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="41" spans="1:6" ht="30.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="19" t="s">
-        <v>60</v>
-      </c>
-      <c r="B41" s="17" t="s">
-        <v>61</v>
-      </c>
-      <c r="C41" s="18"/>
-      <c r="D41" s="15">
-        <v>4</v>
-      </c>
-      <c r="F41">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="42" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A42" s="19" t="s">
-        <v>62</v>
-      </c>
-      <c r="B42" s="17" t="s">
-        <v>63</v>
-      </c>
-      <c r="C42" s="18"/>
-      <c r="D42" s="15">
-        <v>0.5</v>
-      </c>
-      <c r="F42">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A43" s="19" t="s">
-        <v>64</v>
-      </c>
-      <c r="B43" s="17" t="s">
-        <v>65</v>
-      </c>
-      <c r="C43" s="18"/>
-      <c r="D43" s="15">
-        <v>0</v>
-      </c>
-      <c r="F43">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="44" spans="1:6" ht="18" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A44" s="5" t="s">
-        <v>66</v>
-      </c>
-      <c r="B44" s="6"/>
-      <c r="C44" s="7"/>
-      <c r="D44" s="6"/>
-      <c r="E44" s="8"/>
-      <c r="F44">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="45" spans="1:6" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="19" t="s">
-        <v>67</v>
-      </c>
-      <c r="B45" s="17" t="s">
-        <v>68</v>
-      </c>
-      <c r="C45" s="18"/>
-      <c r="D45" s="15">
-        <v>0.01</v>
-      </c>
-      <c r="F45">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="46" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A46" s="19" t="s">
-        <v>69</v>
-      </c>
-      <c r="B46" s="17" t="s">
-        <v>70</v>
       </c>
       <c r="C46" s="18"/>
       <c r="D46" s="15">
-        <v>365</v>
+        <v>34</v>
       </c>
       <c r="F46">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A47" s="19" t="s">
+        <v>51</v>
+      </c>
+      <c r="B47" s="17" t="s">
+        <v>52</v>
+      </c>
+      <c r="C47" s="18"/>
+      <c r="D47" s="15">
+        <v>3</v>
+      </c>
+      <c r="F47">
         <v>45</v>
       </c>
     </row>
-    <row r="47" spans="1:6" ht="18" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A47" s="5" t="s">
-        <v>71</v>
-      </c>
-      <c r="B47" s="6"/>
-      <c r="C47" s="7"/>
-      <c r="D47" s="6"/>
-      <c r="E47" s="8"/>
-      <c r="F47">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="48" spans="1:6" ht="30.75" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A48" s="19" t="s">
-        <v>72</v>
+        <v>53</v>
       </c>
       <c r="B48" s="17" t="s">
-        <v>73</v>
+        <v>54</v>
       </c>
       <c r="C48" s="18"/>
       <c r="D48" s="15">
-        <v>0.25</v>
-      </c>
-      <c r="E48" t="s">
-        <v>74</v>
+        <v>1</v>
       </c>
       <c r="F48">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="49" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A49" s="19" t="s">
-        <v>75</v>
+        <v>55</v>
       </c>
       <c r="B49" s="17" t="s">
-        <v>76</v>
+        <v>56</v>
       </c>
       <c r="C49" s="18"/>
       <c r="D49" s="15">
-        <v>0.25</v>
+        <v>1.45</v>
       </c>
       <c r="F49">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="A50" s="19" t="s">
+        <v>57</v>
+      </c>
+      <c r="B50" s="17" t="s">
+        <v>58</v>
+      </c>
+      <c r="C50" s="18"/>
+      <c r="D50" s="15">
+        <v>0.23100000000000001</v>
+      </c>
+      <c r="F50">
         <v>48</v>
       </c>
     </row>
-    <row r="50" spans="1:6" ht="18" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A50" s="5" t="s">
-        <v>77</v>
-      </c>
-      <c r="B50" s="6"/>
-      <c r="C50" s="7"/>
-      <c r="D50" s="6"/>
-      <c r="E50" s="8" t="s">
-        <v>78</v>
-      </c>
-      <c r="F50">
+    <row r="51" spans="1:6" ht="18" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A51" s="5" t="s">
+        <v>116</v>
+      </c>
+      <c r="B51" s="6"/>
+      <c r="C51" s="7"/>
+      <c r="D51" s="6"/>
+      <c r="E51" s="8"/>
+      <c r="F51">
         <v>49</v>
       </c>
     </row>
-    <row r="51" spans="1:6" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A51" s="19" t="s">
-        <v>79</v>
-      </c>
-      <c r="B51" s="17" t="s">
-        <v>80</v>
-      </c>
-      <c r="C51" s="18"/>
-      <c r="D51" s="12" t="s">
-        <v>81</v>
-      </c>
-      <c r="E51" t="s">
-        <v>82</v>
-      </c>
-      <c r="F51">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:6" ht="18.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A52" s="19" t="s">
-        <v>83</v>
+        <v>117</v>
       </c>
       <c r="B52" s="17" t="s">
-        <v>84</v>
+        <v>118</v>
       </c>
       <c r="C52" s="18"/>
       <c r="D52" s="15">
+        <v>180</v>
+      </c>
+      <c r="F52">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A53" s="19" t="s">
+        <v>59</v>
+      </c>
+      <c r="B53" s="17" t="s">
+        <v>120</v>
+      </c>
+      <c r="C53" s="18"/>
+      <c r="D53" s="15">
+        <v>4</v>
+      </c>
+      <c r="F53">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A54" s="19" t="s">
+        <v>60</v>
+      </c>
+      <c r="B54" s="17" t="s">
+        <v>121</v>
+      </c>
+      <c r="C54" s="18"/>
+      <c r="D54" s="15">
+        <v>0.5</v>
+      </c>
+      <c r="F54">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A55" s="19" t="s">
+        <v>61</v>
+      </c>
+      <c r="B55" s="17" t="s">
+        <v>122</v>
+      </c>
+      <c r="C55" s="18"/>
+      <c r="D55" s="15">
+        <v>0</v>
+      </c>
+      <c r="F55">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" ht="18" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A56" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="B56" s="7"/>
+      <c r="C56" s="7"/>
+      <c r="D56" s="6"/>
+      <c r="E56" s="8"/>
+      <c r="F56">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A57" s="19" t="s">
+        <v>63</v>
+      </c>
+      <c r="B57" s="17" t="s">
+        <v>64</v>
+      </c>
+      <c r="C57" s="18"/>
+      <c r="D57" s="15">
+        <v>0.01</v>
+      </c>
+      <c r="F57">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A58" s="19" t="s">
+        <v>65</v>
+      </c>
+      <c r="B58" s="17" t="s">
+        <v>66</v>
+      </c>
+      <c r="C58" s="18"/>
+      <c r="D58" s="15">
+        <v>365</v>
+      </c>
+      <c r="F58">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6" ht="18" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A59" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="B59" s="6"/>
+      <c r="C59" s="7"/>
+      <c r="D59" s="6"/>
+      <c r="E59" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="F59">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A60" s="19" t="s">
+        <v>69</v>
+      </c>
+      <c r="B60" s="17" t="s">
+        <v>70</v>
+      </c>
+      <c r="C60" s="18"/>
+      <c r="D60" s="12" t="s">
+        <v>71</v>
+      </c>
+      <c r="E60" t="s">
+        <v>72</v>
+      </c>
+      <c r="F60">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A61" s="19" t="s">
+        <v>73</v>
+      </c>
+      <c r="B61" s="17" t="s">
+        <v>74</v>
+      </c>
+      <c r="C61" s="18"/>
+      <c r="D61" s="15">
         <v>207</v>
       </c>
-      <c r="F52">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A53" s="19" t="s">
-        <v>85</v>
-      </c>
-      <c r="B53" s="17" t="s">
-        <v>86</v>
-      </c>
-      <c r="C53" s="18">
+      <c r="F61">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A62" s="19" t="s">
+        <v>75</v>
+      </c>
+      <c r="B62" s="17" t="s">
+        <v>76</v>
+      </c>
+      <c r="C62" s="18">
         <v>1</v>
       </c>
-      <c r="D53" s="15">
+      <c r="D62" s="15">
         <v>30</v>
       </c>
-      <c r="F53">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A54" s="19"/>
-      <c r="B54" s="17" t="s">
-        <v>86</v>
-      </c>
-      <c r="C54" s="18">
+      <c r="F62">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A63" s="19"/>
+      <c r="B63" s="17" t="s">
+        <v>76</v>
+      </c>
+      <c r="C63" s="18">
         <v>2</v>
       </c>
-      <c r="D54" s="15">
+      <c r="D63" s="15">
         <v>40</v>
       </c>
-      <c r="F54">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A55" s="19"/>
-      <c r="B55" s="17" t="s">
-        <v>86</v>
-      </c>
-      <c r="C55" s="18">
-        <v>3</v>
-      </c>
-      <c r="D55" s="15">
-        <v>50</v>
-      </c>
-      <c r="F55">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A56" s="19"/>
-      <c r="B56" s="17" t="s">
-        <v>86</v>
-      </c>
-      <c r="C56" s="18">
-        <v>4</v>
-      </c>
-      <c r="D56" s="15"/>
-      <c r="F56">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A57" s="19"/>
-      <c r="B57" s="17" t="s">
-        <v>86</v>
-      </c>
-      <c r="C57" s="18">
-        <v>5</v>
-      </c>
-      <c r="D57" s="15"/>
-      <c r="F57">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A58" s="19" t="s">
-        <v>87</v>
-      </c>
-      <c r="B58" s="17" t="s">
-        <v>88</v>
-      </c>
-      <c r="C58" s="18">
-        <v>1</v>
-      </c>
-      <c r="D58" s="15">
-        <v>0.01</v>
-      </c>
-      <c r="F58">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A59" s="19"/>
-      <c r="B59" s="17" t="s">
-        <v>88</v>
-      </c>
-      <c r="C59" s="18">
-        <v>2</v>
-      </c>
-      <c r="D59" s="15">
-        <v>0.25</v>
-      </c>
-      <c r="F59">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A60" s="19"/>
-      <c r="B60" s="17" t="s">
-        <v>88</v>
-      </c>
-      <c r="C60" s="18">
-        <v>3</v>
-      </c>
-      <c r="D60" s="15">
-        <v>0.67</v>
-      </c>
-      <c r="F60">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A61" s="19"/>
-      <c r="B61" s="17" t="s">
-        <v>88</v>
-      </c>
-      <c r="C61" s="18">
-        <v>4</v>
-      </c>
-      <c r="D61" s="15"/>
-      <c r="F61">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A62" s="19"/>
-      <c r="B62" s="17" t="s">
-        <v>88</v>
-      </c>
-      <c r="C62" s="18">
-        <v>5</v>
-      </c>
-      <c r="D62" s="15"/>
-      <c r="F62">
+      <c r="F63">
         <v>61</v>
-      </c>
-    </row>
-    <row r="63" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A63" s="19" t="s">
-        <v>89</v>
-      </c>
-      <c r="B63" s="17" t="s">
-        <v>90</v>
-      </c>
-      <c r="C63" s="18">
-        <v>1</v>
-      </c>
-      <c r="D63" s="15">
-        <v>1</v>
-      </c>
-      <c r="F63">
-        <v>62</v>
       </c>
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A64" s="19"/>
       <c r="B64" s="17" t="s">
-        <v>90</v>
+        <v>76</v>
       </c>
       <c r="C64" s="18">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D64" s="15">
-        <v>1</v>
+        <v>50</v>
       </c>
       <c r="F64">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A65" s="19"/>
       <c r="B65" s="17" t="s">
-        <v>90</v>
+        <v>76</v>
       </c>
       <c r="C65" s="18">
-        <v>3</v>
-      </c>
-      <c r="D65" s="15">
-        <v>1</v>
-      </c>
+        <v>4</v>
+      </c>
+      <c r="D65" s="15"/>
       <c r="F65">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="66" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A66" s="19"/>
       <c r="B66" s="17" t="s">
-        <v>90</v>
+        <v>76</v>
       </c>
       <c r="C66" s="18">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D66" s="15"/>
       <c r="F66">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="67" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A67" s="19" t="s">
+        <v>77</v>
+      </c>
+      <c r="B67" s="17" t="s">
+        <v>78</v>
+      </c>
+      <c r="C67" s="18">
+        <v>1</v>
+      </c>
+      <c r="D67" s="15">
+        <v>0.01</v>
+      </c>
+      <c r="F67">
         <v>65</v>
       </c>
     </row>
-    <row r="67" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A67" s="19"/>
-      <c r="B67" s="17" t="s">
-        <v>90</v>
-      </c>
-      <c r="C67" s="18">
-        <v>5</v>
-      </c>
-      <c r="D67" s="15"/>
-      <c r="F67">
+    <row r="68" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A68" s="19"/>
+      <c r="B68" s="17" t="s">
+        <v>78</v>
+      </c>
+      <c r="C68" s="18">
+        <v>2</v>
+      </c>
+      <c r="D68" s="15">
+        <v>0.25</v>
+      </c>
+      <c r="F68">
         <v>66</v>
       </c>
     </row>
-    <row r="68" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A68" s="19" t="s">
-        <v>91</v>
-      </c>
-      <c r="B68" s="17" t="s">
-        <v>92</v>
-      </c>
-      <c r="C68" s="18"/>
-      <c r="D68" s="12" t="s">
-        <v>93</v>
-      </c>
-      <c r="F68">
+    <row r="69" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A69" s="19"/>
+      <c r="B69" s="17" t="s">
+        <v>78</v>
+      </c>
+      <c r="C69" s="18">
+        <v>3</v>
+      </c>
+      <c r="D69" s="15">
+        <v>0.67</v>
+      </c>
+      <c r="F69">
         <v>67</v>
       </c>
     </row>
-    <row r="69" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A69" s="19" t="s">
-        <v>94</v>
-      </c>
-      <c r="B69" s="17" t="s">
-        <v>95</v>
-      </c>
-      <c r="C69" s="18"/>
-      <c r="D69" s="15">
-        <v>365</v>
-      </c>
-      <c r="F69">
+    <row r="70" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A70" s="19"/>
+      <c r="B70" s="17" t="s">
+        <v>78</v>
+      </c>
+      <c r="C70" s="18">
+        <v>4</v>
+      </c>
+      <c r="D70" s="15"/>
+      <c r="F70">
         <v>68</v>
-      </c>
-    </row>
-    <row r="70" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A70" s="19" t="s">
-        <v>96</v>
-      </c>
-      <c r="B70" s="17" t="s">
-        <v>97</v>
-      </c>
-      <c r="C70" s="18">
-        <v>1</v>
-      </c>
-      <c r="D70" s="15">
-        <v>0</v>
-      </c>
-      <c r="F70">
-        <v>69</v>
       </c>
     </row>
     <row r="71" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A71" s="19"/>
       <c r="B71" s="17" t="s">
-        <v>97</v>
+        <v>78</v>
       </c>
       <c r="C71" s="18">
-        <v>2</v>
-      </c>
-      <c r="D71" s="15">
-        <v>0.2</v>
-      </c>
+        <v>5</v>
+      </c>
+      <c r="D71" s="15"/>
       <c r="F71">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="72" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A72" s="19" t="s">
+        <v>79</v>
+      </c>
+      <c r="B72" s="17" t="s">
+        <v>80</v>
+      </c>
+      <c r="C72" s="18">
+        <v>1</v>
+      </c>
+      <c r="D72" s="15">
+        <v>1</v>
+      </c>
+      <c r="F72">
         <v>70</v>
-      </c>
-    </row>
-    <row r="72" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A72" s="19"/>
-      <c r="B72" s="17" t="s">
-        <v>97</v>
-      </c>
-      <c r="C72" s="18">
-        <v>3</v>
-      </c>
-      <c r="D72" s="15">
-        <v>0.5</v>
-      </c>
-      <c r="F72">
-        <v>71</v>
       </c>
     </row>
     <row r="73" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A73" s="19"/>
       <c r="B73" s="17" t="s">
-        <v>97</v>
+        <v>80</v>
       </c>
       <c r="C73" s="18">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="D73" s="15">
-        <v>0.68</v>
+        <v>1</v>
       </c>
       <c r="F73">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="74" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A74" s="19"/>
       <c r="B74" s="17" t="s">
-        <v>97</v>
+        <v>80</v>
       </c>
       <c r="C74" s="18">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D74" s="15">
-        <v>1.1200000000000001</v>
+        <v>1</v>
       </c>
       <c r="F74">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="75" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A75" s="19"/>
+      <c r="B75" s="17" t="s">
+        <v>80</v>
+      </c>
+      <c r="C75" s="18">
+        <v>4</v>
+      </c>
+      <c r="D75" s="15"/>
+      <c r="F75">
         <v>73</v>
-      </c>
-    </row>
-    <row r="75" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A75" s="19" t="s">
-        <v>98</v>
-      </c>
-      <c r="B75" s="17" t="s">
-        <v>99</v>
-      </c>
-      <c r="C75" s="18">
-        <v>1</v>
-      </c>
-      <c r="D75" s="15">
-        <v>0</v>
-      </c>
-      <c r="F75">
-        <v>74</v>
       </c>
     </row>
     <row r="76" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A76" s="19"/>
       <c r="B76" s="17" t="s">
-        <v>99</v>
+        <v>80</v>
       </c>
       <c r="C76" s="18">
+        <v>5</v>
+      </c>
+      <c r="D76" s="15"/>
+      <c r="F76">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="77" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A77" s="19" t="s">
+        <v>81</v>
+      </c>
+      <c r="B77" s="17" t="s">
+        <v>82</v>
+      </c>
+      <c r="C77" s="18"/>
+      <c r="D77" s="12" t="s">
+        <v>83</v>
+      </c>
+      <c r="F77">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="78" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A78" s="19" t="s">
+        <v>84</v>
+      </c>
+      <c r="B78" s="17" t="s">
+        <v>85</v>
+      </c>
+      <c r="C78" s="18"/>
+      <c r="D78" s="15">
+        <v>365</v>
+      </c>
+      <c r="F78">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="79" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A79" s="19" t="s">
+        <v>86</v>
+      </c>
+      <c r="B79" s="17" t="s">
+        <v>87</v>
+      </c>
+      <c r="C79" s="18">
+        <v>1</v>
+      </c>
+      <c r="D79" s="15">
+        <v>0</v>
+      </c>
+      <c r="F79">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="80" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A80" s="19"/>
+      <c r="B80" s="17" t="s">
+        <v>87</v>
+      </c>
+      <c r="C80" s="18">
         <v>2</v>
       </c>
-      <c r="D76" s="15">
-        <v>0</v>
-      </c>
-      <c r="F76">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="77" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A77" s="19"/>
-      <c r="B77" s="17" t="s">
-        <v>99</v>
-      </c>
-      <c r="C77" s="18">
-        <v>3</v>
-      </c>
-      <c r="D77" s="15">
-        <v>0</v>
-      </c>
-      <c r="F77">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="78" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A78" s="19"/>
-      <c r="B78" s="17" t="s">
-        <v>99</v>
-      </c>
-      <c r="C78" s="18">
-        <v>4</v>
-      </c>
-      <c r="D78" s="15">
-        <v>1</v>
-      </c>
-      <c r="F78">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="79" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A79" s="19"/>
-      <c r="B79" s="17" t="s">
-        <v>99</v>
-      </c>
-      <c r="C79" s="18">
-        <v>5</v>
-      </c>
-      <c r="D79" s="15">
-        <v>1</v>
-      </c>
-      <c r="F79">
+      <c r="D80" s="15">
+        <v>0.2</v>
+      </c>
+      <c r="F80">
         <v>78</v>
-      </c>
-    </row>
-    <row r="80" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A80" s="19" t="s">
-        <v>100</v>
-      </c>
-      <c r="B80" s="17" t="s">
-        <v>101</v>
-      </c>
-      <c r="C80" s="18">
-        <v>1</v>
-      </c>
-      <c r="D80" s="15">
-        <v>500</v>
-      </c>
-      <c r="F80">
-        <v>79</v>
       </c>
     </row>
     <row r="81" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A81" s="19"/>
       <c r="B81" s="17" t="s">
-        <v>101</v>
+        <v>87</v>
       </c>
       <c r="C81" s="18">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D81" s="15">
-        <v>300</v>
+        <v>0.5</v>
       </c>
       <c r="F81">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="82" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A82" s="19"/>
       <c r="B82" s="17" t="s">
-        <v>101</v>
+        <v>87</v>
       </c>
       <c r="C82" s="18">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D82" s="15">
-        <v>200</v>
+        <v>0.68</v>
       </c>
       <c r="F82">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="83" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A83" s="19"/>
       <c r="B83" s="17" t="s">
-        <v>101</v>
+        <v>87</v>
       </c>
       <c r="C83" s="18">
+        <v>5</v>
+      </c>
+      <c r="D83" s="15">
+        <v>1.1200000000000001</v>
+      </c>
+      <c r="F83">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="84" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A84" s="19" t="s">
+        <v>88</v>
+      </c>
+      <c r="B84" s="17" t="s">
+        <v>89</v>
+      </c>
+      <c r="C84" s="18">
+        <v>1</v>
+      </c>
+      <c r="D84" s="15">
+        <v>0</v>
+      </c>
+      <c r="F84">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="85" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A85" s="19"/>
+      <c r="B85" s="17" t="s">
+        <v>89</v>
+      </c>
+      <c r="C85" s="18">
+        <v>2</v>
+      </c>
+      <c r="D85" s="15">
+        <v>0</v>
+      </c>
+      <c r="F85">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="86" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A86" s="19"/>
+      <c r="B86" s="17" t="s">
+        <v>89</v>
+      </c>
+      <c r="C86" s="18">
+        <v>3</v>
+      </c>
+      <c r="D86" s="15">
+        <v>0</v>
+      </c>
+      <c r="F86">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="87" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A87" s="19"/>
+      <c r="B87" s="17" t="s">
+        <v>89</v>
+      </c>
+      <c r="C87" s="18">
         <v>4</v>
       </c>
-      <c r="D83" s="15">
+      <c r="D87" s="15">
+        <v>1</v>
+      </c>
+      <c r="F87">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="88" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A88" s="19"/>
+      <c r="B88" s="17" t="s">
+        <v>89</v>
+      </c>
+      <c r="C88" s="18">
+        <v>5</v>
+      </c>
+      <c r="D88" s="15">
+        <v>1</v>
+      </c>
+      <c r="F88">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="89" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A89" s="19" t="s">
+        <v>90</v>
+      </c>
+      <c r="B89" s="17" t="s">
+        <v>91</v>
+      </c>
+      <c r="C89" s="18">
+        <v>1</v>
+      </c>
+      <c r="D89" s="15">
+        <v>500</v>
+      </c>
+      <c r="F89">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="90" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A90" s="19"/>
+      <c r="B90" s="17" t="s">
+        <v>91</v>
+      </c>
+      <c r="C90" s="18">
+        <v>2</v>
+      </c>
+      <c r="D90" s="15">
+        <v>300</v>
+      </c>
+      <c r="F90">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="91" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A91" s="19"/>
+      <c r="B91" s="17" t="s">
+        <v>91</v>
+      </c>
+      <c r="C91" s="18">
+        <v>3</v>
+      </c>
+      <c r="D91" s="15">
         <v>200</v>
       </c>
-      <c r="F83">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="84" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A84" s="19"/>
-      <c r="B84" s="17" t="s">
-        <v>101</v>
-      </c>
-      <c r="C84" s="18">
+      <c r="F91">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="92" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A92" s="19"/>
+      <c r="B92" s="17" t="s">
+        <v>91</v>
+      </c>
+      <c r="C92" s="18">
+        <v>4</v>
+      </c>
+      <c r="D92" s="15">
+        <v>200</v>
+      </c>
+      <c r="F92">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="93" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A93" s="19"/>
+      <c r="B93" s="17" t="s">
+        <v>91</v>
+      </c>
+      <c r="C93" s="18">
         <v>5</v>
       </c>
-      <c r="D84" s="15">
+      <c r="D93" s="15">
         <v>300</v>
       </c>
-      <c r="F84">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="85" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A85" s="20"/>
-      <c r="B85" s="21"/>
-      <c r="C85" s="22"/>
-    </row>
-    <row r="86" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A86" s="20"/>
-      <c r="B86" s="21"/>
-      <c r="C86" s="22"/>
-    </row>
-    <row r="87" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A87" s="20"/>
-      <c r="B87" s="21"/>
-      <c r="C87" s="22"/>
-    </row>
-    <row r="88" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A88" s="20"/>
-      <c r="B88" s="21"/>
-      <c r="C88" s="22"/>
-    </row>
-    <row r="89" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A89" s="20"/>
-      <c r="B89" s="21"/>
-      <c r="C89" s="22"/>
-    </row>
-    <row r="90" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A90" s="20"/>
-      <c r="B90" s="21"/>
-      <c r="C90" s="22"/>
-    </row>
-    <row r="91" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A91" s="20"/>
-      <c r="B91" s="21"/>
-      <c r="C91" s="22"/>
-    </row>
-    <row r="92" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A92" s="20"/>
-      <c r="B92" s="21"/>
-      <c r="C92" s="22"/>
-    </row>
-    <row r="93" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A93" s="20"/>
-      <c r="B93" s="21"/>
-      <c r="C93" s="22"/>
+      <c r="F93">
+        <v>91</v>
+      </c>
     </row>
     <row r="94" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A94" s="20"/>
@@ -4883,12 +5125,58 @@
       <c r="B204" s="21"/>
       <c r="C204" s="22"/>
     </row>
+    <row r="205" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A205" s="20"/>
+      <c r="B205" s="21"/>
+      <c r="C205" s="22"/>
+    </row>
+    <row r="206" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A206" s="20"/>
+      <c r="B206" s="21"/>
+      <c r="C206" s="22"/>
+    </row>
+    <row r="207" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A207" s="20"/>
+      <c r="B207" s="21"/>
+      <c r="C207" s="22"/>
+    </row>
+    <row r="208" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A208" s="20"/>
+      <c r="B208" s="21"/>
+      <c r="C208" s="22"/>
+    </row>
+    <row r="209" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A209" s="20"/>
+      <c r="B209" s="21"/>
+      <c r="C209" s="22"/>
+    </row>
+    <row r="210" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A210" s="20"/>
+      <c r="B210" s="21"/>
+      <c r="C210" s="22"/>
+    </row>
+    <row r="211" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A211" s="20"/>
+      <c r="B211" s="21"/>
+      <c r="C211" s="22"/>
+    </row>
+    <row r="212" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A212" s="20"/>
+      <c r="B212" s="21"/>
+      <c r="C212" s="22"/>
+    </row>
+    <row r="213" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A213" s="20"/>
+      <c r="B213" s="21"/>
+      <c r="C213" s="22"/>
+    </row>
   </sheetData>
-  <mergeCells count="4">
-    <mergeCell ref="A16:A18"/>
-    <mergeCell ref="A19:A21"/>
-    <mergeCell ref="A25:A30"/>
-    <mergeCell ref="A31:A33"/>
+  <mergeCells count="5">
+    <mergeCell ref="A29:A34"/>
+    <mergeCell ref="A40:A44"/>
+    <mergeCell ref="A16:A20"/>
+    <mergeCell ref="A21:A25"/>
+    <mergeCell ref="A35:A39"/>
   </mergeCells>
   <dataValidations count="13">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D7" xr:uid="{76366DFC-F994-4B24-8F58-3C475A37D29A}">
@@ -4904,11 +5192,11 @@
       <formula1>1</formula1>
       <formula2>366</formula2>
     </dataValidation>
-    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D22 D42:D45 D47:D50" xr:uid="{99673017-9BA7-4007-B122-EE6B62E8329F}">
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D26 D54:D57 D59" xr:uid="{99673017-9BA7-4007-B122-EE6B62E8329F}">
       <formula1>0</formula1>
       <formula2>1</formula2>
     </dataValidation>
-    <dataValidation type="whole" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D46" xr:uid="{AD51276E-9E22-4C8A-A243-458D6265E1F0}">
+    <dataValidation type="whole" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D58" xr:uid="{AD51276E-9E22-4C8A-A243-458D6265E1F0}">
       <formula1>0</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D6" xr:uid="{9966BE53-3AF7-47D9-9DC3-79C6924CF42E}">

</xml_diff>

<commit_message>
Changed how nested dictionaries are built #broken
</commit_message>
<xml_diff>
--- a/notebooks/GenVeg/GenVeg_Example_Simulation.xlsx
+++ b/notebooks/GenVeg/GenVeg_Example_Simulation.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Python\landlab\notebooks\GenVeg\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A69C6B99-D6C7-42DA-B9DC-D9A4C803A581}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5EE6CACA-7F5A-40ED-9292-B4C1C0E55F9A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{4FA2BB3E-4334-4C54-90D8-DFF869504B66}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="360" uniqueCount="123">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="348" uniqueCount="126">
   <si>
     <t>Parameter</t>
   </si>
@@ -565,6 +565,15 @@
   </si>
   <si>
     <t>carb_cost_dispersal</t>
+  </si>
+  <si>
+    <t>predictor</t>
+  </si>
+  <si>
+    <t>response</t>
+  </si>
+  <si>
+    <t>mort_variable_name</t>
   </si>
 </sst>
 </file>
@@ -3164,10 +3173,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7A5B2ED1-E60A-481E-A183-520033C5AF7F}">
-  <dimension ref="A1:G213"/>
+  <dimension ref="A1:G203"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A38" workbookViewId="0">
-      <selection activeCell="J54" sqref="J54"/>
+    <sheetView tabSelected="1" topLeftCell="A58" workbookViewId="0">
+      <selection activeCell="D82" sqref="D82"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4062,9 +4071,11 @@
         <v>69</v>
       </c>
       <c r="B60" s="17" t="s">
-        <v>70</v>
-      </c>
-      <c r="C60" s="18"/>
+        <v>125</v>
+      </c>
+      <c r="C60" s="18">
+        <v>1</v>
+      </c>
       <c r="D60" s="12" t="s">
         <v>71</v>
       </c>
@@ -4080,9 +4091,11 @@
         <v>73</v>
       </c>
       <c r="B61" s="17" t="s">
-        <v>74</v>
-      </c>
-      <c r="C61" s="18"/>
+        <v>105</v>
+      </c>
+      <c r="C61" s="18">
+        <v>1</v>
+      </c>
       <c r="D61" s="15">
         <v>207</v>
       </c>
@@ -4095,7 +4108,7 @@
         <v>75</v>
       </c>
       <c r="B62" s="17" t="s">
-        <v>76</v>
+        <v>123</v>
       </c>
       <c r="C62" s="18">
         <v>1</v>
@@ -4110,10 +4123,10 @@
     <row r="63" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A63" s="19"/>
       <c r="B63" s="17" t="s">
-        <v>76</v>
+        <v>123</v>
       </c>
       <c r="C63" s="18">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D63" s="15">
         <v>40</v>
@@ -4125,10 +4138,10 @@
     <row r="64" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A64" s="19"/>
       <c r="B64" s="17" t="s">
-        <v>76</v>
+        <v>123</v>
       </c>
       <c r="C64" s="18">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D64" s="15">
         <v>50</v>
@@ -4140,10 +4153,10 @@
     <row r="65" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A65" s="19"/>
       <c r="B65" s="17" t="s">
-        <v>76</v>
+        <v>123</v>
       </c>
       <c r="C65" s="18">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="D65" s="15"/>
       <c r="F65">
@@ -4153,10 +4166,10 @@
     <row r="66" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A66" s="19"/>
       <c r="B66" s="17" t="s">
-        <v>76</v>
+        <v>123</v>
       </c>
       <c r="C66" s="18">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="D66" s="15"/>
       <c r="F66">
@@ -4168,7 +4181,7 @@
         <v>77</v>
       </c>
       <c r="B67" s="17" t="s">
-        <v>78</v>
+        <v>124</v>
       </c>
       <c r="C67" s="18">
         <v>1</v>
@@ -4183,10 +4196,10 @@
     <row r="68" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A68" s="19"/>
       <c r="B68" s="17" t="s">
-        <v>78</v>
+        <v>124</v>
       </c>
       <c r="C68" s="18">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D68" s="15">
         <v>0.25</v>
@@ -4198,10 +4211,10 @@
     <row r="69" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A69" s="19"/>
       <c r="B69" s="17" t="s">
-        <v>78</v>
+        <v>124</v>
       </c>
       <c r="C69" s="18">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D69" s="15">
         <v>0.67</v>
@@ -4213,10 +4226,10 @@
     <row r="70" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A70" s="19"/>
       <c r="B70" s="17" t="s">
-        <v>78</v>
+        <v>124</v>
       </c>
       <c r="C70" s="18">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="D70" s="15"/>
       <c r="F70">
@@ -4226,349 +4239,253 @@
     <row r="71" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A71" s="19"/>
       <c r="B71" s="17" t="s">
-        <v>78</v>
+        <v>124</v>
       </c>
       <c r="C71" s="18">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="D71" s="15"/>
       <c r="F71">
         <v>69</v>
       </c>
     </row>
-    <row r="72" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A72" s="19" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="B72" s="17" t="s">
-        <v>80</v>
+        <v>125</v>
       </c>
       <c r="C72" s="18">
-        <v>1</v>
-      </c>
-      <c r="D72" s="15">
-        <v>1</v>
+        <v>2</v>
+      </c>
+      <c r="D72" s="12" t="s">
+        <v>83</v>
       </c>
       <c r="F72">
-        <v>70</v>
+        <v>75</v>
       </c>
     </row>
     <row r="73" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A73" s="19"/>
+      <c r="A73" s="19" t="s">
+        <v>84</v>
+      </c>
       <c r="B73" s="17" t="s">
-        <v>80</v>
+        <v>105</v>
       </c>
       <c r="C73" s="18">
         <v>2</v>
       </c>
       <c r="D73" s="15">
-        <v>1</v>
+        <v>365</v>
       </c>
       <c r="F73">
-        <v>71</v>
+        <v>76</v>
       </c>
     </row>
     <row r="74" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A74" s="19"/>
+      <c r="A74" s="19" t="s">
+        <v>86</v>
+      </c>
       <c r="B74" s="17" t="s">
-        <v>80</v>
+        <v>123</v>
       </c>
       <c r="C74" s="18">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D74" s="15">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F74">
-        <v>72</v>
+        <v>77</v>
       </c>
     </row>
     <row r="75" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A75" s="19"/>
       <c r="B75" s="17" t="s">
-        <v>80</v>
+        <v>123</v>
       </c>
       <c r="C75" s="18">
-        <v>4</v>
-      </c>
-      <c r="D75" s="15"/>
+        <v>2</v>
+      </c>
+      <c r="D75" s="15">
+        <v>0.5</v>
+      </c>
       <c r="F75">
-        <v>73</v>
+        <v>78</v>
       </c>
     </row>
     <row r="76" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A76" s="19"/>
       <c r="B76" s="17" t="s">
+        <v>123</v>
+      </c>
+      <c r="C76" s="18">
+        <v>2</v>
+      </c>
+      <c r="D76" s="15">
+        <v>0.6</v>
+      </c>
+      <c r="F76">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="77" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A77" s="19"/>
+      <c r="B77" s="17" t="s">
+        <v>123</v>
+      </c>
+      <c r="C77" s="18">
+        <v>2</v>
+      </c>
+      <c r="D77" s="15">
+        <v>0.68</v>
+      </c>
+      <c r="F77">
         <v>80</v>
       </c>
-      <c r="C76" s="18">
-        <v>5</v>
-      </c>
-      <c r="D76" s="15"/>
-      <c r="F76">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="77" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A77" s="19" t="s">
+    </row>
+    <row r="78" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A78" s="19"/>
+      <c r="B78" s="17" t="s">
+        <v>123</v>
+      </c>
+      <c r="C78" s="18">
+        <v>2</v>
+      </c>
+      <c r="D78" s="15">
+        <v>1.1200000000000001</v>
+      </c>
+      <c r="F78">
         <v>81</v>
-      </c>
-      <c r="B77" s="17" t="s">
-        <v>82</v>
-      </c>
-      <c r="C77" s="18"/>
-      <c r="D77" s="12" t="s">
-        <v>83</v>
-      </c>
-      <c r="F77">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="78" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A78" s="19" t="s">
-        <v>84</v>
-      </c>
-      <c r="B78" s="17" t="s">
-        <v>85</v>
-      </c>
-      <c r="C78" s="18"/>
-      <c r="D78" s="15">
-        <v>365</v>
-      </c>
-      <c r="F78">
-        <v>76</v>
       </c>
     </row>
     <row r="79" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A79" s="19" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="B79" s="17" t="s">
-        <v>87</v>
+        <v>124</v>
       </c>
       <c r="C79" s="18">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D79" s="15">
         <v>0</v>
       </c>
       <c r="F79">
-        <v>77</v>
+        <v>82</v>
       </c>
     </row>
     <row r="80" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A80" s="19"/>
       <c r="B80" s="17" t="s">
-        <v>87</v>
+        <v>124</v>
       </c>
       <c r="C80" s="18">
         <v>2</v>
       </c>
       <c r="D80" s="15">
-        <v>0.2</v>
+        <v>0</v>
       </c>
       <c r="F80">
-        <v>78</v>
+        <v>83</v>
       </c>
     </row>
     <row r="81" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A81" s="19"/>
       <c r="B81" s="17" t="s">
-        <v>87</v>
+        <v>124</v>
       </c>
       <c r="C81" s="18">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D81" s="15">
-        <v>0.5</v>
+        <v>0.3</v>
       </c>
       <c r="F81">
-        <v>79</v>
+        <v>84</v>
       </c>
     </row>
     <row r="82" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A82" s="19"/>
       <c r="B82" s="17" t="s">
-        <v>87</v>
+        <v>124</v>
       </c>
       <c r="C82" s="18">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="D82" s="15">
-        <v>0.68</v>
+        <v>1</v>
       </c>
       <c r="F82">
-        <v>80</v>
+        <v>85</v>
       </c>
     </row>
     <row r="83" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A83" s="19"/>
       <c r="B83" s="17" t="s">
-        <v>87</v>
+        <v>124</v>
       </c>
       <c r="C83" s="18">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="D83" s="15">
-        <v>1.1200000000000001</v>
+        <v>1</v>
       </c>
       <c r="F83">
-        <v>81</v>
+        <v>86</v>
       </c>
     </row>
     <row r="84" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A84" s="19" t="s">
-        <v>88</v>
-      </c>
-      <c r="B84" s="17" t="s">
-        <v>89</v>
-      </c>
-      <c r="C84" s="18">
-        <v>1</v>
-      </c>
-      <c r="D84" s="15">
-        <v>0</v>
-      </c>
-      <c r="F84">
-        <v>82</v>
-      </c>
+      <c r="A84" s="20"/>
+      <c r="B84" s="21"/>
+      <c r="C84" s="22"/>
     </row>
     <row r="85" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A85" s="19"/>
-      <c r="B85" s="17" t="s">
-        <v>89</v>
-      </c>
-      <c r="C85" s="18">
-        <v>2</v>
-      </c>
-      <c r="D85" s="15">
-        <v>0</v>
-      </c>
-      <c r="F85">
-        <v>83</v>
-      </c>
+      <c r="A85" s="20"/>
+      <c r="B85" s="21"/>
+      <c r="C85" s="22"/>
     </row>
     <row r="86" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A86" s="19"/>
-      <c r="B86" s="17" t="s">
-        <v>89</v>
-      </c>
-      <c r="C86" s="18">
-        <v>3</v>
-      </c>
-      <c r="D86" s="15">
-        <v>0</v>
-      </c>
-      <c r="F86">
-        <v>84</v>
-      </c>
+      <c r="A86" s="20"/>
+      <c r="B86" s="21"/>
+      <c r="C86" s="22"/>
     </row>
     <row r="87" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A87" s="19"/>
-      <c r="B87" s="17" t="s">
-        <v>89</v>
-      </c>
-      <c r="C87" s="18">
-        <v>4</v>
-      </c>
-      <c r="D87" s="15">
-        <v>1</v>
-      </c>
-      <c r="F87">
-        <v>85</v>
-      </c>
+      <c r="A87" s="20"/>
+      <c r="B87" s="21"/>
+      <c r="C87" s="22"/>
     </row>
     <row r="88" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A88" s="19"/>
-      <c r="B88" s="17" t="s">
-        <v>89</v>
-      </c>
-      <c r="C88" s="18">
-        <v>5</v>
-      </c>
-      <c r="D88" s="15">
-        <v>1</v>
-      </c>
-      <c r="F88">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="89" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A89" s="19" t="s">
-        <v>90</v>
-      </c>
-      <c r="B89" s="17" t="s">
-        <v>91</v>
-      </c>
-      <c r="C89" s="18">
-        <v>1</v>
-      </c>
-      <c r="D89" s="15">
-        <v>500</v>
-      </c>
-      <c r="F89">
-        <v>87</v>
-      </c>
+      <c r="A88" s="20"/>
+      <c r="B88" s="21"/>
+      <c r="C88" s="22"/>
+    </row>
+    <row r="89" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A89" s="20"/>
+      <c r="B89" s="21"/>
+      <c r="C89" s="22"/>
     </row>
     <row r="90" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A90" s="19"/>
-      <c r="B90" s="17" t="s">
-        <v>91</v>
-      </c>
-      <c r="C90" s="18">
-        <v>2</v>
-      </c>
-      <c r="D90" s="15">
-        <v>300</v>
-      </c>
-      <c r="F90">
-        <v>88</v>
-      </c>
+      <c r="A90" s="20"/>
+      <c r="B90" s="21"/>
+      <c r="C90" s="22"/>
     </row>
     <row r="91" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A91" s="19"/>
-      <c r="B91" s="17" t="s">
-        <v>91</v>
-      </c>
-      <c r="C91" s="18">
-        <v>3</v>
-      </c>
-      <c r="D91" s="15">
-        <v>200</v>
-      </c>
-      <c r="F91">
-        <v>89</v>
-      </c>
+      <c r="A91" s="20"/>
+      <c r="B91" s="21"/>
+      <c r="C91" s="22"/>
     </row>
     <row r="92" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A92" s="19"/>
-      <c r="B92" s="17" t="s">
-        <v>91</v>
-      </c>
-      <c r="C92" s="18">
-        <v>4</v>
-      </c>
-      <c r="D92" s="15">
-        <v>200</v>
-      </c>
-      <c r="F92">
-        <v>90</v>
-      </c>
+      <c r="A92" s="20"/>
+      <c r="B92" s="21"/>
+      <c r="C92" s="22"/>
     </row>
     <row r="93" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A93" s="19"/>
-      <c r="B93" s="17" t="s">
-        <v>91</v>
-      </c>
-      <c r="C93" s="18">
-        <v>5</v>
-      </c>
-      <c r="D93" s="15">
-        <v>300</v>
-      </c>
-      <c r="F93">
-        <v>91</v>
-      </c>
+      <c r="A93" s="20"/>
+      <c r="B93" s="21"/>
+      <c r="C93" s="22"/>
     </row>
     <row r="94" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A94" s="20"/>
@@ -5119,56 +5036,6 @@
       <c r="A203" s="20"/>
       <c r="B203" s="21"/>
       <c r="C203" s="22"/>
-    </row>
-    <row r="204" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A204" s="20"/>
-      <c r="B204" s="21"/>
-      <c r="C204" s="22"/>
-    </row>
-    <row r="205" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A205" s="20"/>
-      <c r="B205" s="21"/>
-      <c r="C205" s="22"/>
-    </row>
-    <row r="206" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A206" s="20"/>
-      <c r="B206" s="21"/>
-      <c r="C206" s="22"/>
-    </row>
-    <row r="207" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A207" s="20"/>
-      <c r="B207" s="21"/>
-      <c r="C207" s="22"/>
-    </row>
-    <row r="208" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A208" s="20"/>
-      <c r="B208" s="21"/>
-      <c r="C208" s="22"/>
-    </row>
-    <row r="209" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A209" s="20"/>
-      <c r="B209" s="21"/>
-      <c r="C209" s="22"/>
-    </row>
-    <row r="210" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A210" s="20"/>
-      <c r="B210" s="21"/>
-      <c r="C210" s="22"/>
-    </row>
-    <row r="211" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A211" s="20"/>
-      <c r="B211" s="21"/>
-      <c r="C211" s="22"/>
-    </row>
-    <row r="212" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A212" s="20"/>
-      <c r="B212" s="21"/>
-      <c r="C212" s="22"/>
-    </row>
-    <row r="213" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A213" s="20"/>
-      <c r="B213" s="21"/>
-      <c r="C213" s="22"/>
     </row>
   </sheetData>
   <mergeCells count="5">

</xml_diff>